<commit_message>
Actualización plan de configuración
</commit_message>
<xml_diff>
--- a/Organización/Configuración/Plan_Configuración.xlsx
+++ b/Organización/Configuración/Plan_Configuración.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="134">
   <si>
     <t>Plan de Administración de Configuración</t>
   </si>
@@ -424,13 +424,16 @@
     <t>Cronograma de calidad</t>
   </si>
   <si>
-    <t>Cronograma_calidad</t>
-  </si>
-  <si>
     <t>Plan_calidad</t>
   </si>
   <si>
     <t>Check List Organizacional</t>
+  </si>
+  <si>
+    <t>PTL_Checklist_organizacional_aammdd</t>
+  </si>
+  <si>
+    <t>PTL_Cronograma_calidad</t>
   </si>
 </sst>
 </file>
@@ -4565,7 +4568,7 @@
         <v>128</v>
       </c>
       <c r="C15" s="29" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="16" spans="1:1024" ht="21" x14ac:dyDescent="0.35">
@@ -4574,15 +4577,17 @@
         <v>129</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A17" s="3"/>
       <c r="B17" s="28" t="s">
+        <v>131</v>
+      </c>
+      <c r="C17" s="29" t="s">
         <v>132</v>
       </c>
-      <c r="C17" s="29"/>
     </row>
     <row r="18" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A18" s="3"/>

</xml_diff>

<commit_message>
Integración cronograma calidad en configuración
</commit_message>
<xml_diff>
--- a/Organización/Configuración/Plan_Configuración.xlsx
+++ b/Organización/Configuración/Plan_Configuración.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="135">
   <si>
     <t>Plan de Administración de Configuración</t>
   </si>
@@ -434,6 +434,9 @@
   </si>
   <si>
     <t>PTL_Cronograma_calidad</t>
+  </si>
+  <si>
+    <t>Cronograma_calidad</t>
   </si>
 </sst>
 </file>
@@ -888,34 +891,31 @@
     <xf numFmtId="0" fontId="8" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="16" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -939,28 +939,31 @@
     <xf numFmtId="0" fontId="14" fillId="16" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1336,10 +1339,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMJ119"/>
+  <dimension ref="A1:AMJ120"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A29" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1391,17 +1394,17 @@
   <sheetData>
     <row r="1" spans="1:1024" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
-      <c r="B1" s="55" t="s">
+      <c r="B1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="55"/>
+      <c r="C1" s="39"/>
     </row>
     <row r="2" spans="1:1024" s="24" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="23"/>
-      <c r="B2" s="58" t="s">
+      <c r="B2" s="42" t="s">
         <v>73</v>
       </c>
-      <c r="C2" s="58"/>
+      <c r="C2" s="42"/>
       <c r="D2" s="17"/>
       <c r="E2" s="23"/>
       <c r="F2" s="23"/>
@@ -3452,10 +3455,10 @@
     </row>
     <row r="4" spans="1:1024" s="24" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A4" s="25"/>
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="38" t="s">
         <v>67</v>
       </c>
-      <c r="C4" s="42"/>
+      <c r="C4" s="38"/>
       <c r="D4" s="23"/>
       <c r="E4" s="23"/>
       <c r="F4" s="23"/>
@@ -4480,10 +4483,10 @@
     </row>
     <row r="5" spans="1:1024" ht="21" x14ac:dyDescent="0.35">
       <c r="A5" s="3"/>
-      <c r="B5" s="56" t="s">
+      <c r="B5" s="40" t="s">
         <v>68</v>
       </c>
-      <c r="C5" s="56"/>
+      <c r="C5" s="40"/>
     </row>
     <row r="6" spans="1:1024" ht="21" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
@@ -4498,10 +4501,10 @@
       <c r="A7" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B7" s="54" t="s">
+      <c r="B7" s="37" t="s">
         <v>89</v>
       </c>
-      <c r="C7" s="54"/>
+      <c r="C7" s="37"/>
     </row>
     <row r="8" spans="1:1024" ht="21" x14ac:dyDescent="0.35">
       <c r="A8" s="3"/>
@@ -4523,10 +4526,10 @@
     </row>
     <row r="10" spans="1:1024" ht="21" x14ac:dyDescent="0.35">
       <c r="A10" s="3"/>
-      <c r="B10" s="57" t="s">
+      <c r="B10" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="57"/>
+      <c r="C10" s="41"/>
     </row>
     <row r="11" spans="1:1024" ht="21" x14ac:dyDescent="0.35">
       <c r="A11" s="3"/>
@@ -4539,10 +4542,10 @@
     </row>
     <row r="12" spans="1:1024" ht="21" x14ac:dyDescent="0.35">
       <c r="A12" s="3"/>
-      <c r="B12" s="57" t="s">
+      <c r="B12" s="41" t="s">
         <v>110</v>
       </c>
-      <c r="C12" s="57"/>
+      <c r="C12" s="41"/>
     </row>
     <row r="13" spans="1:1024" ht="21" x14ac:dyDescent="0.35">
       <c r="A13" s="3"/>
@@ -4591,10 +4594,10 @@
     </row>
     <row r="18" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A18" s="3"/>
-      <c r="B18" s="59" t="s">
+      <c r="B18" s="43" t="s">
         <v>109</v>
       </c>
-      <c r="C18" s="59"/>
+      <c r="C18" s="43"/>
     </row>
     <row r="19" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A19" s="3"/>
@@ -4607,10 +4610,10 @@
     </row>
     <row r="20" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A20" s="3"/>
-      <c r="B20" s="60" t="s">
+      <c r="B20" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="61"/>
+      <c r="C20" s="45"/>
     </row>
     <row r="21" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A21" s="3"/>
@@ -4636,22 +4639,22 @@
       <c r="C23" s="15"/>
     </row>
     <row r="24" spans="1:3" s="4" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B24" s="56" t="s">
+      <c r="B24" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="C24" s="56"/>
+      <c r="C24" s="40"/>
     </row>
     <row r="25" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="37" t="s">
+      <c r="B25" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="C25" s="37"/>
+      <c r="C25" s="53"/>
     </row>
     <row r="26" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="40" t="s">
+      <c r="B26" s="56" t="s">
         <v>120</v>
       </c>
-      <c r="C26" s="41"/>
+      <c r="C26" s="57"/>
     </row>
     <row r="27" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B27" s="36" t="s">
@@ -4670,10 +4673,10 @@
       </c>
     </row>
     <row r="29" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="40" t="s">
+      <c r="B29" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="C29" s="41"/>
+      <c r="C29" s="57"/>
     </row>
     <row r="30" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B30" s="30" t="s">
@@ -4716,10 +4719,10 @@
       </c>
     </row>
     <row r="35" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B35" s="40" t="s">
+      <c r="B35" s="56" t="s">
         <v>89</v>
       </c>
-      <c r="C35" s="41"/>
+      <c r="C35" s="57"/>
     </row>
     <row r="36" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B36" s="30" t="s">
@@ -4746,10 +4749,10 @@
       </c>
     </row>
     <row r="39" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B39" s="40" t="s">
+      <c r="B39" s="56" t="s">
         <v>96</v>
       </c>
-      <c r="C39" s="41"/>
+      <c r="C39" s="57"/>
     </row>
     <row r="40" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A40" s="3"/>
@@ -4779,10 +4782,10 @@
       </c>
     </row>
     <row r="43" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B43" s="40" t="s">
+      <c r="B43" s="56" t="s">
         <v>101</v>
       </c>
-      <c r="C43" s="41"/>
+      <c r="C43" s="57"/>
     </row>
     <row r="44" spans="1:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="3"/>
@@ -4795,168 +4798,173 @@
     </row>
     <row r="45" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="3"/>
-      <c r="B45" s="46" t="s">
+      <c r="B45" s="61" t="s">
         <v>110</v>
       </c>
-      <c r="C45" s="46"/>
+      <c r="C45" s="61"/>
     </row>
     <row r="46" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="3"/>
-      <c r="B46" s="32" t="s">
-        <v>114</v>
+      <c r="B46" s="28" t="s">
+        <v>129</v>
       </c>
       <c r="C46" s="29" t="s">
-        <v>117</v>
+        <v>134</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="3"/>
       <c r="B47" s="32" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C47" s="29" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="3"/>
       <c r="B48" s="32" t="s">
+        <v>115</v>
+      </c>
+      <c r="C48" s="29" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="3"/>
+      <c r="B49" s="32" t="s">
         <v>118</v>
       </c>
-      <c r="C48" s="32" t="s">
+      <c r="C49" s="32" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="49" spans="1:3" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B49" s="26"/>
-      <c r="C49" s="26"/>
-    </row>
-    <row r="50" spans="1:3" s="4" customFormat="1" ht="61.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B50" s="45" t="s">
+    <row r="50" spans="1:3" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B50" s="26"/>
+      <c r="C50" s="26"/>
+    </row>
+    <row r="51" spans="1:3" s="4" customFormat="1" ht="61.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B51" s="60" t="s">
         <v>127</v>
       </c>
-      <c r="C50" s="45"/>
-    </row>
-    <row r="51" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B51" s="42" t="s">
+      <c r="C51" s="60"/>
+    </row>
+    <row r="52" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B52" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="C51" s="42"/>
-    </row>
-    <row r="52" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B52" s="14" t="s">
+      <c r="C52" s="38"/>
+    </row>
+    <row r="53" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B53" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C52" s="14" t="s">
+      <c r="C53" s="14" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B53" s="43" t="s">
+    <row r="54" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B54" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="C53" s="44"/>
-    </row>
-    <row r="54" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B54" s="33" t="s">
+      <c r="C54" s="59"/>
+    </row>
+    <row r="55" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B55" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="C54" s="33" t="s">
+      <c r="C55" s="33" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B55" s="16"/>
-      <c r="C55" s="16"/>
-    </row>
-    <row r="56" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B56" s="38" t="s">
+    <row r="56" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B56" s="16"/>
+      <c r="C56" s="16"/>
+    </row>
+    <row r="57" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B57" s="54" t="s">
         <v>63</v>
       </c>
-      <c r="C56" s="39"/>
-    </row>
-    <row r="57" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B57" s="49" t="s">
+      <c r="C57" s="55"/>
+    </row>
+    <row r="58" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B58" s="48" t="s">
         <v>66</v>
       </c>
-      <c r="C57" s="50"/>
-    </row>
-    <row r="58" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B58" s="51"/>
-      <c r="C58" s="52"/>
-    </row>
-    <row r="59" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B59" s="16"/>
-      <c r="C59" s="16"/>
-    </row>
-    <row r="60" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B60" s="42" t="s">
+      <c r="C58" s="49"/>
+    </row>
+    <row r="59" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B59" s="50"/>
+      <c r="C59" s="51"/>
+    </row>
+    <row r="60" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B60" s="16"/>
+      <c r="C60" s="16"/>
+    </row>
+    <row r="61" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B61" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="C60" s="42"/>
-    </row>
-    <row r="61" spans="1:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B61" s="53" t="s">
+      <c r="C61" s="38"/>
+    </row>
+    <row r="62" spans="1:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B62" s="52" t="s">
         <v>64</v>
       </c>
-      <c r="C61" s="53"/>
-    </row>
-    <row r="62" spans="1:3" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B62" s="53"/>
-      <c r="C62" s="53"/>
-    </row>
-    <row r="63" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B63" s="18"/>
-      <c r="C63" s="19"/>
-    </row>
-    <row r="64" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="5"/>
-      <c r="B64" s="48" t="s">
+      <c r="C62" s="52"/>
+    </row>
+    <row r="63" spans="1:3" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B63" s="52"/>
+      <c r="C63" s="52"/>
+    </row>
+    <row r="64" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B64" s="18"/>
+      <c r="C64" s="19"/>
+    </row>
+    <row r="65" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="5"/>
+      <c r="B65" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="C64" s="48"/>
-    </row>
-    <row r="65" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B65" s="47"/>
       <c r="C65" s="47"/>
     </row>
-    <row r="66" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B66" s="20"/>
-      <c r="C66" s="20"/>
-    </row>
-    <row r="67" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="B67" s="19"/>
-      <c r="C67" s="19"/>
-    </row>
-    <row r="68" spans="1:8" ht="21" x14ac:dyDescent="0.2">
-      <c r="B68" s="21" t="s">
+    <row r="66" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B66" s="46"/>
+      <c r="C66" s="46"/>
+    </row>
+    <row r="67" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B67" s="20"/>
+      <c r="C67" s="20"/>
+    </row>
+    <row r="68" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="B68" s="19"/>
+      <c r="C68" s="19"/>
+    </row>
+    <row r="69" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="B69" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="C68" s="21" t="s">
+      <c r="C69" s="21" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="21" x14ac:dyDescent="0.2">
-      <c r="A69" s="6"/>
-      <c r="B69" s="34" t="s">
+    <row r="70" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A70" s="6"/>
+      <c r="B70" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="C69" s="35"/>
-    </row>
-    <row r="70" spans="1:8" ht="21" x14ac:dyDescent="0.2">
-      <c r="B70" s="34"/>
       <c r="C70" s="35"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B71" s="7"/>
-      <c r="C71" s="7"/>
-    </row>
-    <row r="72" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A72" s="5"/>
-      <c r="B72" s="6"/>
-      <c r="C72" s="6"/>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="B71" s="34"/>
+      <c r="C71" s="35"/>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B72" s="7"/>
+      <c r="C72" s="7"/>
+    </row>
+    <row r="73" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A73" s="5"/>
       <c r="B73" s="6"/>
       <c r="C73" s="6"/>
     </row>
@@ -4971,11 +4979,6 @@
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B76" s="6"/>
       <c r="C76" s="6"/>
-      <c r="D76" s="6"/>
-      <c r="E76" s="6"/>
-      <c r="F76" s="6"/>
-      <c r="G76" s="6"/>
-      <c r="H76" s="6"/>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B77" s="6"/>
@@ -5329,6 +5332,8 @@
       <c r="H115" s="6"/>
     </row>
     <row r="116" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B116" s="6"/>
+      <c r="C116" s="6"/>
       <c r="D116" s="6"/>
       <c r="E116" s="6"/>
       <c r="F116" s="6"/>
@@ -5356,8 +5361,31 @@
       <c r="G119" s="6"/>
       <c r="H119" s="6"/>
     </row>
+    <row r="120" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="D120" s="6"/>
+      <c r="E120" s="6"/>
+      <c r="F120" s="6"/>
+      <c r="G120" s="6"/>
+      <c r="H120" s="6"/>
+    </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="B58:C59"/>
+    <mergeCell ref="B62:C63"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B1:C1"/>
@@ -5368,22 +5396,6 @@
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B57:C58"/>
-    <mergeCell ref="B61:C62"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B29:C29"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Actualizacion del plan de configuracion
</commit_message>
<xml_diff>
--- a/Organización/Configuración/Plan_Configuración.xlsx
+++ b/Organización/Configuración/Plan_Configuración.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="143">
   <si>
     <t>Plan de Administración de Configuración</t>
   </si>
@@ -244,15 +244,9 @@
     <t>Herramientas de Trabajo</t>
   </si>
   <si>
-    <t>GitHub</t>
-  </si>
-  <si>
     <t>P</t>
   </si>
   <si>
-    <t>Para la correcta identificacion de un archivo se toma la siguiente base , carpeta origen/Carpeta/subcarpeta/ archivo. Ejemplo : Origen/Organización/Plantillas/PTL_Requerimientos</t>
-  </si>
-  <si>
     <t>PTL Plan de proyecto</t>
   </si>
   <si>
@@ -286,12 +280,6 @@
     <t>Cotización</t>
   </si>
   <si>
-    <t>Correo de cotización</t>
-  </si>
-  <si>
-    <t>Correo_cotización</t>
-  </si>
-  <si>
     <t>Comprobante de pago</t>
   </si>
   <si>
@@ -322,30 +310,12 @@
     <t>Cierre</t>
   </si>
   <si>
-    <t>Garantía</t>
-  </si>
-  <si>
-    <t>Correo de validación de solicitud</t>
-  </si>
-  <si>
-    <t>Correo_validación_&lt;nombre de solicitud&gt;</t>
-  </si>
-  <si>
     <t>Ciclo de Vida</t>
   </si>
   <si>
     <t>Ciclo_de_vida</t>
   </si>
   <si>
-    <t>PTL_Plan_proyecto_nombreproyecto</t>
-  </si>
-  <si>
-    <t>PTL_Estimación_nombreproyecto</t>
-  </si>
-  <si>
-    <t>PTL_Requerimientos_nombreproyecto</t>
-  </si>
-  <si>
     <t>Ciclo_Vida</t>
   </si>
   <si>
@@ -370,21 +340,6 @@
     <t>No_conformidades</t>
   </si>
   <si>
-    <t>Prospectación</t>
-  </si>
-  <si>
-    <t>Correo de asignación</t>
-  </si>
-  <si>
-    <t>Correo de portafolio</t>
-  </si>
-  <si>
-    <t>Correo_portafolio</t>
-  </si>
-  <si>
-    <t>Correo_asignación</t>
-  </si>
-  <si>
     <t>Encuesta de satisfacción</t>
   </si>
   <si>
@@ -478,9 +433,6 @@
     <t>PTL_Minuta</t>
   </si>
   <si>
-    <t>carta_aceptación</t>
-  </si>
-  <si>
     <t>Carta de aceptación/confirmación</t>
   </si>
   <si>
@@ -488,6 +440,27 @@
   </si>
   <si>
     <t>Se genera un respaldo del CRM en forma semanal cuyo responsable de ejecución sera:    .</t>
+  </si>
+  <si>
+    <t>GitHub (bajo el gestor source tree)</t>
+  </si>
+  <si>
+    <t>Procesos del ciclo de vida</t>
+  </si>
+  <si>
+    <t>Procesos_SOS</t>
+  </si>
+  <si>
+    <t>Para la correcta identificacion de un archivo se toma la siguiente base , carpeta origen/Carpeta/subcarpeta/ archivo. Ejemplo : Origen/Organización/Planeación/PTL_Plan_proyecto</t>
+  </si>
+  <si>
+    <t>PTL_Plan_proyecto</t>
+  </si>
+  <si>
+    <t>PTL_Estimación</t>
+  </si>
+  <si>
+    <t>PTL_Requerimientos</t>
   </si>
 </sst>
 </file>
@@ -612,7 +585,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="20">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -700,12 +673,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
-        <bgColor rgb="FFC0C0C0"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor rgb="FFCFE7F5"/>
       </patternFill>
     </fill>
@@ -719,12 +686,6 @@
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor rgb="FFCFE7F5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.249977111117893"/>
-        <bgColor rgb="FFC0C0C0"/>
       </patternFill>
     </fill>
   </fills>
@@ -855,7 +816,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -908,32 +869,29 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -956,12 +914,6 @@
     <xf numFmtId="0" fontId="6" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -971,7 +923,7 @@
     <xf numFmtId="0" fontId="7" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -989,7 +941,7 @@
     <xf numFmtId="0" fontId="10" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1010,19 +962,19 @@
     <xf numFmtId="0" fontId="10" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1398,10 +1350,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMJ127"/>
+  <dimension ref="A1:AMJ121"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A70" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F75" sqref="F75"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1453,17 +1405,17 @@
   <sheetData>
     <row r="1" spans="1:1024" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="38"/>
+      <c r="C1" s="37"/>
     </row>
     <row r="2" spans="1:1024" s="22" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="21"/>
-      <c r="B2" s="40" t="s">
-        <v>72</v>
-      </c>
-      <c r="C2" s="40"/>
+      <c r="B2" s="39" t="s">
+        <v>139</v>
+      </c>
+      <c r="C2" s="39"/>
       <c r="D2" s="15"/>
       <c r="E2" s="21"/>
       <c r="F2" s="21"/>
@@ -3514,10 +3466,10 @@
     </row>
     <row r="4" spans="1:1024" s="22" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A4" s="23"/>
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="C4" s="37"/>
+      <c r="C4" s="36"/>
       <c r="D4" s="21"/>
       <c r="E4" s="21"/>
       <c r="F4" s="21"/>
@@ -4542,10 +4494,10 @@
     </row>
     <row r="5" spans="1:1024" ht="21" x14ac:dyDescent="0.35">
       <c r="A5" s="3"/>
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="C5" s="39"/>
+      <c r="C5" s="38"/>
     </row>
     <row r="6" spans="1:1024" ht="21" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
@@ -4556,42 +4508,47 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:1024" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="42" t="s">
-        <v>112</v>
-      </c>
-      <c r="C7" s="43"/>
-    </row>
-    <row r="8" spans="1:1024" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="34" t="s">
-        <v>113</v>
-      </c>
-      <c r="C8" s="34" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1024" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="34" t="s">
-        <v>114</v>
-      </c>
-      <c r="C9" s="34" t="s">
-        <v>115</v>
+    <row r="7" spans="1:1024" ht="21" x14ac:dyDescent="0.35">
+      <c r="A7" s="3"/>
+      <c r="B7" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="42"/>
+    </row>
+    <row r="8" spans="1:1024" ht="21" x14ac:dyDescent="0.35">
+      <c r="A8" s="3"/>
+      <c r="B8" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1024" ht="21" x14ac:dyDescent="0.35">
+      <c r="A9" s="3"/>
+      <c r="B9" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" s="27" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="10" spans="1:1024" ht="21" x14ac:dyDescent="0.35">
-      <c r="A10" s="3"/>
-      <c r="B10" s="44" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="45"/>
+      <c r="A10" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10" s="34" t="s">
+        <v>84</v>
+      </c>
+      <c r="C10" s="35"/>
     </row>
     <row r="11" spans="1:1024" ht="21" x14ac:dyDescent="0.35">
       <c r="A11" s="3"/>
       <c r="B11" s="26" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C11" s="27" t="s">
-        <v>103</v>
+        <v>140</v>
       </c>
     </row>
     <row r="12" spans="1:1024" ht="21" x14ac:dyDescent="0.35">
@@ -4600,518 +4557,522 @@
         <v>74</v>
       </c>
       <c r="C12" s="27" t="s">
-        <v>102</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:1024" ht="21" x14ac:dyDescent="0.35">
-      <c r="A13" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B13" s="35" t="s">
-        <v>88</v>
-      </c>
-      <c r="C13" s="36"/>
+      <c r="A13" s="3"/>
+      <c r="B13" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="C13" s="42"/>
     </row>
     <row r="14" spans="1:1024" ht="21" x14ac:dyDescent="0.35">
       <c r="A14" s="3"/>
       <c r="B14" s="26" t="s">
-        <v>73</v>
+        <v>133</v>
       </c>
       <c r="C14" s="27" t="s">
-        <v>101</v>
+        <v>134</v>
       </c>
     </row>
     <row r="15" spans="1:1024" ht="21" x14ac:dyDescent="0.35">
       <c r="A15" s="3"/>
-      <c r="B15" s="26" t="s">
-        <v>76</v>
-      </c>
-      <c r="C15" s="27" t="s">
-        <v>77</v>
-      </c>
+      <c r="B15" s="40" t="s">
+        <v>95</v>
+      </c>
+      <c r="C15" s="40"/>
     </row>
     <row r="16" spans="1:1024" ht="21" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
-      <c r="B16" s="44" t="s">
-        <v>95</v>
-      </c>
-      <c r="C16" s="45"/>
+      <c r="B16" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="C16" s="27" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="17" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A17" s="3"/>
       <c r="B17" s="26" t="s">
-        <v>149</v>
+        <v>76</v>
       </c>
       <c r="C17" s="27" t="s">
-        <v>150</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A18" s="3"/>
-      <c r="B18" s="41" t="s">
+      <c r="B18" s="26" t="s">
         <v>105</v>
       </c>
-      <c r="C18" s="41"/>
+      <c r="C18" s="27" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="19" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A19" s="3"/>
-      <c r="B19" s="27" t="s">
-        <v>81</v>
+      <c r="B19" s="26" t="s">
+        <v>106</v>
       </c>
       <c r="C19" s="27" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A20" s="3"/>
       <c r="B20" s="26" t="s">
-        <v>78</v>
+        <v>108</v>
       </c>
       <c r="C20" s="27" t="s">
-        <v>79</v>
+        <v>109</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A21" s="3"/>
-      <c r="B21" s="26" t="s">
-        <v>120</v>
-      </c>
-      <c r="C21" s="27" t="s">
-        <v>122</v>
-      </c>
+      <c r="B21" s="41" t="s">
+        <v>116</v>
+      </c>
+      <c r="C21" s="42"/>
     </row>
     <row r="22" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A22" s="3"/>
-      <c r="B22" s="26" t="s">
-        <v>121</v>
-      </c>
-      <c r="C22" s="27" t="s">
-        <v>125</v>
+      <c r="B22" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="C22" s="30" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A23" s="3"/>
-      <c r="B23" s="26" t="s">
-        <v>123</v>
-      </c>
-      <c r="C23" s="27" t="s">
-        <v>124</v>
+      <c r="B23" s="30" t="s">
+        <v>120</v>
+      </c>
+      <c r="C23" s="30" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A24" s="3"/>
-      <c r="B24" s="44" t="s">
+      <c r="B24" s="30" t="s">
         <v>131</v>
       </c>
-      <c r="C24" s="45"/>
+      <c r="C24" s="30" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="25" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A25" s="3"/>
       <c r="B25" s="30" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="C25" s="30" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A26" s="3"/>
       <c r="B26" s="30" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="C26" s="30" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A27" s="3"/>
-      <c r="B27" s="30" t="s">
-        <v>146</v>
-      </c>
-      <c r="C27" s="30" t="s">
-        <v>147</v>
-      </c>
+      <c r="B27" s="41" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="42"/>
     </row>
     <row r="28" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A28" s="3"/>
-      <c r="B28" s="30" t="s">
-        <v>136</v>
-      </c>
-      <c r="C28" s="30" t="s">
-        <v>138</v>
+      <c r="B28" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28" s="27" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A29" s="3"/>
-      <c r="B29" s="30" t="s">
-        <v>137</v>
-      </c>
-      <c r="C29" s="30" t="s">
-        <v>145</v>
-      </c>
+      <c r="B29" s="43" t="s">
+        <v>94</v>
+      </c>
+      <c r="C29" s="43"/>
     </row>
     <row r="30" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A30" s="3"/>
-      <c r="B30" s="44" t="s">
-        <v>4</v>
-      </c>
-      <c r="C30" s="45"/>
+      <c r="B30" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="C30" s="27" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="31" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A31" s="3"/>
       <c r="B31" s="27" t="s">
-        <v>35</v>
+        <v>137</v>
       </c>
       <c r="C31" s="27" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A32" s="3"/>
-      <c r="B32" s="46" t="s">
-        <v>104</v>
-      </c>
-      <c r="C32" s="46"/>
-    </row>
-    <row r="33" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A33" s="3"/>
-      <c r="B33" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="C33" s="27" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" s="4" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B34" s="39" t="s">
-        <v>126</v>
-      </c>
-      <c r="C34" s="39"/>
-    </row>
-    <row r="35" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B35" s="54" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" s="4" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B32" s="38" t="s">
+        <v>111</v>
+      </c>
+      <c r="C32" s="38"/>
+    </row>
+    <row r="33" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B33" s="51" t="s">
+        <v>78</v>
+      </c>
+      <c r="C33" s="51"/>
+    </row>
+    <row r="34" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B34" s="57" t="s">
+        <v>16</v>
+      </c>
+      <c r="C34" s="58"/>
+    </row>
+    <row r="35" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B35" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="C35" s="54"/>
-    </row>
-    <row r="36" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="60" t="s">
-        <v>16</v>
-      </c>
-      <c r="C36" s="61"/>
+      <c r="C35" s="29" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B36" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="C36" s="29" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="37" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B37" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="C37" s="29" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B38" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="C37" s="29" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B38" s="28" t="s">
-        <v>6</v>
-      </c>
       <c r="C38" s="29" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B39" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="C39" s="29" t="s">
-        <v>83</v>
-      </c>
+    </row>
+    <row r="39" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B39" s="57" t="s">
+        <v>84</v>
+      </c>
+      <c r="C39" s="58"/>
     </row>
     <row r="40" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B40" s="28" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C40" s="29" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B41" s="28" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C41" s="29" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B42" s="60" t="s">
         <v>88</v>
       </c>
-      <c r="C42" s="61"/>
-    </row>
-    <row r="43" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B43" s="28" t="s">
+    </row>
+    <row r="42" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B42" s="28" t="s">
         <v>89</v>
       </c>
-      <c r="C43" s="29" t="s">
+      <c r="C42" s="29" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B43" s="57" t="s">
+        <v>91</v>
+      </c>
+      <c r="C43" s="58"/>
+    </row>
+    <row r="44" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="A44" s="3"/>
       <c r="B44" s="28" t="s">
-        <v>91</v>
-      </c>
-      <c r="C44" s="29" t="s">
-        <v>92</v>
+        <v>102</v>
+      </c>
+      <c r="C44" s="30" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B45" s="28" t="s">
-        <v>93</v>
-      </c>
-      <c r="C45" s="29" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B46" s="60" t="s">
+      <c r="A45" s="3"/>
+      <c r="B45" s="59" t="s">
         <v>95</v>
       </c>
-      <c r="C46" s="61"/>
-    </row>
-    <row r="47" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="C45" s="59"/>
+    </row>
+    <row r="46" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="3"/>
+      <c r="B46" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="C46" s="27" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="3"/>
-      <c r="B47" s="28" t="s">
-        <v>149</v>
-      </c>
-      <c r="C47" s="30" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="B47" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="C47" s="27" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="3"/>
-      <c r="B48" s="28" t="s">
-        <v>117</v>
-      </c>
-      <c r="C48" s="30" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B49" s="60" t="s">
-        <v>96</v>
-      </c>
-      <c r="C49" s="61"/>
-    </row>
-    <row r="50" spans="1:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B48" s="60" t="s">
+        <v>116</v>
+      </c>
+      <c r="C48" s="61"/>
+    </row>
+    <row r="49" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="3"/>
+      <c r="B49" s="30" t="s">
+        <v>124</v>
+      </c>
+      <c r="C49" s="27" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="3"/>
-      <c r="B50" s="28" t="s">
-        <v>97</v>
-      </c>
-      <c r="C50" s="30" t="s">
-        <v>98</v>
+      <c r="B50" s="30" t="s">
+        <v>125</v>
+      </c>
+      <c r="C50" s="27" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="3"/>
-      <c r="B51" s="62" t="s">
-        <v>105</v>
-      </c>
-      <c r="C51" s="62"/>
-    </row>
-    <row r="52" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="3"/>
-      <c r="B52" s="30" t="s">
-        <v>109</v>
-      </c>
-      <c r="C52" s="27" t="s">
+      <c r="B51" s="30" t="s">
+        <v>126</v>
+      </c>
+      <c r="C51" s="27" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="3"/>
-      <c r="B53" s="30" t="s">
-        <v>110</v>
-      </c>
-      <c r="C53" s="27" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="3"/>
-      <c r="B54" s="63" t="s">
-        <v>131</v>
-      </c>
-      <c r="C54" s="64"/>
-    </row>
-    <row r="55" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="3"/>
-      <c r="B55" s="30" t="s">
-        <v>139</v>
-      </c>
-      <c r="C55" s="27" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="3"/>
-      <c r="B56" s="30" t="s">
-        <v>140</v>
-      </c>
-      <c r="C56" s="27" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="3"/>
-      <c r="B57" s="30" t="s">
-        <v>141</v>
-      </c>
-      <c r="C57" s="27" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B58" s="24"/>
-      <c r="C58" s="24"/>
-    </row>
-    <row r="59" spans="1:3" s="4" customFormat="1" ht="61.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B59" s="59" t="s">
-        <v>119</v>
-      </c>
-      <c r="C59" s="59"/>
-    </row>
-    <row r="60" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B60" s="37" t="s">
+    <row r="52" spans="1:3" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B52" s="24"/>
+      <c r="C52" s="24"/>
+    </row>
+    <row r="53" spans="1:3" s="4" customFormat="1" ht="61.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B53" s="56" t="s">
+        <v>104</v>
+      </c>
+      <c r="C53" s="56"/>
+    </row>
+    <row r="54" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B54" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="C60" s="37"/>
-    </row>
-    <row r="61" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B61" s="13" t="s">
+      <c r="C54" s="36"/>
+    </row>
+    <row r="55" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B55" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C61" s="13" t="s">
+      <c r="C55" s="13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B62" s="57" t="s">
+    <row r="56" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B56" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="C62" s="58"/>
-    </row>
-    <row r="63" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B63" s="31" t="s">
+      <c r="C56" s="55"/>
+    </row>
+    <row r="57" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B57" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="C63" s="31" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B64" s="14"/>
-      <c r="C64" s="14"/>
-    </row>
-    <row r="65" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B65" s="55" t="s">
+      <c r="C57" s="31" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B58" s="14"/>
+      <c r="C58" s="14"/>
+    </row>
+    <row r="59" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B59" s="52" t="s">
         <v>63</v>
       </c>
-      <c r="C65" s="56"/>
-    </row>
-    <row r="66" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B66" s="49" t="s">
+      <c r="C59" s="53"/>
+    </row>
+    <row r="60" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B60" s="46" t="s">
         <v>66</v>
       </c>
-      <c r="C66" s="50"/>
-    </row>
-    <row r="67" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B67" s="51"/>
-      <c r="C67" s="52"/>
-    </row>
-    <row r="68" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B68" s="14"/>
-      <c r="C68" s="14"/>
-    </row>
-    <row r="69" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B69" s="37" t="s">
+      <c r="C60" s="47"/>
+    </row>
+    <row r="61" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B61" s="48"/>
+      <c r="C61" s="49"/>
+    </row>
+    <row r="62" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B62" s="14"/>
+      <c r="C62" s="14"/>
+    </row>
+    <row r="63" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B63" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="C69" s="37"/>
-    </row>
-    <row r="70" spans="1:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B70" s="53" t="s">
+      <c r="C63" s="36"/>
+    </row>
+    <row r="64" spans="1:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B64" s="50" t="s">
         <v>64</v>
       </c>
-      <c r="C70" s="53"/>
-    </row>
-    <row r="71" spans="1:3" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B71" s="53"/>
-      <c r="C71" s="53"/>
-    </row>
-    <row r="72" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B72" s="16"/>
-      <c r="C72" s="17"/>
-    </row>
-    <row r="73" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A73" s="5"/>
-      <c r="B73" s="48" t="s">
+      <c r="C64" s="50"/>
+    </row>
+    <row r="65" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B65" s="50"/>
+      <c r="C65" s="50"/>
+    </row>
+    <row r="66" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B66" s="16"/>
+      <c r="C66" s="17"/>
+    </row>
+    <row r="67" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A67" s="5"/>
+      <c r="B67" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="C73" s="48"/>
-    </row>
-    <row r="74" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B74" s="47" t="s">
-        <v>151</v>
-      </c>
-      <c r="C74" s="47"/>
-    </row>
-    <row r="75" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B75" s="18"/>
-      <c r="C75" s="18"/>
-    </row>
-    <row r="76" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="B76" s="17"/>
-      <c r="C76" s="17"/>
-    </row>
-    <row r="77" spans="1:3" ht="21" x14ac:dyDescent="0.2">
-      <c r="B77" s="19" t="s">
+      <c r="C67" s="45"/>
+    </row>
+    <row r="68" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B68" s="44" t="s">
+        <v>135</v>
+      </c>
+      <c r="C68" s="44"/>
+    </row>
+    <row r="69" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B69" s="18"/>
+      <c r="C69" s="18"/>
+    </row>
+    <row r="70" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="B70" s="17"/>
+      <c r="C70" s="17"/>
+    </row>
+    <row r="71" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="B71" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="C77" s="19" t="s">
+      <c r="C71" s="19" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="21" x14ac:dyDescent="0.2">
-      <c r="A78" s="6"/>
-      <c r="B78" s="32" t="s">
-        <v>70</v>
-      </c>
-      <c r="C78" s="33" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" ht="21" x14ac:dyDescent="0.2">
-      <c r="B79" s="32" t="s">
-        <v>128</v>
-      </c>
-      <c r="C79" s="33" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A80" s="5"/>
+    <row r="72" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A72" s="6"/>
+      <c r="B72" s="32" t="s">
+        <v>136</v>
+      </c>
+      <c r="C72" s="33" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="B73" s="32" t="s">
+        <v>113</v>
+      </c>
+      <c r="C73" s="33" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A74" s="5"/>
+      <c r="B74" s="6"/>
+      <c r="C74" s="6"/>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B75" s="6"/>
+      <c r="C75" s="6"/>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B76" s="6"/>
+      <c r="C76" s="6"/>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B77" s="6"/>
+      <c r="C77" s="6"/>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B78" s="6"/>
+      <c r="C78" s="6"/>
+      <c r="D78" s="6"/>
+      <c r="E78" s="6"/>
+      <c r="F78" s="6"/>
+      <c r="G78" s="6"/>
+      <c r="H78" s="6"/>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B79" s="6"/>
+      <c r="C79" s="6"/>
+      <c r="D79" s="6"/>
+      <c r="E79" s="6"/>
+      <c r="F79" s="6"/>
+      <c r="G79" s="6"/>
+      <c r="H79" s="6"/>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B80" s="6"/>
       <c r="C80" s="6"/>
+      <c r="D80" s="6"/>
+      <c r="E80" s="6"/>
+      <c r="F80" s="6"/>
+      <c r="G80" s="6"/>
+      <c r="H80" s="6"/>
     </row>
     <row r="81" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B81" s="6"/>
       <c r="C81" s="6"/>
+      <c r="D81" s="6"/>
+      <c r="E81" s="6"/>
+      <c r="F81" s="6"/>
+      <c r="G81" s="6"/>
+      <c r="H81" s="6"/>
     </row>
     <row r="82" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B82" s="6"/>
       <c r="C82" s="6"/>
+      <c r="D82" s="6"/>
+      <c r="E82" s="6"/>
+      <c r="F82" s="6"/>
+      <c r="G82" s="6"/>
+      <c r="H82" s="6"/>
     </row>
     <row r="83" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B83" s="6"/>
       <c r="C83" s="6"/>
+      <c r="D83" s="6"/>
+      <c r="E83" s="6"/>
+      <c r="F83" s="6"/>
+      <c r="G83" s="6"/>
+      <c r="H83" s="6"/>
     </row>
     <row r="84" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B84" s="6"/>
@@ -5420,8 +5381,6 @@
       <c r="H117" s="6"/>
     </row>
     <row r="118" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B118" s="6"/>
-      <c r="C118" s="6"/>
       <c r="D118" s="6"/>
       <c r="E118" s="6"/>
       <c r="F118" s="6"/>
@@ -5429,8 +5388,6 @@
       <c r="H118" s="6"/>
     </row>
     <row r="119" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B119" s="6"/>
-      <c r="C119" s="6"/>
       <c r="D119" s="6"/>
       <c r="E119" s="6"/>
       <c r="F119" s="6"/>
@@ -5438,8 +5395,6 @@
       <c r="H119" s="6"/>
     </row>
     <row r="120" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B120" s="6"/>
-      <c r="C120" s="6"/>
       <c r="D120" s="6"/>
       <c r="E120" s="6"/>
       <c r="F120" s="6"/>
@@ -5447,95 +5402,45 @@
       <c r="H120" s="6"/>
     </row>
     <row r="121" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B121" s="6"/>
-      <c r="C121" s="6"/>
       <c r="D121" s="6"/>
       <c r="E121" s="6"/>
       <c r="F121" s="6"/>
       <c r="G121" s="6"/>
       <c r="H121" s="6"/>
     </row>
-    <row r="122" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B122" s="6"/>
-      <c r="C122" s="6"/>
-      <c r="D122" s="6"/>
-      <c r="E122" s="6"/>
-      <c r="F122" s="6"/>
-      <c r="G122" s="6"/>
-      <c r="H122" s="6"/>
-    </row>
-    <row r="123" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B123" s="6"/>
-      <c r="C123" s="6"/>
-      <c r="D123" s="6"/>
-      <c r="E123" s="6"/>
-      <c r="F123" s="6"/>
-      <c r="G123" s="6"/>
-      <c r="H123" s="6"/>
-    </row>
-    <row r="124" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="D124" s="6"/>
-      <c r="E124" s="6"/>
-      <c r="F124" s="6"/>
-      <c r="G124" s="6"/>
-      <c r="H124" s="6"/>
-    </row>
-    <row r="125" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="D125" s="6"/>
-      <c r="E125" s="6"/>
-      <c r="F125" s="6"/>
-      <c r="G125" s="6"/>
-      <c r="H125" s="6"/>
-    </row>
-    <row r="126" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="D126" s="6"/>
-      <c r="E126" s="6"/>
-      <c r="F126" s="6"/>
-      <c r="G126" s="6"/>
-      <c r="H126" s="6"/>
-    </row>
-    <row r="127" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="D127" s="6"/>
-      <c r="E127" s="6"/>
-      <c r="F127" s="6"/>
-      <c r="G127" s="6"/>
-      <c r="H127" s="6"/>
-    </row>
   </sheetData>
-  <mergeCells count="29">
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B62:C62"/>
+  <mergeCells count="27">
+    <mergeCell ref="B33:C33"/>
     <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B36:C36"/>
     <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B66:C67"/>
-    <mergeCell ref="B70:C71"/>
-    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B60:C61"/>
+    <mergeCell ref="B64:C65"/>
+    <mergeCell ref="B10:C10"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B32:C32"/>
     <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B21:C21"/>
     <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B13:C13"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C78" r:id="rId1"/>
-    <hyperlink ref="C79" r:id="rId2"/>
+    <hyperlink ref="C72" r:id="rId1"/>
+    <hyperlink ref="C73" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId3"/>

</xml_diff>

<commit_message>
Cambio de estructura de Minutas de proyectos
</commit_message>
<xml_diff>
--- a/Organización/Configuración/Plan_Configuración.xlsx
+++ b/Organización/Configuración/Plan_Configuración.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Novela\Documents\Qualtop\SOS\Organización\Configuración\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="875"/>
   </bookViews>
@@ -21,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="144">
   <si>
     <t>Plan de Administración de Configuración</t>
   </si>
@@ -304,9 +309,6 @@
     <t>Minuta de Compromiso</t>
   </si>
   <si>
-    <t>Minuta_compromiso</t>
-  </si>
-  <si>
     <t>Cierre</t>
   </si>
   <si>
@@ -421,9 +423,6 @@
     <t>Reporte_monitoreo_aammdd</t>
   </si>
   <si>
-    <t>Concentrado_metricas_aammdd</t>
-  </si>
-  <si>
     <t>Plan_Métricas_aaaa</t>
   </si>
   <si>
@@ -439,9 +438,6 @@
     <t>PTL_carta_aceptación</t>
   </si>
   <si>
-    <t>Se genera un respaldo del CRM en forma semanal cuyo responsable de ejecución sera:    .</t>
-  </si>
-  <si>
     <t>GitHub (bajo el gestor source tree)</t>
   </si>
   <si>
@@ -461,6 +457,18 @@
   </si>
   <si>
     <t>PTL_Requerimientos</t>
+  </si>
+  <si>
+    <t>Minutas de Proyectos</t>
+  </si>
+  <si>
+    <t>Minuta_compromiso_aammdd</t>
+  </si>
+  <si>
+    <t>Concentrado_métricas_aammdd</t>
+  </si>
+  <si>
+    <t>Se genera un respaldo del CRM en forma semanal cuyo responsable de ejecución es:</t>
   </si>
 </sst>
 </file>
@@ -893,57 +901,6 @@
     <xf numFmtId="0" fontId="16" fillId="15" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -951,6 +908,9 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -977,9 +937,57 @@
     <xf numFmtId="0" fontId="6" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1064,7 +1072,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1106,7 +1114,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1141,7 +1149,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1350,13 +1358,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMJ121"/>
+  <dimension ref="A1:AMJ122"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="585" ySplit="2940" topLeftCell="B34" activePane="bottomRight"/>
+      <selection activeCell="A26" sqref="A26"/>
+      <selection pane="topRight" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomLeft" activeCell="A34" sqref="A34:XFD34"/>
+      <selection pane="bottomRight" activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.85546875" style="1"/>
     <col min="2" max="2" width="53.5703125" style="1" customWidth="1"/>
@@ -1405,17 +1417,17 @@
   <sheetData>
     <row r="1" spans="1:1024" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="37"/>
+      <c r="C1" s="55"/>
     </row>
     <row r="2" spans="1:1024" s="22" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="21"/>
-      <c r="B2" s="39" t="s">
-        <v>139</v>
-      </c>
-      <c r="C2" s="39"/>
+      <c r="B2" s="57" t="s">
+        <v>136</v>
+      </c>
+      <c r="C2" s="57"/>
       <c r="D2" s="15"/>
       <c r="E2" s="21"/>
       <c r="F2" s="21"/>
@@ -3466,10 +3478,10 @@
     </row>
     <row r="4" spans="1:1024" s="22" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A4" s="23"/>
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="C4" s="36"/>
+      <c r="C4" s="37"/>
       <c r="D4" s="21"/>
       <c r="E4" s="21"/>
       <c r="F4" s="21"/>
@@ -4494,10 +4506,10 @@
     </row>
     <row r="5" spans="1:1024" ht="21" x14ac:dyDescent="0.35">
       <c r="A5" s="3"/>
-      <c r="B5" s="38" t="s">
+      <c r="B5" s="56" t="s">
         <v>68</v>
       </c>
-      <c r="C5" s="38"/>
+      <c r="C5" s="56"/>
     </row>
     <row r="6" spans="1:1024" ht="21" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
@@ -4510,10 +4522,10 @@
     </row>
     <row r="7" spans="1:1024" ht="21" x14ac:dyDescent="0.35">
       <c r="A7" s="3"/>
-      <c r="B7" s="41" t="s">
+      <c r="B7" s="59" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="42"/>
+      <c r="C7" s="60"/>
     </row>
     <row r="8" spans="1:1024" ht="21" x14ac:dyDescent="0.35">
       <c r="A8" s="3"/>
@@ -4521,7 +4533,7 @@
         <v>73</v>
       </c>
       <c r="C8" s="27" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="9" spans="1:1024" ht="21" x14ac:dyDescent="0.35">
@@ -4530,17 +4542,17 @@
         <v>72</v>
       </c>
       <c r="C9" s="27" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:1024" ht="21" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B10" s="34" t="s">
+      <c r="B10" s="53" t="s">
         <v>84</v>
       </c>
-      <c r="C10" s="35"/>
+      <c r="C10" s="54"/>
     </row>
     <row r="11" spans="1:1024" ht="21" x14ac:dyDescent="0.35">
       <c r="A11" s="3"/>
@@ -4548,7 +4560,7 @@
         <v>71</v>
       </c>
       <c r="C11" s="27" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="12" spans="1:1024" ht="21" x14ac:dyDescent="0.35">
@@ -4562,26 +4574,26 @@
     </row>
     <row r="13" spans="1:1024" ht="21" x14ac:dyDescent="0.35">
       <c r="A13" s="3"/>
-      <c r="B13" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="C13" s="42"/>
+      <c r="B13" s="59" t="s">
+        <v>90</v>
+      </c>
+      <c r="C13" s="60"/>
     </row>
     <row r="14" spans="1:1024" ht="21" x14ac:dyDescent="0.35">
       <c r="A14" s="3"/>
       <c r="B14" s="26" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C14" s="27" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="15" spans="1:1024" ht="21" x14ac:dyDescent="0.35">
       <c r="A15" s="3"/>
-      <c r="B15" s="40" t="s">
-        <v>95</v>
-      </c>
-      <c r="C15" s="40"/>
+      <c r="B15" s="58" t="s">
+        <v>94</v>
+      </c>
+      <c r="C15" s="58"/>
     </row>
     <row r="16" spans="1:1024" ht="21" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
@@ -4589,7 +4601,7 @@
         <v>79</v>
       </c>
       <c r="C16" s="27" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="21" x14ac:dyDescent="0.35">
@@ -4604,88 +4616,88 @@
     <row r="18" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A18" s="3"/>
       <c r="B18" s="26" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C18" s="27" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A19" s="3"/>
       <c r="B19" s="26" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C19" s="27" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A20" s="3"/>
       <c r="B20" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="C20" s="27" t="s">
         <v>108</v>
-      </c>
-      <c r="C20" s="27" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A21" s="3"/>
-      <c r="B21" s="41" t="s">
-        <v>116</v>
-      </c>
-      <c r="C21" s="42"/>
+      <c r="B21" s="59" t="s">
+        <v>115</v>
+      </c>
+      <c r="C21" s="60"/>
     </row>
     <row r="22" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A22" s="3"/>
       <c r="B22" s="30" t="s">
+        <v>116</v>
+      </c>
+      <c r="C22" s="30" t="s">
         <v>117</v>
-      </c>
-      <c r="C22" s="30" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A23" s="3"/>
       <c r="B23" s="30" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C23" s="30" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A24" s="3"/>
       <c r="B24" s="30" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C24" s="30" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A25" s="3"/>
       <c r="B25" s="30" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C25" s="30" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A26" s="3"/>
       <c r="B26" s="30" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C26" s="30" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A27" s="3"/>
-      <c r="B27" s="41" t="s">
+      <c r="B27" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="C27" s="42"/>
+      <c r="C27" s="60"/>
     </row>
     <row r="28" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A28" s="3"/>
@@ -4693,322 +4705,324 @@
         <v>35</v>
       </c>
       <c r="C28" s="27" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A29" s="3"/>
-      <c r="B29" s="43" t="s">
-        <v>94</v>
-      </c>
-      <c r="C29" s="43"/>
+      <c r="B29" s="61" t="s">
+        <v>93</v>
+      </c>
+      <c r="C29" s="61"/>
     </row>
     <row r="30" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A30" s="3"/>
       <c r="B30" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="C30" s="27" t="s">
         <v>92</v>
-      </c>
-      <c r="C30" s="27" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A31" s="3"/>
       <c r="B31" s="27" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C31" s="27" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="32" spans="1:3" s="4" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B32" s="38" t="s">
-        <v>111</v>
-      </c>
-      <c r="C32" s="38"/>
-    </row>
-    <row r="33" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B33" s="51" t="s">
+      <c r="B32" s="56" t="s">
+        <v>110</v>
+      </c>
+      <c r="C32" s="56"/>
+    </row>
+    <row r="33" spans="1:3" s="4" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B33" s="34" t="s">
+        <v>140</v>
+      </c>
+      <c r="C33" s="34"/>
+    </row>
+    <row r="34" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B34" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="C34" s="29" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B35" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="C33" s="51"/>
-    </row>
-    <row r="34" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B34" s="57" t="s">
+      <c r="C35" s="34"/>
+    </row>
+    <row r="36" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B36" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="C34" s="58"/>
-    </row>
-    <row r="35" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B35" s="28" t="s">
-        <v>80</v>
-      </c>
-      <c r="C35" s="29" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="C36" s="29" t="s">
-        <v>6</v>
-      </c>
+      <c r="C36" s="42"/>
     </row>
     <row r="37" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B37" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="C37" s="29" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B38" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="C38" s="29" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B39" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="C37" s="29" t="s">
+      <c r="C39" s="29" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B38" s="28" t="s">
-        <v>82</v>
-      </c>
-      <c r="C38" s="29" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B39" s="57" t="s">
-        <v>84</v>
-      </c>
-      <c r="C39" s="58"/>
     </row>
     <row r="40" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B40" s="28" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C40" s="29" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B41" s="28" t="s">
-        <v>87</v>
-      </c>
-      <c r="C41" s="29" t="s">
-        <v>88</v>
-      </c>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B41" s="41" t="s">
+        <v>84</v>
+      </c>
+      <c r="C41" s="42"/>
     </row>
     <row r="42" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B42" s="28" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C42" s="29" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B43" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="C43" s="29" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B44" s="41" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B43" s="57" t="s">
-        <v>91</v>
-      </c>
-      <c r="C43" s="58"/>
-    </row>
-    <row r="44" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A44" s="3"/>
-      <c r="B44" s="28" t="s">
+      <c r="C44" s="42"/>
+    </row>
+    <row r="45" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="A45" s="3"/>
+      <c r="B45" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="C45" s="30" t="s">
         <v>102</v>
       </c>
-      <c r="C44" s="30" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="3"/>
-      <c r="B45" s="59" t="s">
-        <v>95</v>
-      </c>
-      <c r="C45" s="59"/>
     </row>
     <row r="46" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="3"/>
-      <c r="B46" s="30" t="s">
-        <v>99</v>
-      </c>
-      <c r="C46" s="27" t="s">
-        <v>112</v>
-      </c>
+      <c r="B46" s="43" t="s">
+        <v>94</v>
+      </c>
+      <c r="C46" s="43"/>
     </row>
     <row r="47" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="3"/>
       <c r="B47" s="30" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C47" s="27" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="3"/>
-      <c r="B48" s="60" t="s">
-        <v>116</v>
-      </c>
-      <c r="C48" s="61"/>
+      <c r="B48" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="C48" s="27" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="49" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="3"/>
-      <c r="B49" s="30" t="s">
-        <v>124</v>
-      </c>
-      <c r="C49" s="27" t="s">
-        <v>129</v>
-      </c>
+      <c r="B49" s="44" t="s">
+        <v>115</v>
+      </c>
+      <c r="C49" s="45"/>
     </row>
     <row r="50" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="3"/>
       <c r="B50" s="30" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C50" s="27" t="s">
-        <v>128</v>
+        <v>142</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="3"/>
       <c r="B51" s="30" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C51" s="27" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="52" spans="1:3" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B52" s="24"/>
-      <c r="C52" s="24"/>
-    </row>
-    <row r="53" spans="1:3" s="4" customFormat="1" ht="61.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B53" s="56" t="s">
-        <v>104</v>
-      </c>
-      <c r="C53" s="56"/>
-    </row>
-    <row r="54" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B54" s="36" t="s">
+    <row r="52" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="3"/>
+      <c r="B52" s="30" t="s">
+        <v>125</v>
+      </c>
+      <c r="C52" s="27" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B53" s="24"/>
+      <c r="C53" s="24"/>
+    </row>
+    <row r="54" spans="1:3" s="4" customFormat="1" ht="61.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B54" s="40" t="s">
+        <v>103</v>
+      </c>
+      <c r="C54" s="40"/>
+    </row>
+    <row r="55" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B55" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="C54" s="36"/>
-    </row>
-    <row r="55" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B55" s="13" t="s">
+      <c r="C55" s="37"/>
+    </row>
+    <row r="56" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B56" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C55" s="13" t="s">
+      <c r="C56" s="13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B56" s="54" t="s">
+    <row r="57" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B57" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="C56" s="55"/>
-    </row>
-    <row r="57" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B57" s="31" t="s">
+      <c r="C57" s="39"/>
+    </row>
+    <row r="58" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B58" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="C57" s="31" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B58" s="14"/>
-      <c r="C58" s="14"/>
-    </row>
-    <row r="59" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B59" s="52" t="s">
+      <c r="C58" s="31" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B59" s="14"/>
+      <c r="C59" s="14"/>
+    </row>
+    <row r="60" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B60" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="C59" s="53"/>
-    </row>
-    <row r="60" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B60" s="46" t="s">
+      <c r="C60" s="36"/>
+    </row>
+    <row r="61" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B61" s="48" t="s">
         <v>66</v>
       </c>
-      <c r="C60" s="47"/>
-    </row>
-    <row r="61" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B61" s="48"/>
       <c r="C61" s="49"/>
     </row>
-    <row r="62" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B62" s="14"/>
-      <c r="C62" s="14"/>
-    </row>
-    <row r="63" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B63" s="36" t="s">
+    <row r="62" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B62" s="50"/>
+      <c r="C62" s="51"/>
+    </row>
+    <row r="63" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B63" s="14"/>
+      <c r="C63" s="14"/>
+    </row>
+    <row r="64" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B64" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="C63" s="36"/>
-    </row>
-    <row r="64" spans="1:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B64" s="50" t="s">
+      <c r="C64" s="37"/>
+    </row>
+    <row r="65" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B65" s="52" t="s">
         <v>64</v>
       </c>
-      <c r="C64" s="50"/>
-    </row>
-    <row r="65" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B65" s="50"/>
-      <c r="C65" s="50"/>
-    </row>
-    <row r="66" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B66" s="16"/>
-      <c r="C66" s="17"/>
-    </row>
-    <row r="67" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A67" s="5"/>
-      <c r="B67" s="45" t="s">
+      <c r="C65" s="52"/>
+    </row>
+    <row r="66" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B66" s="52"/>
+      <c r="C66" s="52"/>
+    </row>
+    <row r="67" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B67" s="16"/>
+      <c r="C67" s="17"/>
+    </row>
+    <row r="68" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A68" s="5"/>
+      <c r="B68" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="C67" s="45"/>
-    </row>
-    <row r="68" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B68" s="44" t="s">
-        <v>135</v>
-      </c>
-      <c r="C68" s="44"/>
-    </row>
-    <row r="69" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B69" s="18"/>
-      <c r="C69" s="18"/>
-    </row>
-    <row r="70" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="B70" s="17"/>
-      <c r="C70" s="17"/>
-    </row>
-    <row r="71" spans="1:8" ht="21" x14ac:dyDescent="0.2">
-      <c r="B71" s="19" t="s">
+      <c r="C68" s="47"/>
+    </row>
+    <row r="69" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B69" s="46" t="s">
+        <v>143</v>
+      </c>
+      <c r="C69" s="46"/>
+    </row>
+    <row r="70" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B70" s="18"/>
+      <c r="C70" s="18"/>
+    </row>
+    <row r="71" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="B71" s="17"/>
+      <c r="C71" s="17"/>
+    </row>
+    <row r="72" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="B72" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="C71" s="19" t="s">
+      <c r="C72" s="19" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="72" spans="1:8" ht="21" x14ac:dyDescent="0.2">
-      <c r="A72" s="6"/>
-      <c r="B72" s="32" t="s">
-        <v>136</v>
-      </c>
-      <c r="C72" s="33" t="s">
+    <row r="73" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A73" s="6"/>
+      <c r="B73" s="32" t="s">
+        <v>133</v>
+      </c>
+      <c r="C73" s="33" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="B74" s="32" t="s">
+        <v>112</v>
+      </c>
+      <c r="C74" s="33" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="73" spans="1:8" ht="21" x14ac:dyDescent="0.2">
-      <c r="B73" s="32" t="s">
-        <v>113</v>
-      </c>
-      <c r="C73" s="33" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A74" s="5"/>
-      <c r="B74" s="6"/>
-      <c r="C74" s="6"/>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A75" s="5"/>
       <c r="B75" s="6"/>
       <c r="C75" s="6"/>
     </row>
@@ -5023,11 +5037,6 @@
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B78" s="6"/>
       <c r="C78" s="6"/>
-      <c r="D78" s="6"/>
-      <c r="E78" s="6"/>
-      <c r="F78" s="6"/>
-      <c r="G78" s="6"/>
-      <c r="H78" s="6"/>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B79" s="6"/>
@@ -5381,6 +5390,8 @@
       <c r="H117" s="6"/>
     </row>
     <row r="118" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B118" s="6"/>
+      <c r="C118" s="6"/>
       <c r="D118" s="6"/>
       <c r="E118" s="6"/>
       <c r="F118" s="6"/>
@@ -5408,23 +5419,16 @@
       <c r="G121" s="6"/>
       <c r="H121" s="6"/>
     </row>
+    <row r="122" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="D122" s="6"/>
+      <c r="E122" s="6"/>
+      <c r="F122" s="6"/>
+      <c r="G122" s="6"/>
+      <c r="H122" s="6"/>
+    </row>
   </sheetData>
-  <mergeCells count="27">
+  <mergeCells count="28">
     <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B60:C61"/>
-    <mergeCell ref="B64:C65"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B1:C1"/>
@@ -5437,10 +5441,25 @@
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="B29:C29"/>
     <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B61:C62"/>
+    <mergeCell ref="B65:C66"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B49:C49"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C72" r:id="rId1"/>
-    <hyperlink ref="C73" r:id="rId2"/>
+    <hyperlink ref="C73" r:id="rId1"/>
+    <hyperlink ref="C74" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId3"/>
@@ -5455,7 +5474,7 @@
       <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="47.28515625"/>
     <col min="3" max="3" width="32"/>

</xml_diff>

<commit_message>
Actualizacion plan de configuracion , agregando seccion cambios
</commit_message>
<xml_diff>
--- a/Organización/Configuración/Plan_Configuración.xlsx
+++ b/Organización/Configuración/Plan_Configuración.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Novela\Documents\Qualtop\SOS\Organización\Configuración\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="875"/>
   </bookViews>
@@ -26,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="148">
   <si>
     <t>Plan de Administración de Configuración</t>
   </si>
@@ -330,9 +325,6 @@
     <t>Plan_Configuración</t>
   </si>
   <si>
-    <t>Requerimientos + Estimación + Plan_de_proyecto</t>
-  </si>
-  <si>
     <t>Checklist de calidad</t>
   </si>
   <si>
@@ -469,6 +461,21 @@
   </si>
   <si>
     <t>Se genera un respaldo del CRM en forma semanal cuyo responsable de ejecución es:</t>
+  </si>
+  <si>
+    <t>PTL de cambios</t>
+  </si>
+  <si>
+    <t>PTL_Solicitud_Cambios</t>
+  </si>
+  <si>
+    <t>Solicitud de cambio</t>
+  </si>
+  <si>
+    <t>Solicitud de cambios_aammdd</t>
+  </si>
+  <si>
+    <t>Requerimientos (Al finalizar etapa de Ventas) + Estimación(Al finalizar etapa de ventas) + Plan_de_proyecto(Al finalizar etapa de planeación)</t>
   </si>
 </sst>
 </file>
@@ -593,7 +600,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="18">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -694,6 +701,12 @@
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor rgb="FFCFE7F5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor rgb="FFC0C0C0"/>
       </patternFill>
     </fill>
   </fills>
@@ -824,7 +837,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -871,9 +884,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -904,13 +914,61 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -937,57 +995,15 @@
     <xf numFmtId="0" fontId="6" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1072,7 +1088,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1114,7 +1130,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1149,7 +1165,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1358,17 +1374,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMJ122"/>
+  <dimension ref="A1:AMJ125"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="585" ySplit="2940" topLeftCell="B34" activePane="bottomRight"/>
-      <selection activeCell="A26" sqref="A26"/>
-      <selection pane="topRight" activeCell="C9" sqref="C9"/>
-      <selection pane="bottomLeft" activeCell="A34" sqref="A34:XFD34"/>
-      <selection pane="bottomRight" activeCell="C48" sqref="C48"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A62" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B72" sqref="B72:C72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.85546875" style="1"/>
     <col min="2" max="2" width="53.5703125" style="1" customWidth="1"/>
@@ -1417,17 +1429,17 @@
   <sheetData>
     <row r="1" spans="1:1024" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
-      <c r="B1" s="55" t="s">
+      <c r="B1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="55"/>
+      <c r="C1" s="37"/>
     </row>
     <row r="2" spans="1:1024" s="22" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="21"/>
-      <c r="B2" s="57" t="s">
-        <v>136</v>
-      </c>
-      <c r="C2" s="57"/>
+      <c r="B2" s="39" t="s">
+        <v>135</v>
+      </c>
+      <c r="C2" s="39"/>
       <c r="D2" s="15"/>
       <c r="E2" s="21"/>
       <c r="F2" s="21"/>
@@ -2452,8 +2464,8 @@
     </row>
     <row r="3" spans="1:1024" s="22" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="21"/>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
       <c r="D3" s="15"/>
       <c r="E3" s="21"/>
       <c r="F3" s="21"/>
@@ -3478,10 +3490,10 @@
     </row>
     <row r="4" spans="1:1024" s="22" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A4" s="23"/>
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="C4" s="37"/>
+      <c r="C4" s="36"/>
       <c r="D4" s="21"/>
       <c r="E4" s="21"/>
       <c r="F4" s="21"/>
@@ -4506,10 +4518,10 @@
     </row>
     <row r="5" spans="1:1024" ht="21" x14ac:dyDescent="0.35">
       <c r="A5" s="3"/>
-      <c r="B5" s="56" t="s">
+      <c r="B5" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="C5" s="56"/>
+      <c r="C5" s="38"/>
     </row>
     <row r="6" spans="1:1024" ht="21" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
@@ -4522,548 +4534,547 @@
     </row>
     <row r="7" spans="1:1024" ht="21" x14ac:dyDescent="0.35">
       <c r="A7" s="3"/>
-      <c r="B7" s="59" t="s">
+      <c r="B7" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="60"/>
+      <c r="C7" s="42"/>
     </row>
     <row r="8" spans="1:1024" ht="21" x14ac:dyDescent="0.35">
       <c r="A8" s="3"/>
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="C8" s="27" t="s">
-        <v>139</v>
+      <c r="C8" s="26" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="9" spans="1:1024" ht="21" x14ac:dyDescent="0.35">
       <c r="A9" s="3"/>
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="C9" s="27" t="s">
-        <v>138</v>
+      <c r="C9" s="26" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:1024" ht="21" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B10" s="53" t="s">
+      <c r="B10" s="34" t="s">
         <v>84</v>
       </c>
-      <c r="C10" s="54"/>
+      <c r="C10" s="35"/>
     </row>
     <row r="11" spans="1:1024" ht="21" x14ac:dyDescent="0.35">
       <c r="A11" s="3"/>
-      <c r="B11" s="26" t="s">
+      <c r="B11" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="C11" s="27" t="s">
-        <v>137</v>
+      <c r="C11" s="26" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="12" spans="1:1024" ht="21" x14ac:dyDescent="0.35">
       <c r="A12" s="3"/>
-      <c r="B12" s="26" t="s">
+      <c r="B12" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="C12" s="27" t="s">
+      <c r="C12" s="26" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:1024" ht="21" x14ac:dyDescent="0.35">
       <c r="A13" s="3"/>
-      <c r="B13" s="59" t="s">
+      <c r="B13" s="41" t="s">
         <v>90</v>
       </c>
-      <c r="C13" s="60"/>
+      <c r="C13" s="42"/>
     </row>
     <row r="14" spans="1:1024" ht="21" x14ac:dyDescent="0.35">
       <c r="A14" s="3"/>
-      <c r="B14" s="26" t="s">
+      <c r="B14" s="25" t="s">
+        <v>130</v>
+      </c>
+      <c r="C14" s="26" t="s">
         <v>131</v>
-      </c>
-      <c r="C14" s="27" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="15" spans="1:1024" ht="21" x14ac:dyDescent="0.35">
       <c r="A15" s="3"/>
-      <c r="B15" s="58" t="s">
+      <c r="B15" s="40" t="s">
         <v>94</v>
       </c>
-      <c r="C15" s="58"/>
+      <c r="C15" s="40"/>
     </row>
     <row r="16" spans="1:1024" ht="21" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
-      <c r="B16" s="27" t="s">
+      <c r="B16" s="26" t="s">
         <v>79</v>
       </c>
-      <c r="C16" s="27" t="s">
+      <c r="C16" s="26" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A17" s="3"/>
-      <c r="B17" s="26" t="s">
+      <c r="B17" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="C17" s="27" t="s">
+      <c r="C17" s="26" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A18" s="3"/>
-      <c r="B18" s="26" t="s">
-        <v>104</v>
-      </c>
-      <c r="C18" s="27" t="s">
-        <v>106</v>
+      <c r="B18" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="C18" s="26" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A19" s="3"/>
-      <c r="B19" s="26" t="s">
-        <v>105</v>
-      </c>
-      <c r="C19" s="27" t="s">
-        <v>109</v>
+      <c r="B19" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="C19" s="26" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A20" s="3"/>
-      <c r="B20" s="26" t="s">
+      <c r="B20" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="C20" s="26" t="s">
         <v>107</v>
-      </c>
-      <c r="C20" s="27" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A21" s="3"/>
-      <c r="B21" s="59" t="s">
-        <v>115</v>
-      </c>
-      <c r="C21" s="60"/>
+      <c r="B21" s="41" t="s">
+        <v>114</v>
+      </c>
+      <c r="C21" s="42"/>
     </row>
     <row r="22" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A22" s="3"/>
-      <c r="B22" s="30" t="s">
+      <c r="B22" s="29" t="s">
+        <v>115</v>
+      </c>
+      <c r="C22" s="29" t="s">
         <v>116</v>
-      </c>
-      <c r="C22" s="30" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A23" s="3"/>
-      <c r="B23" s="30" t="s">
-        <v>119</v>
-      </c>
-      <c r="C23" s="30" t="s">
+      <c r="B23" s="29" t="s">
         <v>118</v>
+      </c>
+      <c r="C23" s="29" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A24" s="3"/>
-      <c r="B24" s="30" t="s">
+      <c r="B24" s="29" t="s">
+        <v>128</v>
+      </c>
+      <c r="C24" s="29" t="s">
         <v>129</v>
-      </c>
-      <c r="C24" s="30" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A25" s="3"/>
-      <c r="B25" s="30" t="s">
-        <v>120</v>
-      </c>
-      <c r="C25" s="30" t="s">
-        <v>122</v>
+      <c r="B25" s="29" t="s">
+        <v>119</v>
+      </c>
+      <c r="C25" s="29" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A26" s="3"/>
-      <c r="B26" s="30" t="s">
-        <v>121</v>
-      </c>
-      <c r="C26" s="30" t="s">
-        <v>128</v>
+      <c r="B26" s="29" t="s">
+        <v>120</v>
+      </c>
+      <c r="C26" s="29" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A27" s="3"/>
-      <c r="B27" s="59" t="s">
+      <c r="B27" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="C27" s="60"/>
+      <c r="C27" s="42"/>
     </row>
     <row r="28" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A28" s="3"/>
-      <c r="B28" s="27" t="s">
+      <c r="B28" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="C28" s="27" t="s">
+      <c r="C28" s="26" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A29" s="3"/>
-      <c r="B29" s="61" t="s">
+      <c r="B29" s="43" t="s">
         <v>93</v>
       </c>
-      <c r="C29" s="61"/>
+      <c r="C29" s="43"/>
     </row>
     <row r="30" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A30" s="3"/>
-      <c r="B30" s="27" t="s">
+      <c r="B30" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="C30" s="27" t="s">
+      <c r="C30" s="26" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A31" s="3"/>
-      <c r="B31" s="27" t="s">
+      <c r="B31" s="26" t="s">
+        <v>133</v>
+      </c>
+      <c r="C31" s="26" t="s">
         <v>134</v>
       </c>
-      <c r="C31" s="27" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" s="4" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B32" s="56" t="s">
-        <v>110</v>
-      </c>
-      <c r="C32" s="56"/>
-    </row>
-    <row r="33" spans="1:3" s="4" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B33" s="34" t="s">
+    </row>
+    <row r="32" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="A32" s="3"/>
+      <c r="B32" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32" s="42"/>
+    </row>
+    <row r="33" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="A33" s="3"/>
+      <c r="B33" s="26" t="s">
+        <v>143</v>
+      </c>
+      <c r="C33" s="26" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" s="4" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B34" s="38" t="s">
+        <v>109</v>
+      </c>
+      <c r="C34" s="38"/>
+    </row>
+    <row r="35" spans="1:3" s="4" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B35" s="33" t="s">
+        <v>139</v>
+      </c>
+      <c r="C35" s="33"/>
+    </row>
+    <row r="36" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B36" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="C36" s="28" t="s">
         <v>140</v>
       </c>
-      <c r="C33" s="34"/>
-    </row>
-    <row r="34" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B34" s="28" t="s">
-        <v>89</v>
-      </c>
-      <c r="C34" s="29" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B35" s="34" t="s">
+    </row>
+    <row r="37" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B37" s="33" t="s">
         <v>78</v>
       </c>
-      <c r="C35" s="34"/>
-    </row>
-    <row r="36" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="41" t="s">
+      <c r="C37" s="33"/>
+    </row>
+    <row r="38" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B38" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="C36" s="42"/>
-    </row>
-    <row r="37" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B37" s="28" t="s">
+      <c r="C38" s="57"/>
+    </row>
+    <row r="39" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B39" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="C37" s="29" t="s">
+      <c r="C39" s="28" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B38" s="28" t="s">
+    <row r="40" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B40" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="C38" s="29" t="s">
+      <c r="C40" s="28" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B39" s="28" t="s">
+    <row r="41" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B41" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="C39" s="29" t="s">
+      <c r="C41" s="28" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B40" s="28" t="s">
+    <row r="42" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B42" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="C40" s="29" t="s">
+      <c r="C42" s="28" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B41" s="41" t="s">
+    <row r="43" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B43" s="56" t="s">
         <v>84</v>
       </c>
-      <c r="C41" s="42"/>
-    </row>
-    <row r="42" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B42" s="28" t="s">
+      <c r="C43" s="57"/>
+    </row>
+    <row r="44" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B44" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="C42" s="29" t="s">
+      <c r="C44" s="28" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B43" s="28" t="s">
+    <row r="45" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B45" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="C43" s="29" t="s">
+      <c r="C45" s="28" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B44" s="41" t="s">
+    <row r="46" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B46" s="56" t="s">
         <v>90</v>
       </c>
-      <c r="C44" s="42"/>
-    </row>
-    <row r="45" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A45" s="3"/>
-      <c r="B45" s="28" t="s">
+      <c r="C46" s="57"/>
+    </row>
+    <row r="47" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="A47" s="3"/>
+      <c r="B47" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="C47" s="29" t="s">
         <v>101</v>
-      </c>
-      <c r="C45" s="30" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="3"/>
-      <c r="B46" s="43" t="s">
-        <v>94</v>
-      </c>
-      <c r="C46" s="43"/>
-    </row>
-    <row r="47" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="3"/>
-      <c r="B47" s="30" t="s">
-        <v>98</v>
-      </c>
-      <c r="C47" s="27" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="3"/>
-      <c r="B48" s="30" t="s">
-        <v>99</v>
-      </c>
-      <c r="C48" s="27" t="s">
-        <v>100</v>
-      </c>
+      <c r="B48" s="58" t="s">
+        <v>94</v>
+      </c>
+      <c r="C48" s="58"/>
     </row>
     <row r="49" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="3"/>
-      <c r="B49" s="44" t="s">
-        <v>115</v>
-      </c>
-      <c r="C49" s="45"/>
+      <c r="B49" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="C49" s="26" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="50" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="3"/>
-      <c r="B50" s="30" t="s">
-        <v>123</v>
-      </c>
-      <c r="C50" s="27" t="s">
-        <v>142</v>
+      <c r="B50" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="C50" s="26" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="3"/>
-      <c r="B51" s="30" t="s">
-        <v>124</v>
-      </c>
-      <c r="C51" s="27" t="s">
-        <v>127</v>
-      </c>
+      <c r="B51" s="59" t="s">
+        <v>114</v>
+      </c>
+      <c r="C51" s="60"/>
     </row>
     <row r="52" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="3"/>
-      <c r="B52" s="30" t="s">
+      <c r="B52" s="29" t="s">
+        <v>122</v>
+      </c>
+      <c r="C52" s="26" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="3"/>
+      <c r="B53" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="C53" s="26" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="3"/>
+      <c r="B54" s="29" t="s">
+        <v>124</v>
+      </c>
+      <c r="C54" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="C52" s="27" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B53" s="24"/>
-      <c r="C53" s="24"/>
-    </row>
-    <row r="54" spans="1:3" s="4" customFormat="1" ht="61.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B54" s="40" t="s">
-        <v>103</v>
-      </c>
-      <c r="C54" s="40"/>
-    </row>
-    <row r="55" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B55" s="37" t="s">
+    </row>
+    <row r="55" spans="1:3" s="4" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B55" s="61" t="s">
+        <v>7</v>
+      </c>
+      <c r="C55" s="61"/>
+    </row>
+    <row r="56" spans="1:3" s="4" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B56" s="62" t="s">
+        <v>145</v>
+      </c>
+      <c r="C56" s="62" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" s="4" customFormat="1" ht="61.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B57" s="55" t="s">
+        <v>102</v>
+      </c>
+      <c r="C57" s="55"/>
+    </row>
+    <row r="58" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B58" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="C55" s="37"/>
-    </row>
-    <row r="56" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B56" s="13" t="s">
+      <c r="C58" s="36"/>
+    </row>
+    <row r="59" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B59" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C56" s="13" t="s">
+      <c r="C59" s="13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B57" s="38" t="s">
+    <row r="60" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B60" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="C57" s="39"/>
-    </row>
-    <row r="58" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B58" s="31" t="s">
+      <c r="C60" s="54"/>
+    </row>
+    <row r="61" spans="1:3" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B61" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="C58" s="31" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B59" s="14"/>
-      <c r="C59" s="14"/>
-    </row>
-    <row r="60" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B60" s="35" t="s">
+      <c r="C61" s="30" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B62" s="14"/>
+      <c r="C62" s="14"/>
+    </row>
+    <row r="63" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B63" s="51" t="s">
         <v>63</v>
       </c>
-      <c r="C60" s="36"/>
-    </row>
-    <row r="61" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B61" s="48" t="s">
+      <c r="C63" s="52"/>
+    </row>
+    <row r="64" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B64" s="46" t="s">
         <v>66</v>
       </c>
-      <c r="C61" s="49"/>
-    </row>
-    <row r="62" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B62" s="50"/>
-      <c r="C62" s="51"/>
-    </row>
-    <row r="63" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B63" s="14"/>
-      <c r="C63" s="14"/>
-    </row>
-    <row r="64" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B64" s="37" t="s">
+      <c r="C64" s="47"/>
+    </row>
+    <row r="65" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B65" s="48"/>
+      <c r="C65" s="49"/>
+    </row>
+    <row r="66" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B66" s="14"/>
+      <c r="C66" s="14"/>
+    </row>
+    <row r="67" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B67" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="C64" s="37"/>
-    </row>
-    <row r="65" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B65" s="52" t="s">
+      <c r="C67" s="36"/>
+    </row>
+    <row r="68" spans="1:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B68" s="50" t="s">
         <v>64</v>
       </c>
-      <c r="C65" s="52"/>
-    </row>
-    <row r="66" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B66" s="52"/>
-      <c r="C66" s="52"/>
-    </row>
-    <row r="67" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B67" s="16"/>
-      <c r="C67" s="17"/>
-    </row>
-    <row r="68" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A68" s="5"/>
-      <c r="B68" s="47" t="s">
+      <c r="C68" s="50"/>
+    </row>
+    <row r="69" spans="1:3" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B69" s="50"/>
+      <c r="C69" s="50"/>
+    </row>
+    <row r="70" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B70" s="16"/>
+      <c r="C70" s="17"/>
+    </row>
+    <row r="71" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A71" s="5"/>
+      <c r="B71" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="C68" s="47"/>
-    </row>
-    <row r="69" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B69" s="46" t="s">
-        <v>143</v>
-      </c>
-      <c r="C69" s="46"/>
-    </row>
-    <row r="70" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B70" s="18"/>
-      <c r="C70" s="18"/>
-    </row>
-    <row r="71" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="B71" s="17"/>
-      <c r="C71" s="17"/>
-    </row>
-    <row r="72" spans="1:8" ht="21" x14ac:dyDescent="0.2">
-      <c r="B72" s="19" t="s">
+      <c r="C71" s="45"/>
+    </row>
+    <row r="72" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B72" s="44" t="s">
+        <v>142</v>
+      </c>
+      <c r="C72" s="44"/>
+    </row>
+    <row r="73" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B73" s="18"/>
+      <c r="C73" s="18"/>
+    </row>
+    <row r="74" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="B74" s="17"/>
+      <c r="C74" s="17"/>
+    </row>
+    <row r="75" spans="1:3" ht="21" x14ac:dyDescent="0.2">
+      <c r="B75" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="C72" s="19" t="s">
+      <c r="C75" s="19" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="73" spans="1:8" ht="21" x14ac:dyDescent="0.2">
-      <c r="A73" s="6"/>
-      <c r="B73" s="32" t="s">
-        <v>133</v>
-      </c>
-      <c r="C73" s="33" t="s">
+    <row r="76" spans="1:3" ht="21" x14ac:dyDescent="0.2">
+      <c r="A76" s="6"/>
+      <c r="B76" s="31" t="s">
+        <v>132</v>
+      </c>
+      <c r="C76" s="32" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="21" x14ac:dyDescent="0.2">
+      <c r="B77" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="C77" s="32" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="21" x14ac:dyDescent="0.2">
-      <c r="B74" s="32" t="s">
-        <v>112</v>
-      </c>
-      <c r="C74" s="33" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A75" s="5"/>
-      <c r="B75" s="6"/>
-      <c r="C75" s="6"/>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B76" s="6"/>
-      <c r="C76" s="6"/>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B77" s="6"/>
-      <c r="C77" s="6"/>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A78" s="5"/>
       <c r="B78" s="6"/>
       <c r="C78" s="6"/>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B79" s="6"/>
       <c r="C79" s="6"/>
-      <c r="D79" s="6"/>
-      <c r="E79" s="6"/>
-      <c r="F79" s="6"/>
-      <c r="G79" s="6"/>
-      <c r="H79" s="6"/>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B80" s="6"/>
       <c r="C80" s="6"/>
-      <c r="D80" s="6"/>
-      <c r="E80" s="6"/>
-      <c r="F80" s="6"/>
-      <c r="G80" s="6"/>
-      <c r="H80" s="6"/>
     </row>
     <row r="81" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B81" s="6"/>
       <c r="C81" s="6"/>
-      <c r="D81" s="6"/>
-      <c r="E81" s="6"/>
-      <c r="F81" s="6"/>
-      <c r="G81" s="6"/>
-      <c r="H81" s="6"/>
     </row>
     <row r="82" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B82" s="6"/>
@@ -5399,6 +5410,8 @@
       <c r="H118" s="6"/>
     </row>
     <row r="119" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B119" s="6"/>
+      <c r="C119" s="6"/>
       <c r="D119" s="6"/>
       <c r="E119" s="6"/>
       <c r="F119" s="6"/>
@@ -5406,6 +5419,8 @@
       <c r="H119" s="6"/>
     </row>
     <row r="120" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B120" s="6"/>
+      <c r="C120" s="6"/>
       <c r="D120" s="6"/>
       <c r="E120" s="6"/>
       <c r="F120" s="6"/>
@@ -5413,6 +5428,8 @@
       <c r="H120" s="6"/>
     </row>
     <row r="121" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B121" s="6"/>
+      <c r="C121" s="6"/>
       <c r="D121" s="6"/>
       <c r="E121" s="6"/>
       <c r="F121" s="6"/>
@@ -5426,14 +5443,51 @@
       <c r="G122" s="6"/>
       <c r="H122" s="6"/>
     </row>
+    <row r="123" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="D123" s="6"/>
+      <c r="E123" s="6"/>
+      <c r="F123" s="6"/>
+      <c r="G123" s="6"/>
+      <c r="H123" s="6"/>
+    </row>
+    <row r="124" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="D124" s="6"/>
+      <c r="E124" s="6"/>
+      <c r="F124" s="6"/>
+      <c r="G124" s="6"/>
+      <c r="H124" s="6"/>
+    </row>
+    <row r="125" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="D125" s="6"/>
+      <c r="E125" s="6"/>
+      <c r="F125" s="6"/>
+      <c r="G125" s="6"/>
+      <c r="H125" s="6"/>
+    </row>
   </sheetData>
-  <mergeCells count="28">
-    <mergeCell ref="B33:C33"/>
+  <mergeCells count="30">
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B64:C65"/>
+    <mergeCell ref="B68:C69"/>
+    <mergeCell ref="B35:C35"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B34:C34"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="B21:C21"/>
@@ -5441,25 +5495,11 @@
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="B29:C29"/>
     <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B61:C62"/>
-    <mergeCell ref="B65:C66"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B32:C32"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C73" r:id="rId1"/>
-    <hyperlink ref="C74" r:id="rId2"/>
+    <hyperlink ref="C76" r:id="rId1"/>
+    <hyperlink ref="C77" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId3"/>
@@ -5474,7 +5514,7 @@
       <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="47.28515625"/>
     <col min="3" max="3" width="32"/>

</xml_diff>

<commit_message>
actualizacion plan de configuracion
</commit_message>
<xml_diff>
--- a/Organización/Configuración/Plan_Configuración.xlsx
+++ b/Organización/Configuración/Plan_Configuración.xlsx
@@ -373,9 +373,6 @@
     <t>https://github.com/Ricardo5/SOSQTP</t>
   </si>
   <si>
-    <t>https://www.bitrix24.net</t>
-  </si>
-  <si>
     <t>Métricas y monitoreo</t>
   </si>
   <si>
@@ -460,9 +457,6 @@
     <t>Concentrado_métricas_aammdd</t>
   </si>
   <si>
-    <t>Se genera un respaldo del CRM en forma semanal cuyo responsable de ejecución es:</t>
-  </si>
-  <si>
     <t>PTL de cambios</t>
   </si>
   <si>
@@ -476,6 +470,12 @@
   </si>
   <si>
     <t>Requerimientos (Al finalizar etapa de Ventas) + Estimación(Al finalizar etapa de ventas) + Plan_de_proyecto(Al finalizar etapa de planeación)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se imite la integración de un mecanismo de respaldos ya que la herramienta bitrix24 genera respaldos por parte de los creadores de forma diaria en cualqueira de sus planes (gratuito y de pago), sin embargo se especificara el metodo a realizar en caso de que el sistema sufra un daño. En caso de requerir una reposición de la base de datos en bitrix24 será necesario ingresar a la pagina del sistema, click en </t>
+  </si>
+  <si>
+    <t>https://contpaqi911.bitrix24.com/</t>
   </si>
 </sst>
 </file>
@@ -837,7 +837,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -911,64 +911,19 @@
     <xf numFmtId="0" fontId="16" fillId="15" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -998,8 +953,56 @@
     <xf numFmtId="0" fontId="6" fillId="16" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1376,8 +1379,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ125"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A62" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B72" sqref="B72:C72"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A63" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C78" sqref="C78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1429,17 +1432,17 @@
   <sheetData>
     <row r="1" spans="1:1024" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="37"/>
+      <c r="C1" s="55"/>
     </row>
     <row r="2" spans="1:1024" s="22" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="21"/>
-      <c r="B2" s="39" t="s">
-        <v>135</v>
-      </c>
-      <c r="C2" s="39"/>
+      <c r="B2" s="57" t="s">
+        <v>134</v>
+      </c>
+      <c r="C2" s="57"/>
       <c r="D2" s="15"/>
       <c r="E2" s="21"/>
       <c r="F2" s="21"/>
@@ -3490,10 +3493,10 @@
     </row>
     <row r="4" spans="1:1024" s="22" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A4" s="23"/>
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="C4" s="36"/>
+      <c r="C4" s="37"/>
       <c r="D4" s="21"/>
       <c r="E4" s="21"/>
       <c r="F4" s="21"/>
@@ -4518,10 +4521,10 @@
     </row>
     <row r="5" spans="1:1024" ht="21" x14ac:dyDescent="0.35">
       <c r="A5" s="3"/>
-      <c r="B5" s="38" t="s">
+      <c r="B5" s="56" t="s">
         <v>68</v>
       </c>
-      <c r="C5" s="38"/>
+      <c r="C5" s="56"/>
     </row>
     <row r="6" spans="1:1024" ht="21" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
@@ -4534,10 +4537,10 @@
     </row>
     <row r="7" spans="1:1024" ht="21" x14ac:dyDescent="0.35">
       <c r="A7" s="3"/>
-      <c r="B7" s="41" t="s">
+      <c r="B7" s="59" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="42"/>
+      <c r="C7" s="60"/>
     </row>
     <row r="8" spans="1:1024" ht="21" x14ac:dyDescent="0.35">
       <c r="A8" s="3"/>
@@ -4545,7 +4548,7 @@
         <v>73</v>
       </c>
       <c r="C8" s="26" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="9" spans="1:1024" ht="21" x14ac:dyDescent="0.35">
@@ -4554,17 +4557,17 @@
         <v>72</v>
       </c>
       <c r="C9" s="26" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10" spans="1:1024" ht="21" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B10" s="34" t="s">
+      <c r="B10" s="53" t="s">
         <v>84</v>
       </c>
-      <c r="C10" s="35"/>
+      <c r="C10" s="54"/>
     </row>
     <row r="11" spans="1:1024" ht="21" x14ac:dyDescent="0.35">
       <c r="A11" s="3"/>
@@ -4572,7 +4575,7 @@
         <v>71</v>
       </c>
       <c r="C11" s="26" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="12" spans="1:1024" ht="21" x14ac:dyDescent="0.35">
@@ -4586,26 +4589,26 @@
     </row>
     <row r="13" spans="1:1024" ht="21" x14ac:dyDescent="0.35">
       <c r="A13" s="3"/>
-      <c r="B13" s="41" t="s">
+      <c r="B13" s="59" t="s">
         <v>90</v>
       </c>
-      <c r="C13" s="42"/>
+      <c r="C13" s="60"/>
     </row>
     <row r="14" spans="1:1024" ht="21" x14ac:dyDescent="0.35">
       <c r="A14" s="3"/>
       <c r="B14" s="25" t="s">
+        <v>129</v>
+      </c>
+      <c r="C14" s="26" t="s">
         <v>130</v>
-      </c>
-      <c r="C14" s="26" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="15" spans="1:1024" ht="21" x14ac:dyDescent="0.35">
       <c r="A15" s="3"/>
-      <c r="B15" s="40" t="s">
+      <c r="B15" s="58" t="s">
         <v>94</v>
       </c>
-      <c r="C15" s="40"/>
+      <c r="C15" s="58"/>
     </row>
     <row r="16" spans="1:1024" ht="21" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
@@ -4654,62 +4657,62 @@
     </row>
     <row r="21" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A21" s="3"/>
-      <c r="B21" s="41" t="s">
-        <v>114</v>
-      </c>
-      <c r="C21" s="42"/>
+      <c r="B21" s="59" t="s">
+        <v>113</v>
+      </c>
+      <c r="C21" s="60"/>
     </row>
     <row r="22" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A22" s="3"/>
       <c r="B22" s="29" t="s">
+        <v>114</v>
+      </c>
+      <c r="C22" s="29" t="s">
         <v>115</v>
-      </c>
-      <c r="C22" s="29" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A23" s="3"/>
       <c r="B23" s="29" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C23" s="29" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A24" s="3"/>
       <c r="B24" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="C24" s="29" t="s">
         <v>128</v>
-      </c>
-      <c r="C24" s="29" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A25" s="3"/>
       <c r="B25" s="29" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C25" s="29" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A26" s="3"/>
       <c r="B26" s="29" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C26" s="29" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A27" s="3"/>
-      <c r="B27" s="41" t="s">
+      <c r="B27" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="C27" s="42"/>
+      <c r="C27" s="60"/>
     </row>
     <row r="28" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A28" s="3"/>
@@ -4722,10 +4725,10 @@
     </row>
     <row r="29" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A29" s="3"/>
-      <c r="B29" s="43" t="s">
+      <c r="B29" s="61" t="s">
         <v>93</v>
       </c>
-      <c r="C29" s="43"/>
+      <c r="C29" s="61"/>
     </row>
     <row r="30" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A30" s="3"/>
@@ -4739,59 +4742,59 @@
     <row r="31" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A31" s="3"/>
       <c r="B31" s="26" t="s">
+        <v>132</v>
+      </c>
+      <c r="C31" s="26" t="s">
         <v>133</v>
-      </c>
-      <c r="C31" s="26" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A32" s="3"/>
-      <c r="B32" s="41" t="s">
+      <c r="B32" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="C32" s="42"/>
+      <c r="C32" s="60"/>
     </row>
     <row r="33" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A33" s="3"/>
       <c r="B33" s="26" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C33" s="26" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="34" spans="1:3" s="4" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B34" s="38" t="s">
+      <c r="B34" s="56" t="s">
         <v>109</v>
       </c>
-      <c r="C34" s="38"/>
+      <c r="C34" s="56"/>
     </row>
     <row r="35" spans="1:3" s="4" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B35" s="33" t="s">
-        <v>139</v>
-      </c>
-      <c r="C35" s="33"/>
+      <c r="B35" s="34" t="s">
+        <v>138</v>
+      </c>
+      <c r="C35" s="34"/>
     </row>
     <row r="36" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B36" s="27" t="s">
         <v>89</v>
       </c>
       <c r="C36" s="28" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B37" s="33" t="s">
+      <c r="B37" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="C37" s="33"/>
+      <c r="C37" s="34"/>
     </row>
     <row r="38" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B38" s="56" t="s">
+      <c r="B38" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="C38" s="57"/>
+      <c r="C38" s="42"/>
     </row>
     <row r="39" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B39" s="27" t="s">
@@ -4826,10 +4829,10 @@
       </c>
     </row>
     <row r="43" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B43" s="56" t="s">
+      <c r="B43" s="41" t="s">
         <v>84</v>
       </c>
-      <c r="C43" s="57"/>
+      <c r="C43" s="42"/>
     </row>
     <row r="44" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B44" s="27" t="s">
@@ -4848,10 +4851,10 @@
       </c>
     </row>
     <row r="46" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B46" s="56" t="s">
+      <c r="B46" s="41" t="s">
         <v>90</v>
       </c>
-      <c r="C46" s="57"/>
+      <c r="C46" s="42"/>
     </row>
     <row r="47" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A47" s="3"/>
@@ -4864,10 +4867,10 @@
     </row>
     <row r="48" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="3"/>
-      <c r="B48" s="58" t="s">
+      <c r="B48" s="43" t="s">
         <v>94</v>
       </c>
-      <c r="C48" s="58"/>
+      <c r="C48" s="43"/>
     </row>
     <row r="49" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="3"/>
@@ -4889,63 +4892,63 @@
     </row>
     <row r="51" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="3"/>
-      <c r="B51" s="59" t="s">
-        <v>114</v>
-      </c>
-      <c r="C51" s="60"/>
+      <c r="B51" s="44" t="s">
+        <v>113</v>
+      </c>
+      <c r="C51" s="45"/>
     </row>
     <row r="52" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="3"/>
       <c r="B52" s="29" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C52" s="26" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="3"/>
       <c r="B53" s="29" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C53" s="26" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="3"/>
       <c r="B54" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="C54" s="26" t="s">
         <v>124</v>
       </c>
-      <c r="C54" s="26" t="s">
-        <v>125</v>
-      </c>
     </row>
     <row r="55" spans="1:3" s="4" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B55" s="61" t="s">
+      <c r="B55" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="C55" s="61"/>
+      <c r="C55" s="46"/>
     </row>
     <row r="56" spans="1:3" s="4" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B56" s="62" t="s">
-        <v>145</v>
-      </c>
-      <c r="C56" s="62" t="s">
-        <v>146</v>
+      <c r="B56" s="33" t="s">
+        <v>143</v>
+      </c>
+      <c r="C56" s="33" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="57" spans="1:3" s="4" customFormat="1" ht="61.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B57" s="55" t="s">
+      <c r="B57" s="40" t="s">
         <v>102</v>
       </c>
-      <c r="C57" s="55"/>
+      <c r="C57" s="40"/>
     </row>
     <row r="58" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B58" s="36" t="s">
+      <c r="B58" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="C58" s="36"/>
+      <c r="C58" s="37"/>
     </row>
     <row r="59" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B59" s="13" t="s">
@@ -4956,17 +4959,17 @@
       </c>
     </row>
     <row r="60" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B60" s="53" t="s">
+      <c r="B60" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="C60" s="54"/>
+      <c r="C60" s="39"/>
     </row>
     <row r="61" spans="1:3" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B61" s="30" t="s">
         <v>65</v>
       </c>
       <c r="C61" s="30" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.35">
@@ -4974,40 +4977,40 @@
       <c r="C62" s="14"/>
     </row>
     <row r="63" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B63" s="51" t="s">
+      <c r="B63" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="C63" s="52"/>
+      <c r="C63" s="36"/>
     </row>
     <row r="64" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B64" s="46" t="s">
+      <c r="B64" s="48" t="s">
         <v>66</v>
       </c>
-      <c r="C64" s="47"/>
+      <c r="C64" s="49"/>
     </row>
     <row r="65" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B65" s="48"/>
-      <c r="C65" s="49"/>
+      <c r="B65" s="50"/>
+      <c r="C65" s="51"/>
     </row>
     <row r="66" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B66" s="14"/>
       <c r="C66" s="14"/>
     </row>
     <row r="67" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B67" s="36" t="s">
+      <c r="B67" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="C67" s="36"/>
+      <c r="C67" s="37"/>
     </row>
     <row r="68" spans="1:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B68" s="50" t="s">
+      <c r="B68" s="52" t="s">
         <v>64</v>
       </c>
-      <c r="C68" s="50"/>
+      <c r="C68" s="52"/>
     </row>
     <row r="69" spans="1:3" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B69" s="50"/>
-      <c r="C69" s="50"/>
+      <c r="B69" s="52"/>
+      <c r="C69" s="52"/>
     </row>
     <row r="70" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B70" s="16"/>
@@ -5015,16 +5018,16 @@
     </row>
     <row r="71" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" s="5"/>
-      <c r="B71" s="45" t="s">
+      <c r="B71" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="C71" s="45"/>
-    </row>
-    <row r="72" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B72" s="44" t="s">
-        <v>142</v>
-      </c>
-      <c r="C72" s="44"/>
+      <c r="C71" s="47"/>
+    </row>
+    <row r="72" spans="1:3" ht="87" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B72" s="62" t="s">
+        <v>146</v>
+      </c>
+      <c r="C72" s="63"/>
     </row>
     <row r="73" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B73" s="18"/>
@@ -5045,7 +5048,7 @@
     <row r="76" spans="1:3" ht="21" x14ac:dyDescent="0.2">
       <c r="A76" s="6"/>
       <c r="B76" s="31" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C76" s="32" t="s">
         <v>112</v>
@@ -5056,7 +5059,7 @@
         <v>111</v>
       </c>
       <c r="C77" s="32" t="s">
-        <v>113</v>
+        <v>147</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
@@ -5466,22 +5469,6 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B64:C65"/>
-    <mergeCell ref="B68:C69"/>
     <mergeCell ref="B35:C35"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B4:C4"/>
@@ -5496,6 +5483,22 @@
     <mergeCell ref="B29:C29"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B64:C65"/>
+    <mergeCell ref="B68:C69"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B55:C55"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C76" r:id="rId1"/>

</xml_diff>

<commit_message>
Actualziacion plan deconfiguracionintegrando nueva herramienta detrabajo
</commit_message>
<xml_diff>
--- a/Organización/Configuración/Plan_Configuración.xlsx
+++ b/Organización/Configuración/Plan_Configuración.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="160">
   <si>
     <t>Plan de Administración de Configuración</t>
   </si>
@@ -492,6 +492,27 @@
   <si>
     <t>Carta de aceptación</t>
   </si>
+  <si>
+    <t>Sistema SOS, se respaldara la base de datos al finalizar cada mes, este respaldo se genera con una peridiocidad amplia debido a que su información por lo generar suele ser estatica la mayor parte del tiempo los archivos de respaldo se deberán almacenar en raíz de carpeta repositorio/backup con el nombre aaaamm.sql.</t>
+  </si>
+  <si>
+    <t>Descripción</t>
+  </si>
+  <si>
+    <t>Sos Software</t>
+  </si>
+  <si>
+    <t>http://192.168.100.253 (local)</t>
+  </si>
+  <si>
+    <t>Almacena los prospectos, Deals del cliente, tareas, herramientas de seguimiento.</t>
+  </si>
+  <si>
+    <t>Almacena todas las salidas del ciclo de vida que no se encuentran dentro de bitrix tales como estimación, plan de proyecto, carta de aceptación, cotización, documentos organizacionales, calidad y métricas.</t>
+  </si>
+  <si>
+    <t>Almacena los productos y servicios que vende SOS, usuarios del sistema, roles de la empresa y guías de requerimientos.</t>
+  </si>
 </sst>
 </file>
 
@@ -596,7 +617,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="22">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -693,6 +714,36 @@
         <bgColor rgb="FFEEECE1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FFEEECE1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor rgb="FFEEECE1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="6">
     <border>
@@ -766,50 +817,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -860,9 +869,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -873,20 +879,14 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -897,6 +897,62 @@
     <xf numFmtId="0" fontId="7" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1267,65 +1323,65 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK125"/>
+  <dimension ref="A1:AMK126"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A39" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A74" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D85" sqref="D85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" style="15"/>
-    <col min="2" max="2" width="53.5703125" style="15"/>
-    <col min="3" max="3" width="81.5703125" style="15"/>
-    <col min="4" max="4" width="23.7109375" style="15"/>
-    <col min="5" max="250" width="12.140625" style="15"/>
-    <col min="251" max="251" width="2.85546875" style="15"/>
-    <col min="252" max="252" width="48.7109375" style="15"/>
-    <col min="253" max="253" width="61" style="15"/>
-    <col min="254" max="254" width="32.140625" style="15"/>
-    <col min="255" max="255" width="11.5703125" style="15"/>
-    <col min="256" max="256" width="1.140625" style="15"/>
-    <col min="257" max="257" width="28.7109375" style="15"/>
-    <col min="258" max="258" width="23.7109375" style="15"/>
-    <col min="259" max="259" width="2.42578125" style="15"/>
-    <col min="260" max="260" width="23.7109375" style="15"/>
-    <col min="261" max="506" width="12.140625" style="15"/>
-    <col min="507" max="507" width="2.85546875" style="15"/>
-    <col min="508" max="508" width="48.7109375" style="15"/>
-    <col min="509" max="509" width="61" style="15"/>
-    <col min="510" max="510" width="32.140625" style="15"/>
-    <col min="511" max="511" width="11.5703125" style="15"/>
-    <col min="512" max="512" width="1.140625" style="15"/>
-    <col min="513" max="513" width="28.7109375" style="15"/>
-    <col min="514" max="514" width="23.7109375" style="15"/>
-    <col min="515" max="515" width="2.42578125" style="15"/>
-    <col min="516" max="516" width="23.7109375" style="15"/>
-    <col min="517" max="762" width="12.140625" style="15"/>
-    <col min="763" max="763" width="2.85546875" style="15"/>
-    <col min="764" max="764" width="48.7109375" style="15"/>
-    <col min="765" max="765" width="61" style="15"/>
-    <col min="766" max="766" width="32.140625" style="15"/>
-    <col min="767" max="767" width="11.5703125" style="15"/>
-    <col min="768" max="768" width="1.140625" style="15"/>
-    <col min="769" max="769" width="28.7109375" style="15"/>
-    <col min="770" max="770" width="23.7109375" style="15"/>
-    <col min="771" max="771" width="2.42578125" style="15"/>
-    <col min="772" max="772" width="23.7109375" style="15"/>
-    <col min="773" max="1018" width="12.140625" style="15"/>
-    <col min="1019" max="1019" width="2.85546875" style="15"/>
-    <col min="1020" max="1020" width="48.7109375" style="15"/>
-    <col min="1021" max="1021" width="61" style="15"/>
-    <col min="1022" max="1022" width="32.140625" style="15"/>
-    <col min="1023" max="1025" width="11.5703125" style="15"/>
+    <col min="1" max="1" width="2.85546875" style="1"/>
+    <col min="2" max="2" width="53.5703125" style="1"/>
+    <col min="3" max="3" width="81.5703125" style="1"/>
+    <col min="4" max="4" width="54.42578125" style="1" customWidth="1"/>
+    <col min="5" max="250" width="12.140625" style="1"/>
+    <col min="251" max="251" width="2.85546875" style="1"/>
+    <col min="252" max="252" width="48.7109375" style="1"/>
+    <col min="253" max="253" width="61" style="1"/>
+    <col min="254" max="254" width="32.140625" style="1"/>
+    <col min="255" max="255" width="11.5703125" style="1"/>
+    <col min="256" max="256" width="1.140625" style="1"/>
+    <col min="257" max="257" width="28.7109375" style="1"/>
+    <col min="258" max="258" width="23.7109375" style="1"/>
+    <col min="259" max="259" width="2.42578125" style="1"/>
+    <col min="260" max="260" width="23.7109375" style="1"/>
+    <col min="261" max="506" width="12.140625" style="1"/>
+    <col min="507" max="507" width="2.85546875" style="1"/>
+    <col min="508" max="508" width="48.7109375" style="1"/>
+    <col min="509" max="509" width="61" style="1"/>
+    <col min="510" max="510" width="32.140625" style="1"/>
+    <col min="511" max="511" width="11.5703125" style="1"/>
+    <col min="512" max="512" width="1.140625" style="1"/>
+    <col min="513" max="513" width="28.7109375" style="1"/>
+    <col min="514" max="514" width="23.7109375" style="1"/>
+    <col min="515" max="515" width="2.42578125" style="1"/>
+    <col min="516" max="516" width="23.7109375" style="1"/>
+    <col min="517" max="762" width="12.140625" style="1"/>
+    <col min="763" max="763" width="2.85546875" style="1"/>
+    <col min="764" max="764" width="48.7109375" style="1"/>
+    <col min="765" max="765" width="61" style="1"/>
+    <col min="766" max="766" width="32.140625" style="1"/>
+    <col min="767" max="767" width="11.5703125" style="1"/>
+    <col min="768" max="768" width="1.140625" style="1"/>
+    <col min="769" max="769" width="28.7109375" style="1"/>
+    <col min="770" max="770" width="23.7109375" style="1"/>
+    <col min="771" max="771" width="2.42578125" style="1"/>
+    <col min="772" max="772" width="23.7109375" style="1"/>
+    <col min="773" max="1018" width="12.140625" style="1"/>
+    <col min="1019" max="1019" width="2.85546875" style="1"/>
+    <col min="1020" max="1020" width="48.7109375" style="1"/>
+    <col min="1021" max="1021" width="61" style="1"/>
+    <col min="1022" max="1022" width="32.140625" style="1"/>
+    <col min="1023" max="1025" width="11.5703125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="42" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="16"/>
-      <c r="B1" s="14" t="s">
+      <c r="A1" s="2"/>
+      <c r="B1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="14"/>
+      <c r="C1" s="47"/>
       <c r="D1"/>
       <c r="E1"/>
       <c r="F1"/>
@@ -2348,31 +2404,31 @@
       <c r="AMI1"/>
       <c r="AMJ1"/>
     </row>
-    <row r="2" spans="1:1024" s="17" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="13" t="s">
+    <row r="2" spans="1:1024" s="3" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="18"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="4"/>
     </row>
-    <row r="3" spans="1:1024" s="17" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="18"/>
+    <row r="3" spans="1:1024" s="3" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="4"/>
     </row>
-    <row r="4" spans="1:1024" s="17" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="20"/>
-      <c r="B4" s="12" t="s">
+    <row r="4" spans="1:1024" s="3" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="6"/>
+      <c r="B4" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="12"/>
+      <c r="C4" s="31"/>
     </row>
     <row r="5" spans="1:1024" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="21"/>
-      <c r="B5" s="11" t="s">
+      <c r="A5" s="7"/>
+      <c r="B5" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="11"/>
+      <c r="C5" s="45"/>
       <c r="D5"/>
       <c r="E5"/>
       <c r="F5"/>
@@ -3396,11 +3452,11 @@
       <c r="AMJ5"/>
     </row>
     <row r="6" spans="1:1024" ht="21" x14ac:dyDescent="0.3">
-      <c r="A6" s="21"/>
-      <c r="B6" s="22" t="s">
+      <c r="A6" s="7"/>
+      <c r="B6" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D6"/>
@@ -4426,11 +4482,11 @@
       <c r="AMJ6"/>
     </row>
     <row r="7" spans="1:1024" ht="21" x14ac:dyDescent="0.3">
-      <c r="A7" s="21"/>
-      <c r="B7" s="23" t="s">
+      <c r="A7" s="7"/>
+      <c r="B7" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="24" t="s">
+      <c r="C7" s="10" t="s">
         <v>7</v>
       </c>
       <c r="D7"/>
@@ -5456,11 +5512,11 @@
       <c r="AMJ7"/>
     </row>
     <row r="8" spans="1:1024" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="21"/>
-      <c r="B8" s="10" t="s">
+      <c r="A8" s="7"/>
+      <c r="B8" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="10"/>
+      <c r="C8" s="44"/>
       <c r="D8"/>
       <c r="E8"/>
       <c r="F8"/>
@@ -6484,11 +6540,11 @@
       <c r="AMJ8"/>
     </row>
     <row r="9" spans="1:1024" ht="21" x14ac:dyDescent="0.35">
-      <c r="A9" s="21"/>
-      <c r="B9" s="25" t="s">
+      <c r="A9" s="7"/>
+      <c r="B9" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="26" t="s">
+      <c r="C9" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D9"/>
@@ -7514,13 +7570,13 @@
       <c r="AMJ9"/>
     </row>
     <row r="10" spans="1:1024" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="9"/>
+      <c r="C10" s="46"/>
       <c r="D10"/>
       <c r="E10"/>
       <c r="F10"/>
@@ -8544,11 +8600,11 @@
       <c r="AMJ10"/>
     </row>
     <row r="11" spans="1:1024" ht="21" x14ac:dyDescent="0.35">
-      <c r="A11" s="21"/>
-      <c r="B11" s="25" t="s">
+      <c r="A11" s="7"/>
+      <c r="B11" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="26" t="s">
+      <c r="C11" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D11"/>
@@ -9574,11 +9630,11 @@
       <c r="AMJ11"/>
     </row>
     <row r="12" spans="1:1024" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="21"/>
-      <c r="B12" s="10" t="s">
+      <c r="A12" s="7"/>
+      <c r="B12" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="10"/>
+      <c r="C12" s="44"/>
       <c r="D12"/>
       <c r="E12"/>
       <c r="F12"/>
@@ -10602,11 +10658,11 @@
       <c r="AMJ12"/>
     </row>
     <row r="13" spans="1:1024" ht="21" x14ac:dyDescent="0.35">
-      <c r="A13" s="21"/>
-      <c r="B13" s="26" t="s">
+      <c r="A13" s="7"/>
+      <c r="B13" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="26" t="s">
+      <c r="C13" s="12" t="s">
         <v>18</v>
       </c>
       <c r="D13"/>
@@ -11632,11 +11688,11 @@
       <c r="AMJ13"/>
     </row>
     <row r="14" spans="1:1024" ht="21" x14ac:dyDescent="0.35">
-      <c r="A14" s="21"/>
-      <c r="B14" s="25" t="s">
+      <c r="A14" s="7"/>
+      <c r="B14" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="26" t="s">
+      <c r="C14" s="12" t="s">
         <v>20</v>
       </c>
       <c r="D14"/>
@@ -12662,11 +12718,11 @@
       <c r="AMJ14"/>
     </row>
     <row r="15" spans="1:1024" ht="21" x14ac:dyDescent="0.35">
-      <c r="A15" s="21"/>
-      <c r="B15" s="25" t="s">
+      <c r="A15" s="7"/>
+      <c r="B15" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="26" t="s">
+      <c r="C15" s="12" t="s">
         <v>22</v>
       </c>
       <c r="D15"/>
@@ -13692,11 +13748,11 @@
       <c r="AMJ15"/>
     </row>
     <row r="16" spans="1:1024" ht="21" x14ac:dyDescent="0.35">
-      <c r="A16" s="21"/>
-      <c r="B16" s="25" t="s">
+      <c r="A16" s="7"/>
+      <c r="B16" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="26" t="s">
+      <c r="C16" s="12" t="s">
         <v>24</v>
       </c>
       <c r="D16"/>
@@ -14722,11 +14778,11 @@
       <c r="AMJ16"/>
     </row>
     <row r="17" spans="1:1024" ht="21" x14ac:dyDescent="0.35">
-      <c r="A17" s="21"/>
-      <c r="B17" s="25" t="s">
+      <c r="A17" s="7"/>
+      <c r="B17" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="26" t="s">
+      <c r="C17" s="12" t="s">
         <v>26</v>
       </c>
       <c r="D17"/>
@@ -15752,11 +15808,11 @@
       <c r="AMJ17"/>
     </row>
     <row r="18" spans="1:1024" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="21"/>
-      <c r="B18" s="10" t="s">
+      <c r="A18" s="7"/>
+      <c r="B18" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="10"/>
+      <c r="C18" s="44"/>
       <c r="D18"/>
       <c r="E18"/>
       <c r="F18"/>
@@ -16780,11 +16836,11 @@
       <c r="AMJ18"/>
     </row>
     <row r="19" spans="1:1024" ht="21" x14ac:dyDescent="0.35">
-      <c r="A19" s="21"/>
-      <c r="B19" s="26" t="s">
+      <c r="A19" s="7"/>
+      <c r="B19" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="26" t="s">
+      <c r="C19" s="12" t="s">
         <v>29</v>
       </c>
       <c r="D19"/>
@@ -17810,11 +17866,11 @@
       <c r="AMJ19"/>
     </row>
     <row r="20" spans="1:1024" ht="21" x14ac:dyDescent="0.35">
-      <c r="A20" s="21"/>
-      <c r="B20" s="26" t="s">
+      <c r="A20" s="7"/>
+      <c r="B20" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="26" t="s">
+      <c r="C20" s="12" t="s">
         <v>31</v>
       </c>
       <c r="D20"/>
@@ -18840,11 +18896,11 @@
       <c r="AMJ20"/>
     </row>
     <row r="21" spans="1:1024" ht="21" x14ac:dyDescent="0.35">
-      <c r="A21" s="21"/>
-      <c r="B21" s="26" t="s">
+      <c r="A21" s="7"/>
+      <c r="B21" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="C21" s="26" t="s">
+      <c r="C21" s="12" t="s">
         <v>33</v>
       </c>
       <c r="D21"/>
@@ -19870,11 +19926,11 @@
       <c r="AMJ21"/>
     </row>
     <row r="22" spans="1:1024" ht="21" x14ac:dyDescent="0.35">
-      <c r="A22" s="21"/>
-      <c r="B22" s="26" t="s">
+      <c r="A22" s="7"/>
+      <c r="B22" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="C22" s="26" t="s">
+      <c r="C22" s="12" t="s">
         <v>35</v>
       </c>
       <c r="D22"/>
@@ -20900,11 +20956,11 @@
       <c r="AMJ22"/>
     </row>
     <row r="23" spans="1:1024" ht="21" x14ac:dyDescent="0.35">
-      <c r="A23" s="21"/>
-      <c r="B23" s="26" t="s">
+      <c r="A23" s="7"/>
+      <c r="B23" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="C23" s="26" t="s">
+      <c r="C23" s="12" t="s">
         <v>37</v>
       </c>
       <c r="D23"/>
@@ -21930,11 +21986,11 @@
       <c r="AMJ23"/>
     </row>
     <row r="24" spans="1:1024" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="21"/>
-      <c r="B24" s="10" t="s">
+      <c r="A24" s="7"/>
+      <c r="B24" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="C24" s="10"/>
+      <c r="C24" s="44"/>
       <c r="D24"/>
       <c r="E24"/>
       <c r="F24"/>
@@ -22958,11 +23014,11 @@
       <c r="AMJ24"/>
     </row>
     <row r="25" spans="1:1024" ht="21" x14ac:dyDescent="0.35">
-      <c r="A25" s="21"/>
-      <c r="B25" s="26" t="s">
+      <c r="A25" s="7"/>
+      <c r="B25" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="C25" s="26" t="s">
+      <c r="C25" s="12" t="s">
         <v>40</v>
       </c>
       <c r="D25"/>
@@ -23988,11 +24044,11 @@
       <c r="AMJ25"/>
     </row>
     <row r="26" spans="1:1024" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="21"/>
-      <c r="B26" s="8" t="s">
+      <c r="A26" s="7"/>
+      <c r="B26" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="C26" s="8"/>
+      <c r="C26" s="43"/>
       <c r="D26"/>
       <c r="E26"/>
       <c r="F26"/>
@@ -25016,11 +25072,11 @@
       <c r="AMJ26"/>
     </row>
     <row r="27" spans="1:1024" ht="21" x14ac:dyDescent="0.35">
-      <c r="A27" s="21"/>
-      <c r="B27" s="26" t="s">
+      <c r="A27" s="7"/>
+      <c r="B27" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C27" s="26" t="s">
+      <c r="C27" s="12" t="s">
         <v>43</v>
       </c>
       <c r="D27"/>
@@ -26046,11 +26102,11 @@
       <c r="AMJ27"/>
     </row>
     <row r="28" spans="1:1024" ht="21" x14ac:dyDescent="0.35">
-      <c r="A28" s="21"/>
-      <c r="B28" s="26" t="s">
+      <c r="A28" s="7"/>
+      <c r="B28" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C28" s="26" t="s">
+      <c r="C28" s="12" t="s">
         <v>45</v>
       </c>
       <c r="D28"/>
@@ -27076,11 +27132,11 @@
       <c r="AMJ28"/>
     </row>
     <row r="29" spans="1:1024" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="21"/>
-      <c r="B29" s="10" t="s">
+      <c r="A29" s="7"/>
+      <c r="B29" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="C29" s="10"/>
+      <c r="C29" s="44"/>
       <c r="D29"/>
       <c r="E29"/>
       <c r="F29"/>
@@ -28104,11 +28160,11 @@
       <c r="AMJ29"/>
     </row>
     <row r="30" spans="1:1024" ht="21" x14ac:dyDescent="0.35">
-      <c r="A30" s="21"/>
-      <c r="B30" s="26" t="s">
+      <c r="A30" s="7"/>
+      <c r="B30" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="C30" s="26" t="s">
+      <c r="C30" s="12" t="s">
         <v>48</v>
       </c>
       <c r="D30"/>
@@ -29133,18 +29189,18 @@
       <c r="AMI30"/>
       <c r="AMJ30"/>
     </row>
-    <row r="31" spans="1:1024" s="27" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B31" s="11" t="s">
+    <row r="31" spans="1:1024" s="13" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B31" s="45" t="s">
         <v>49</v>
       </c>
-      <c r="C31" s="11"/>
+      <c r="C31" s="45"/>
     </row>
     <row r="32" spans="1:1024" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A32" s="27"/>
-      <c r="B32" s="9" t="s">
+      <c r="A32" s="13"/>
+      <c r="B32" s="46" t="s">
         <v>50</v>
       </c>
-      <c r="C32" s="9"/>
+      <c r="C32" s="46"/>
       <c r="D32"/>
       <c r="E32"/>
       <c r="F32"/>
@@ -30169,10 +30225,10 @@
     </row>
     <row r="33" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33"/>
-      <c r="B33" s="25" t="s">
+      <c r="B33" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="C33" s="28" t="s">
+      <c r="C33" s="14" t="s">
         <v>52</v>
       </c>
       <c r="D33"/>
@@ -31199,10 +31255,10 @@
     </row>
     <row r="34" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34"/>
-      <c r="B34" s="50" t="s">
+      <c r="B34" s="33" t="s">
         <v>149</v>
       </c>
-      <c r="C34" s="51"/>
+      <c r="C34" s="34"/>
       <c r="D34"/>
       <c r="E34"/>
       <c r="F34"/>
@@ -32227,10 +32283,10 @@
     </row>
     <row r="35" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35"/>
-      <c r="B35" s="50" t="s">
+      <c r="B35" s="33" t="s">
         <v>150</v>
       </c>
-      <c r="C35" s="51"/>
+      <c r="C35" s="34"/>
       <c r="D35"/>
       <c r="E35"/>
       <c r="F35"/>
@@ -33254,11 +33310,11 @@
       <c r="AMJ35"/>
     </row>
     <row r="36" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="21"/>
-      <c r="B36" s="7" t="s">
+      <c r="A36" s="7"/>
+      <c r="B36" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="C36" s="7"/>
+      <c r="C36" s="35"/>
       <c r="D36"/>
       <c r="E36"/>
       <c r="F36"/>
@@ -34282,11 +34338,11 @@
       <c r="AMJ36"/>
     </row>
     <row r="37" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="21"/>
-      <c r="B37" s="26" t="s">
+      <c r="A37" s="7"/>
+      <c r="B37" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="C37" s="26" t="s">
+      <c r="C37" s="12" t="s">
         <v>67</v>
       </c>
       <c r="D37"/>
@@ -35312,11 +35368,11 @@
       <c r="AMJ37"/>
     </row>
     <row r="38" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="21"/>
-      <c r="B38" s="26" t="s">
+      <c r="A38" s="7"/>
+      <c r="B38" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="C38" s="26" t="s">
+      <c r="C38" s="12" t="s">
         <v>69</v>
       </c>
       <c r="D38"/>
@@ -36342,11 +36398,11 @@
       <c r="AMJ38"/>
     </row>
     <row r="39" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="21"/>
-      <c r="B39" s="26" t="s">
+      <c r="A39" s="7"/>
+      <c r="B39" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="C39" s="26" t="s">
+      <c r="C39" s="12" t="s">
         <v>71</v>
       </c>
       <c r="D39"/>
@@ -37373,10 +37429,10 @@
     </row>
     <row r="40" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40"/>
-      <c r="B40" s="50" t="s">
+      <c r="B40" s="33" t="s">
         <v>151</v>
       </c>
-      <c r="C40" s="51"/>
+      <c r="C40" s="34"/>
       <c r="D40"/>
       <c r="E40"/>
       <c r="F40"/>
@@ -38401,10 +38457,10 @@
     </row>
     <row r="41" spans="1:1024" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41"/>
-      <c r="B41" s="9" t="s">
+      <c r="B41" s="46" t="s">
         <v>53</v>
       </c>
-      <c r="C41" s="9"/>
+      <c r="C41" s="46"/>
       <c r="D41"/>
       <c r="E41"/>
       <c r="F41"/>
@@ -39429,10 +39485,10 @@
     </row>
     <row r="42" spans="1:1024" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42"/>
-      <c r="B42" s="7" t="s">
+      <c r="B42" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="C42" s="7"/>
+      <c r="C42" s="35"/>
       <c r="D42"/>
       <c r="E42"/>
       <c r="F42"/>
@@ -40457,10 +40513,10 @@
     </row>
     <row r="43" spans="1:1024" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43"/>
-      <c r="B43" s="25" t="s">
+      <c r="B43" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="C43" s="28" t="s">
+      <c r="C43" s="14" t="s">
         <v>54</v>
       </c>
       <c r="D43"/>
@@ -41487,10 +41543,10 @@
     </row>
     <row r="44" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44"/>
-      <c r="B44" s="25" t="s">
+      <c r="B44" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="C44" s="28" t="s">
+      <c r="C44" s="14" t="s">
         <v>55</v>
       </c>
       <c r="D44"/>
@@ -42517,10 +42573,10 @@
     </row>
     <row r="45" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45"/>
-      <c r="B45" s="25" t="s">
+      <c r="B45" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="C45" s="28" t="s">
+      <c r="C45" s="14" t="s">
         <v>57</v>
       </c>
       <c r="D45"/>
@@ -43547,10 +43603,10 @@
     </row>
     <row r="46" spans="1:1024" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46"/>
-      <c r="B46" s="7" t="s">
+      <c r="B46" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="C46" s="7"/>
+      <c r="C46" s="35"/>
       <c r="D46"/>
       <c r="E46"/>
       <c r="F46"/>
@@ -44575,10 +44631,10 @@
     </row>
     <row r="47" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47"/>
-      <c r="B47" s="25" t="s">
+      <c r="B47" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="C47" s="28" t="s">
+      <c r="C47" s="14" t="s">
         <v>59</v>
       </c>
       <c r="D47"/>
@@ -45605,10 +45661,10 @@
     </row>
     <row r="48" spans="1:1024" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48"/>
-      <c r="B48" s="7" t="s">
+      <c r="B48" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="C48" s="7"/>
+      <c r="C48" s="35"/>
       <c r="D48"/>
       <c r="E48"/>
       <c r="F48"/>
@@ -46632,11 +46688,11 @@
       <c r="AMJ48"/>
     </row>
     <row r="49" spans="1:1024" ht="21" x14ac:dyDescent="0.35">
-      <c r="A49" s="21"/>
-      <c r="B49" s="25" t="s">
+      <c r="A49" s="7"/>
+      <c r="B49" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="C49" s="26" t="s">
+      <c r="C49" s="12" t="s">
         <v>61</v>
       </c>
       <c r="D49"/>
@@ -47662,11 +47718,11 @@
       <c r="AMJ49"/>
     </row>
     <row r="50" spans="1:1024" ht="21" x14ac:dyDescent="0.35">
-      <c r="A50" s="21"/>
-      <c r="B50" s="25" t="s">
+      <c r="A50" s="7"/>
+      <c r="B50" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="C50" s="26" t="s">
+      <c r="C50" s="12" t="s">
         <v>152</v>
       </c>
       <c r="D50"/>
@@ -48692,11 +48748,11 @@
       <c r="AMJ50"/>
     </row>
     <row r="51" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="21"/>
-      <c r="B51" s="7" t="s">
+      <c r="A51" s="7"/>
+      <c r="B51" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="C51" s="7"/>
+      <c r="C51" s="35"/>
       <c r="D51"/>
       <c r="E51"/>
       <c r="F51"/>
@@ -49720,11 +49776,11 @@
       <c r="AMJ51"/>
     </row>
     <row r="52" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="21"/>
-      <c r="B52" s="26" t="s">
+      <c r="A52" s="7"/>
+      <c r="B52" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="C52" s="26" t="s">
+      <c r="C52" s="12" t="s">
         <v>63</v>
       </c>
       <c r="D52"/>
@@ -50750,11 +50806,11 @@
       <c r="AMJ52"/>
     </row>
     <row r="53" spans="1:1024" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="21"/>
-      <c r="B53" s="26" t="s">
+      <c r="A53" s="7"/>
+      <c r="B53" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="C53" s="26" t="s">
+      <c r="C53" s="12" t="s">
         <v>65</v>
       </c>
       <c r="D53"/>
@@ -51779,18 +51835,18 @@
       <c r="AMI53"/>
       <c r="AMJ53"/>
     </row>
-    <row r="54" spans="1:1024" s="27" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B54" s="7" t="s">
+    <row r="54" spans="1:1024" s="13" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B54" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="C54" s="7"/>
+      <c r="C54" s="35"/>
     </row>
     <row r="55" spans="1:1024" ht="27" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A55" s="27"/>
-      <c r="B55" s="26" t="s">
+      <c r="A55" s="13"/>
+      <c r="B55" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="C55" s="26" t="s">
+      <c r="C55" s="12" t="s">
         <v>73</v>
       </c>
       <c r="D55"/>
@@ -51800,11 +51856,11 @@
       <c r="H55"/>
     </row>
     <row r="56" spans="1:1024" ht="61.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A56" s="27"/>
-      <c r="B56" s="6" t="s">
+      <c r="A56" s="13"/>
+      <c r="B56" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="C56" s="6"/>
+      <c r="C56" s="40"/>
       <c r="D56"/>
       <c r="E56"/>
       <c r="F56"/>
@@ -51813,10 +51869,10 @@
     </row>
     <row r="57" spans="1:1024" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57"/>
-      <c r="B57" s="12" t="s">
+      <c r="B57" s="31" t="s">
         <v>75</v>
       </c>
-      <c r="C57" s="12"/>
+      <c r="C57" s="31"/>
       <c r="D57"/>
       <c r="E57"/>
       <c r="F57"/>
@@ -51825,10 +51881,10 @@
     </row>
     <row r="58" spans="1:1024" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58"/>
-      <c r="B58" s="29" t="s">
+      <c r="B58" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="C58" s="29" t="s">
+      <c r="C58" s="15" t="s">
         <v>77</v>
       </c>
       <c r="D58"/>
@@ -51839,10 +51895,10 @@
     </row>
     <row r="59" spans="1:1024" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59"/>
-      <c r="B59" s="5" t="s">
+      <c r="B59" s="41" t="s">
         <v>75</v>
       </c>
-      <c r="C59" s="5"/>
+      <c r="C59" s="41"/>
       <c r="D59"/>
       <c r="E59"/>
       <c r="F59"/>
@@ -51851,10 +51907,10 @@
     </row>
     <row r="60" spans="1:1024" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60"/>
-      <c r="B60" s="30" t="s">
+      <c r="B60" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="C60" s="30" t="s">
+      <c r="C60" s="16" t="s">
         <v>79</v>
       </c>
       <c r="D60"/>
@@ -51865,8 +51921,8 @@
     </row>
     <row r="61" spans="1:1024" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61"/>
-      <c r="B61" s="31"/>
-      <c r="C61" s="31"/>
+      <c r="B61" s="17"/>
+      <c r="C61" s="17"/>
       <c r="D61"/>
       <c r="E61"/>
       <c r="F61"/>
@@ -51875,10 +51931,10 @@
     </row>
     <row r="62" spans="1:1024" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62"/>
-      <c r="B62" s="4" t="s">
+      <c r="B62" s="42" t="s">
         <v>80</v>
       </c>
-      <c r="C62" s="4"/>
+      <c r="C62" s="42"/>
       <c r="D62"/>
       <c r="E62"/>
       <c r="F62"/>
@@ -51887,10 +51943,10 @@
     </row>
     <row r="63" spans="1:1024" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63"/>
-      <c r="B63" s="3" t="s">
+      <c r="B63" s="36" t="s">
         <v>81</v>
       </c>
-      <c r="C63" s="3"/>
+      <c r="C63" s="36"/>
       <c r="D63"/>
       <c r="E63"/>
       <c r="F63"/>
@@ -51899,8 +51955,8 @@
     </row>
     <row r="64" spans="1:1024" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64"/>
-      <c r="B64" s="3"/>
-      <c r="C64" s="3"/>
+      <c r="B64" s="36"/>
+      <c r="C64" s="36"/>
       <c r="D64"/>
       <c r="E64"/>
       <c r="F64"/>
@@ -51909,8 +51965,8 @@
     </row>
     <row r="65" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65"/>
-      <c r="B65" s="31"/>
-      <c r="C65" s="31"/>
+      <c r="B65" s="17"/>
+      <c r="C65" s="17"/>
       <c r="D65"/>
       <c r="E65"/>
       <c r="F65"/>
@@ -51919,10 +51975,10 @@
     </row>
     <row r="66" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66"/>
-      <c r="B66" s="12" t="s">
+      <c r="B66" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="C66" s="12"/>
+      <c r="C66" s="31"/>
       <c r="D66"/>
       <c r="E66"/>
       <c r="F66"/>
@@ -51931,10 +51987,10 @@
     </row>
     <row r="67" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67"/>
-      <c r="B67" s="2" t="s">
+      <c r="B67" s="37" t="s">
         <v>82</v>
       </c>
-      <c r="C67" s="2"/>
+      <c r="C67" s="37"/>
       <c r="D67"/>
       <c r="E67"/>
       <c r="F67"/>
@@ -51943,8 +51999,8 @@
     </row>
     <row r="68" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68"/>
-      <c r="B68" s="2"/>
-      <c r="C68" s="2"/>
+      <c r="B68" s="37"/>
+      <c r="C68" s="37"/>
       <c r="D68"/>
       <c r="E68"/>
       <c r="F68"/>
@@ -51953,8 +52009,8 @@
     </row>
     <row r="69" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69"/>
-      <c r="B69" s="32"/>
-      <c r="C69" s="33"/>
+      <c r="B69" s="18"/>
+      <c r="C69" s="19"/>
       <c r="D69"/>
       <c r="E69"/>
       <c r="F69"/>
@@ -51962,11 +52018,11 @@
       <c r="H69"/>
     </row>
     <row r="70" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A70" s="34"/>
-      <c r="B70" s="1" t="s">
+      <c r="A70" s="20"/>
+      <c r="B70" s="38" t="s">
         <v>83</v>
       </c>
-      <c r="C70" s="1"/>
+      <c r="C70" s="38"/>
       <c r="D70"/>
       <c r="E70"/>
       <c r="F70"/>
@@ -51975,71 +52031,69 @@
     </row>
     <row r="71" spans="1:8" ht="167.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71"/>
-      <c r="B71" s="48" t="s">
+      <c r="B71" s="39" t="s">
         <v>84</v>
       </c>
-      <c r="C71" s="48"/>
+      <c r="C71" s="39"/>
       <c r="D71"/>
       <c r="E71"/>
       <c r="F71"/>
       <c r="G71"/>
       <c r="H71"/>
     </row>
-    <row r="72" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:8" ht="85.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72"/>
-      <c r="B72" s="35"/>
-      <c r="C72" s="35"/>
+      <c r="B72" s="39" t="s">
+        <v>153</v>
+      </c>
+      <c r="C72" s="39"/>
       <c r="D72"/>
       <c r="E72"/>
       <c r="F72"/>
       <c r="G72"/>
       <c r="H72"/>
     </row>
-    <row r="73" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73"/>
-      <c r="B73" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="C73" s="12"/>
+      <c r="B73" s="49"/>
+      <c r="C73" s="49"/>
       <c r="D73"/>
       <c r="E73"/>
       <c r="F73"/>
       <c r="G73"/>
       <c r="H73"/>
     </row>
-    <row r="74" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A74"/>
-      <c r="B74" s="49" t="s">
-        <v>86</v>
+      <c r="B74" s="31" t="s">
+        <v>85</v>
       </c>
-      <c r="C74" s="49"/>
+      <c r="C74" s="31"/>
       <c r="D74"/>
       <c r="E74"/>
       <c r="F74"/>
       <c r="G74"/>
       <c r="H74"/>
     </row>
-    <row r="75" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A75"/>
-      <c r="B75" s="36" t="s">
-        <v>87</v>
+      <c r="B75" s="32" t="s">
+        <v>86</v>
       </c>
-      <c r="C75" s="36" t="s">
-        <v>88</v>
-      </c>
+      <c r="C75" s="32"/>
       <c r="D75"/>
       <c r="E75"/>
       <c r="F75"/>
       <c r="G75"/>
       <c r="H75"/>
     </row>
-    <row r="76" spans="1:8" ht="74.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76"/>
-      <c r="B76" s="37" t="s">
-        <v>89</v>
+      <c r="B76" s="21" t="s">
+        <v>87</v>
       </c>
-      <c r="C76" s="37" t="s">
-        <v>90</v>
+      <c r="C76" s="21" t="s">
+        <v>88</v>
       </c>
       <c r="D76"/>
       <c r="E76"/>
@@ -52047,13 +52101,13 @@
       <c r="G76"/>
       <c r="H76"/>
     </row>
-    <row r="77" spans="1:8" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:8" ht="74.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77"/>
-      <c r="B77" s="37" t="s">
-        <v>91</v>
+      <c r="B77" s="22" t="s">
+        <v>89</v>
       </c>
-      <c r="C77" s="37" t="s">
-        <v>92</v>
+      <c r="C77" s="22" t="s">
+        <v>90</v>
       </c>
       <c r="D77"/>
       <c r="E77"/>
@@ -52061,24 +52115,24 @@
       <c r="G77"/>
       <c r="H77"/>
     </row>
-    <row r="78" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:8" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78"/>
-      <c r="B78" s="33"/>
-      <c r="C78" s="33"/>
+      <c r="B78" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="C78" s="22" t="s">
+        <v>92</v>
+      </c>
       <c r="D78"/>
       <c r="E78"/>
       <c r="F78"/>
       <c r="G78"/>
       <c r="H78"/>
     </row>
-    <row r="79" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:8" ht="21" x14ac:dyDescent="0.35">
       <c r="A79"/>
-      <c r="B79" s="38" t="s">
-        <v>93</v>
-      </c>
-      <c r="C79" s="38" t="s">
-        <v>94</v>
-      </c>
+      <c r="B79" s="19"/>
+      <c r="C79" s="19"/>
       <c r="D79"/>
       <c r="E79"/>
       <c r="F79"/>
@@ -52086,55 +52140,72 @@
       <c r="H79"/>
     </row>
     <row r="80" spans="1:8" ht="21" x14ac:dyDescent="0.2">
-      <c r="A80" s="39"/>
-      <c r="B80" s="40" t="s">
-        <v>95</v>
+      <c r="A80"/>
+      <c r="B80" s="23" t="s">
+        <v>93</v>
       </c>
-      <c r="C80" s="41" t="s">
-        <v>96</v>
+      <c r="C80" s="23" t="s">
+        <v>94</v>
       </c>
-      <c r="D80"/>
+      <c r="D80" s="54" t="s">
+        <v>154</v>
+      </c>
       <c r="E80"/>
       <c r="F80"/>
       <c r="G80"/>
       <c r="H80"/>
     </row>
-    <row r="81" spans="1:8" ht="21" x14ac:dyDescent="0.2">
-      <c r="A81"/>
-      <c r="B81" s="40" t="s">
-        <v>97</v>
+    <row r="81" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A81" s="24"/>
+      <c r="B81" s="50" t="s">
+        <v>95</v>
       </c>
-      <c r="C81" s="41" t="s">
-        <v>98</v>
+      <c r="C81" s="51" t="s">
+        <v>96</v>
       </c>
-      <c r="D81"/>
+      <c r="D81" s="52" t="s">
+        <v>158</v>
+      </c>
       <c r="E81"/>
       <c r="F81"/>
       <c r="G81"/>
       <c r="H81"/>
     </row>
-    <row r="82" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A82" s="34"/>
-      <c r="B82" s="39"/>
-      <c r="C82" s="39"/>
-      <c r="D82"/>
+    <row r="82" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A82"/>
+      <c r="B82" s="50" t="s">
+        <v>97</v>
+      </c>
+      <c r="C82" s="51" t="s">
+        <v>98</v>
+      </c>
+      <c r="D82" s="52" t="s">
+        <v>157</v>
+      </c>
       <c r="E82"/>
       <c r="F82"/>
       <c r="G82"/>
       <c r="H82"/>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B83" s="39"/>
-      <c r="C83" s="39"/>
-      <c r="D83"/>
+    <row r="83" spans="1:8" ht="27" x14ac:dyDescent="0.3">
+      <c r="A83" s="20"/>
+      <c r="B83" s="53" t="s">
+        <v>155</v>
+      </c>
+      <c r="C83" s="53" t="s">
+        <v>156</v>
+      </c>
+      <c r="D83" s="52" t="s">
+        <v>159</v>
+      </c>
       <c r="E83"/>
       <c r="F83"/>
       <c r="G83"/>
       <c r="H83"/>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B84" s="39"/>
-      <c r="C84" s="39"/>
+      <c r="B84" s="24"/>
+      <c r="C84" s="24"/>
       <c r="D84"/>
       <c r="E84"/>
       <c r="F84"/>
@@ -52142,8 +52213,8 @@
       <c r="H84"/>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B85" s="39"/>
-      <c r="C85" s="39"/>
+      <c r="B85" s="24"/>
+      <c r="C85" s="24"/>
       <c r="D85"/>
       <c r="E85"/>
       <c r="F85"/>
@@ -52151,369 +52222,397 @@
       <c r="H85"/>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B86" s="39"/>
-      <c r="C86" s="39"/>
-      <c r="D86" s="39"/>
-      <c r="E86" s="39"/>
-      <c r="F86" s="39"/>
-      <c r="G86" s="39"/>
-      <c r="H86" s="39"/>
+      <c r="B86" s="24"/>
+      <c r="C86" s="24"/>
+      <c r="D86"/>
+      <c r="E86"/>
+      <c r="F86"/>
+      <c r="G86"/>
+      <c r="H86"/>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B87" s="39"/>
-      <c r="C87" s="39"/>
-      <c r="D87" s="39"/>
-      <c r="E87" s="39"/>
-      <c r="F87" s="39"/>
-      <c r="G87" s="39"/>
-      <c r="H87" s="39"/>
+      <c r="B87" s="24"/>
+      <c r="C87" s="24"/>
+      <c r="D87" s="24"/>
+      <c r="E87" s="24"/>
+      <c r="F87" s="24"/>
+      <c r="G87" s="24"/>
+      <c r="H87" s="24"/>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B88" s="39"/>
-      <c r="C88" s="39"/>
-      <c r="D88" s="39"/>
-      <c r="E88" s="39"/>
-      <c r="F88" s="39"/>
-      <c r="G88" s="39"/>
-      <c r="H88" s="39"/>
+      <c r="B88" s="24"/>
+      <c r="C88" s="24"/>
+      <c r="D88" s="24"/>
+      <c r="E88" s="24"/>
+      <c r="F88" s="24"/>
+      <c r="G88" s="24"/>
+      <c r="H88" s="24"/>
     </row>
-    <row r="89" spans="1:8" ht="409.6" x14ac:dyDescent="0.25">
-      <c r="B89" s="39"/>
-      <c r="C89" s="39"/>
-      <c r="D89" s="39"/>
-      <c r="E89" s="39"/>
-      <c r="F89" s="39"/>
-      <c r="G89" s="39"/>
-      <c r="H89" s="39"/>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B89" s="24"/>
+      <c r="C89" s="24"/>
+      <c r="D89" s="24"/>
+      <c r="E89" s="24"/>
+      <c r="F89" s="24"/>
+      <c r="G89" s="24"/>
+      <c r="H89" s="24"/>
     </row>
-    <row r="90" spans="1:8" ht="409.6" x14ac:dyDescent="0.25">
-      <c r="B90" s="39"/>
-      <c r="C90" s="39"/>
-      <c r="D90" s="39"/>
-      <c r="E90" s="39"/>
-      <c r="F90" s="39"/>
-      <c r="G90" s="39"/>
-      <c r="H90" s="39"/>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B90" s="24"/>
+      <c r="C90" s="24"/>
+      <c r="D90" s="24"/>
+      <c r="E90" s="24"/>
+      <c r="F90" s="24"/>
+      <c r="G90" s="24"/>
+      <c r="H90" s="24"/>
     </row>
-    <row r="91" spans="1:8" ht="409.6" x14ac:dyDescent="0.25">
-      <c r="B91" s="39"/>
-      <c r="C91" s="39"/>
-      <c r="D91" s="39"/>
-      <c r="E91" s="39"/>
-      <c r="F91" s="39"/>
-      <c r="G91" s="39"/>
-      <c r="H91" s="39"/>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B91" s="24"/>
+      <c r="C91" s="24"/>
+      <c r="D91" s="24"/>
+      <c r="E91" s="24"/>
+      <c r="F91" s="24"/>
+      <c r="G91" s="24"/>
+      <c r="H91" s="24"/>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B92" s="39"/>
-      <c r="C92" s="39"/>
-      <c r="D92" s="39"/>
-      <c r="E92" s="39"/>
-      <c r="F92" s="39"/>
-      <c r="G92" s="39"/>
-      <c r="H92" s="39"/>
+      <c r="B92" s="24"/>
+      <c r="C92" s="24"/>
+      <c r="D92" s="24"/>
+      <c r="E92" s="24"/>
+      <c r="F92" s="24"/>
+      <c r="G92" s="24"/>
+      <c r="H92" s="24"/>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B93" s="39"/>
-      <c r="C93" s="39"/>
-      <c r="D93" s="39"/>
-      <c r="E93" s="39"/>
-      <c r="F93" s="39"/>
-      <c r="G93" s="39"/>
-      <c r="H93" s="39"/>
+      <c r="B93" s="24"/>
+      <c r="C93" s="24"/>
+      <c r="D93" s="24"/>
+      <c r="E93" s="24"/>
+      <c r="F93" s="24"/>
+      <c r="G93" s="24"/>
+      <c r="H93" s="24"/>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B94" s="39"/>
-      <c r="C94" s="39"/>
-      <c r="D94" s="39"/>
-      <c r="E94" s="39"/>
-      <c r="F94" s="39"/>
-      <c r="G94" s="39"/>
-      <c r="H94" s="39"/>
+      <c r="B94" s="24"/>
+      <c r="C94" s="24"/>
+      <c r="D94" s="24"/>
+      <c r="E94" s="24"/>
+      <c r="F94" s="24"/>
+      <c r="G94" s="24"/>
+      <c r="H94" s="24"/>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B95" s="39"/>
-      <c r="C95" s="39"/>
-      <c r="D95" s="39"/>
-      <c r="E95" s="39"/>
-      <c r="F95" s="39"/>
-      <c r="G95" s="39"/>
-      <c r="H95" s="39"/>
+      <c r="B95" s="24"/>
+      <c r="C95" s="24"/>
+      <c r="D95" s="24"/>
+      <c r="E95" s="24"/>
+      <c r="F95" s="24"/>
+      <c r="G95" s="24"/>
+      <c r="H95" s="24"/>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B96" s="39"/>
-      <c r="C96" s="39"/>
-      <c r="D96" s="39"/>
-      <c r="E96" s="39"/>
-      <c r="F96" s="39"/>
-      <c r="G96" s="39"/>
-      <c r="H96" s="39"/>
+      <c r="B96" s="24"/>
+      <c r="C96" s="24"/>
+      <c r="D96" s="24"/>
+      <c r="E96" s="24"/>
+      <c r="F96" s="24"/>
+      <c r="G96" s="24"/>
+      <c r="H96" s="24"/>
     </row>
     <row r="97" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B97" s="39"/>
-      <c r="C97" s="39"/>
-      <c r="D97" s="39"/>
-      <c r="E97" s="39"/>
-      <c r="F97" s="39"/>
-      <c r="G97" s="39"/>
-      <c r="H97" s="39"/>
+      <c r="B97" s="24"/>
+      <c r="C97" s="24"/>
+      <c r="D97" s="24"/>
+      <c r="E97" s="24"/>
+      <c r="F97" s="24"/>
+      <c r="G97" s="24"/>
+      <c r="H97" s="24"/>
     </row>
     <row r="98" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B98" s="39"/>
-      <c r="C98" s="39"/>
-      <c r="D98" s="39"/>
-      <c r="E98" s="39"/>
-      <c r="F98" s="39"/>
-      <c r="G98" s="39"/>
-      <c r="H98" s="39"/>
+      <c r="B98" s="24"/>
+      <c r="C98" s="24"/>
+      <c r="D98" s="24"/>
+      <c r="E98" s="24"/>
+      <c r="F98" s="24"/>
+      <c r="G98" s="24"/>
+      <c r="H98" s="24"/>
     </row>
     <row r="99" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B99" s="39"/>
-      <c r="C99" s="39"/>
-      <c r="D99" s="39"/>
-      <c r="E99" s="39"/>
-      <c r="F99" s="39"/>
-      <c r="G99" s="39"/>
-      <c r="H99" s="39"/>
+      <c r="B99" s="24"/>
+      <c r="C99" s="24"/>
+      <c r="D99" s="24"/>
+      <c r="E99" s="24"/>
+      <c r="F99" s="24"/>
+      <c r="G99" s="24"/>
+      <c r="H99" s="24"/>
     </row>
     <row r="100" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B100" s="39"/>
-      <c r="C100" s="39"/>
-      <c r="D100" s="39"/>
-      <c r="E100" s="39"/>
-      <c r="F100" s="39"/>
-      <c r="G100" s="39"/>
-      <c r="H100" s="39"/>
+      <c r="B100" s="24"/>
+      <c r="C100" s="24"/>
+      <c r="D100" s="24"/>
+      <c r="E100" s="24"/>
+      <c r="F100" s="24"/>
+      <c r="G100" s="24"/>
+      <c r="H100" s="24"/>
     </row>
     <row r="101" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B101" s="39"/>
-      <c r="C101" s="39"/>
-      <c r="D101" s="39"/>
-      <c r="E101" s="39"/>
-      <c r="F101" s="39"/>
-      <c r="G101" s="39"/>
-      <c r="H101" s="39"/>
+      <c r="B101" s="24"/>
+      <c r="C101" s="24"/>
+      <c r="D101" s="24"/>
+      <c r="E101" s="24"/>
+      <c r="F101" s="24"/>
+      <c r="G101" s="24"/>
+      <c r="H101" s="24"/>
     </row>
     <row r="102" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B102" s="39"/>
-      <c r="C102" s="39"/>
-      <c r="D102" s="39"/>
-      <c r="E102" s="39"/>
-      <c r="F102" s="39"/>
-      <c r="G102" s="39"/>
-      <c r="H102" s="39"/>
+      <c r="B102" s="24"/>
+      <c r="C102" s="24"/>
+      <c r="D102" s="24"/>
+      <c r="E102" s="24"/>
+      <c r="F102" s="24"/>
+      <c r="G102" s="24"/>
+      <c r="H102" s="24"/>
     </row>
     <row r="103" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B103" s="39"/>
-      <c r="C103" s="39"/>
-      <c r="D103" s="39"/>
-      <c r="E103" s="39"/>
-      <c r="F103" s="39"/>
-      <c r="G103" s="39"/>
-      <c r="H103" s="39"/>
+      <c r="B103" s="24"/>
+      <c r="C103" s="24"/>
+      <c r="D103" s="24"/>
+      <c r="E103" s="24"/>
+      <c r="F103" s="24"/>
+      <c r="G103" s="24"/>
+      <c r="H103" s="24"/>
     </row>
     <row r="104" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B104" s="39"/>
-      <c r="C104" s="39"/>
-      <c r="D104" s="39"/>
-      <c r="E104" s="39"/>
-      <c r="F104" s="39"/>
-      <c r="G104" s="39"/>
-      <c r="H104" s="39"/>
+      <c r="B104" s="24"/>
+      <c r="C104" s="24"/>
+      <c r="D104" s="24"/>
+      <c r="E104" s="24"/>
+      <c r="F104" s="24"/>
+      <c r="G104" s="24"/>
+      <c r="H104" s="24"/>
     </row>
     <row r="105" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B105" s="39"/>
-      <c r="C105" s="39"/>
-      <c r="D105" s="39"/>
-      <c r="E105" s="39"/>
-      <c r="F105" s="39"/>
-      <c r="G105" s="39"/>
-      <c r="H105" s="39"/>
+      <c r="B105" s="24"/>
+      <c r="C105" s="24"/>
+      <c r="D105" s="24"/>
+      <c r="E105" s="24"/>
+      <c r="F105" s="24"/>
+      <c r="G105" s="24"/>
+      <c r="H105" s="24"/>
     </row>
     <row r="106" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B106" s="39"/>
-      <c r="C106" s="39"/>
-      <c r="D106" s="39"/>
-      <c r="E106" s="39"/>
-      <c r="F106" s="39"/>
-      <c r="G106" s="39"/>
-      <c r="H106" s="39"/>
+      <c r="B106" s="24"/>
+      <c r="C106" s="24"/>
+      <c r="D106" s="24"/>
+      <c r="E106" s="24"/>
+      <c r="F106" s="24"/>
+      <c r="G106" s="24"/>
+      <c r="H106" s="24"/>
     </row>
     <row r="107" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B107" s="39"/>
-      <c r="C107" s="39"/>
-      <c r="D107" s="39"/>
-      <c r="E107" s="39"/>
-      <c r="F107" s="39"/>
-      <c r="G107" s="39"/>
-      <c r="H107" s="39"/>
+      <c r="B107" s="24"/>
+      <c r="C107" s="24"/>
+      <c r="D107" s="24"/>
+      <c r="E107" s="24"/>
+      <c r="F107" s="24"/>
+      <c r="G107" s="24"/>
+      <c r="H107" s="24"/>
     </row>
     <row r="108" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B108" s="39"/>
-      <c r="C108" s="39"/>
-      <c r="D108" s="39"/>
-      <c r="E108" s="39"/>
-      <c r="F108" s="39"/>
-      <c r="G108" s="39"/>
-      <c r="H108" s="39"/>
+      <c r="B108" s="24"/>
+      <c r="C108" s="24"/>
+      <c r="D108" s="24"/>
+      <c r="E108" s="24"/>
+      <c r="F108" s="24"/>
+      <c r="G108" s="24"/>
+      <c r="H108" s="24"/>
     </row>
     <row r="109" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B109" s="39"/>
-      <c r="C109" s="39"/>
-      <c r="D109" s="39"/>
-      <c r="E109" s="39"/>
-      <c r="F109" s="39"/>
-      <c r="G109" s="39"/>
-      <c r="H109" s="39"/>
+      <c r="B109" s="24"/>
+      <c r="C109" s="24"/>
+      <c r="D109" s="24"/>
+      <c r="E109" s="24"/>
+      <c r="F109" s="24"/>
+      <c r="G109" s="24"/>
+      <c r="H109" s="24"/>
     </row>
     <row r="110" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B110" s="39"/>
-      <c r="C110" s="39"/>
-      <c r="D110" s="39"/>
-      <c r="E110" s="39"/>
-      <c r="F110" s="39"/>
-      <c r="G110" s="39"/>
-      <c r="H110" s="39"/>
+      <c r="B110" s="24"/>
+      <c r="C110" s="24"/>
+      <c r="D110" s="24"/>
+      <c r="E110" s="24"/>
+      <c r="F110" s="24"/>
+      <c r="G110" s="24"/>
+      <c r="H110" s="24"/>
     </row>
     <row r="111" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B111" s="39"/>
-      <c r="C111" s="39"/>
-      <c r="D111" s="39"/>
-      <c r="E111" s="39"/>
-      <c r="F111" s="39"/>
-      <c r="G111" s="39"/>
-      <c r="H111" s="39"/>
+      <c r="B111" s="24"/>
+      <c r="C111" s="24"/>
+      <c r="D111" s="24"/>
+      <c r="E111" s="24"/>
+      <c r="F111" s="24"/>
+      <c r="G111" s="24"/>
+      <c r="H111" s="24"/>
     </row>
     <row r="112" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B112" s="39"/>
-      <c r="C112" s="39"/>
-      <c r="D112" s="39"/>
-      <c r="E112" s="39"/>
-      <c r="F112" s="39"/>
-      <c r="G112" s="39"/>
-      <c r="H112" s="39"/>
+      <c r="B112" s="24"/>
+      <c r="C112" s="24"/>
+      <c r="D112" s="24"/>
+      <c r="E112" s="24"/>
+      <c r="F112" s="24"/>
+      <c r="G112" s="24"/>
+      <c r="H112" s="24"/>
     </row>
     <row r="113" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B113" s="39"/>
-      <c r="C113" s="39"/>
-      <c r="D113" s="39"/>
-      <c r="E113" s="39"/>
-      <c r="F113" s="39"/>
-      <c r="G113" s="39"/>
-      <c r="H113" s="39"/>
+      <c r="B113" s="24"/>
+      <c r="C113" s="24"/>
+      <c r="D113" s="24"/>
+      <c r="E113" s="24"/>
+      <c r="F113" s="24"/>
+      <c r="G113" s="24"/>
+      <c r="H113" s="24"/>
     </row>
     <row r="114" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B114" s="39"/>
-      <c r="C114" s="39"/>
-      <c r="D114" s="39"/>
-      <c r="E114" s="39"/>
-      <c r="F114" s="39"/>
-      <c r="G114" s="39"/>
-      <c r="H114" s="39"/>
+      <c r="B114" s="24"/>
+      <c r="C114" s="24"/>
+      <c r="D114" s="24"/>
+      <c r="E114" s="24"/>
+      <c r="F114" s="24"/>
+      <c r="G114" s="24"/>
+      <c r="H114" s="24"/>
     </row>
     <row r="115" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B115" s="39"/>
-      <c r="C115" s="39"/>
-      <c r="D115" s="39"/>
-      <c r="E115" s="39"/>
-      <c r="F115" s="39"/>
-      <c r="G115" s="39"/>
-      <c r="H115" s="39"/>
+      <c r="B115" s="24"/>
+      <c r="C115" s="24"/>
+      <c r="D115" s="24"/>
+      <c r="E115" s="24"/>
+      <c r="F115" s="24"/>
+      <c r="G115" s="24"/>
+      <c r="H115" s="24"/>
     </row>
     <row r="116" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B116" s="39"/>
-      <c r="C116" s="39"/>
-      <c r="D116" s="39"/>
-      <c r="E116" s="39"/>
-      <c r="F116" s="39"/>
-      <c r="G116" s="39"/>
-      <c r="H116" s="39"/>
+      <c r="B116" s="24"/>
+      <c r="C116" s="24"/>
+      <c r="D116" s="24"/>
+      <c r="E116" s="24"/>
+      <c r="F116" s="24"/>
+      <c r="G116" s="24"/>
+      <c r="H116" s="24"/>
     </row>
     <row r="117" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B117" s="39"/>
-      <c r="C117" s="39"/>
-      <c r="D117" s="39"/>
-      <c r="E117" s="39"/>
-      <c r="F117" s="39"/>
-      <c r="G117" s="39"/>
-      <c r="H117" s="39"/>
+      <c r="B117" s="24"/>
+      <c r="C117" s="24"/>
+      <c r="D117" s="24"/>
+      <c r="E117" s="24"/>
+      <c r="F117" s="24"/>
+      <c r="G117" s="24"/>
+      <c r="H117" s="24"/>
     </row>
     <row r="118" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B118" s="39"/>
-      <c r="C118" s="39"/>
-      <c r="D118" s="39"/>
-      <c r="E118" s="39"/>
-      <c r="F118" s="39"/>
-      <c r="G118" s="39"/>
-      <c r="H118" s="39"/>
+      <c r="B118" s="24"/>
+      <c r="C118" s="24"/>
+      <c r="D118" s="24"/>
+      <c r="E118" s="24"/>
+      <c r="F118" s="24"/>
+      <c r="G118" s="24"/>
+      <c r="H118" s="24"/>
     </row>
     <row r="119" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B119" s="39"/>
-      <c r="C119" s="39"/>
-      <c r="D119" s="39"/>
-      <c r="E119" s="39"/>
-      <c r="F119" s="39"/>
-      <c r="G119" s="39"/>
-      <c r="H119" s="39"/>
+      <c r="B119" s="24"/>
+      <c r="C119" s="24"/>
+      <c r="D119" s="24"/>
+      <c r="E119" s="24"/>
+      <c r="F119" s="24"/>
+      <c r="G119" s="24"/>
+      <c r="H119" s="24"/>
     </row>
     <row r="120" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B120" s="39"/>
-      <c r="C120" s="39"/>
-      <c r="D120" s="39"/>
-      <c r="E120" s="39"/>
-      <c r="F120" s="39"/>
-      <c r="G120" s="39"/>
-      <c r="H120" s="39"/>
+      <c r="B120" s="24"/>
+      <c r="C120" s="24"/>
+      <c r="D120" s="24"/>
+      <c r="E120" s="24"/>
+      <c r="F120" s="24"/>
+      <c r="G120" s="24"/>
+      <c r="H120" s="24"/>
     </row>
     <row r="121" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B121" s="39"/>
-      <c r="C121" s="39"/>
-      <c r="D121" s="39"/>
-      <c r="E121" s="39"/>
-      <c r="F121" s="39"/>
-      <c r="G121" s="39"/>
-      <c r="H121" s="39"/>
+      <c r="B121" s="24"/>
+      <c r="C121" s="24"/>
+      <c r="D121" s="24"/>
+      <c r="E121" s="24"/>
+      <c r="F121" s="24"/>
+      <c r="G121" s="24"/>
+      <c r="H121" s="24"/>
     </row>
     <row r="122" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B122" s="39"/>
-      <c r="C122" s="39"/>
-      <c r="D122" s="39"/>
-      <c r="E122" s="39"/>
-      <c r="F122" s="39"/>
-      <c r="G122" s="39"/>
-      <c r="H122" s="39"/>
+      <c r="B122" s="24"/>
+      <c r="C122" s="24"/>
+      <c r="D122" s="24"/>
+      <c r="E122" s="24"/>
+      <c r="F122" s="24"/>
+      <c r="G122" s="24"/>
+      <c r="H122" s="24"/>
     </row>
     <row r="123" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B123" s="39"/>
-      <c r="C123" s="39"/>
-      <c r="D123" s="39"/>
-      <c r="E123" s="39"/>
-      <c r="F123" s="39"/>
-      <c r="G123" s="39"/>
-      <c r="H123" s="39"/>
+      <c r="B123" s="24"/>
+      <c r="C123" s="24"/>
+      <c r="D123" s="24"/>
+      <c r="E123" s="24"/>
+      <c r="F123" s="24"/>
+      <c r="G123" s="24"/>
+      <c r="H123" s="24"/>
     </row>
     <row r="124" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B124" s="39"/>
-      <c r="C124" s="39"/>
-      <c r="D124" s="39"/>
-      <c r="E124" s="39"/>
-      <c r="F124" s="39"/>
-      <c r="G124" s="39"/>
-      <c r="H124" s="39"/>
+      <c r="B124" s="24"/>
+      <c r="C124" s="24"/>
+      <c r="D124" s="24"/>
+      <c r="E124" s="24"/>
+      <c r="F124" s="24"/>
+      <c r="G124" s="24"/>
+      <c r="H124" s="24"/>
     </row>
     <row r="125" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B125" s="39"/>
-      <c r="C125" s="39"/>
-      <c r="D125" s="39"/>
-      <c r="E125" s="39"/>
-      <c r="F125" s="39"/>
-      <c r="G125" s="39"/>
-      <c r="H125" s="39"/>
+      <c r="B125" s="24"/>
+      <c r="C125" s="24"/>
+      <c r="D125" s="24"/>
+      <c r="E125" s="24"/>
+      <c r="F125" s="24"/>
+      <c r="G125" s="24"/>
+      <c r="H125" s="24"/>
+    </row>
+    <row r="126" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B126" s="24"/>
+      <c r="C126" s="24"/>
+      <c r="D126" s="24"/>
+      <c r="E126" s="24"/>
+      <c r="F126" s="24"/>
+      <c r="G126" s="24"/>
+      <c r="H126" s="24"/>
     </row>
   </sheetData>
-  <mergeCells count="34">
-    <mergeCell ref="B73:C73"/>
+  <mergeCells count="35">
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B41:C41"/>
     <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B75:C75"/>
     <mergeCell ref="B34:C34"/>
     <mergeCell ref="B40:C40"/>
     <mergeCell ref="B35:C35"/>
@@ -52528,31 +52627,13 @@
     <mergeCell ref="B57:C57"/>
     <mergeCell ref="B59:C59"/>
     <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B8:C8"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C80" r:id="rId1"/>
-    <hyperlink ref="C81" r:id="rId2"/>
+    <hyperlink ref="C81" r:id="rId1"/>
+    <hyperlink ref="C82" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -52586,154 +52667,154 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="42" t="s">
+      <c r="A5" s="25" t="s">
         <v>100</v>
       </c>
-      <c r="B5" s="42" t="s">
+      <c r="B5" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="42" t="s">
+      <c r="C5" s="25" t="s">
         <v>101</v>
       </c>
-      <c r="D5" s="42" t="s">
+      <c r="D5" s="25" t="s">
         <v>102</v>
       </c>
-      <c r="E5" s="42" t="s">
+      <c r="E5" s="25" t="s">
         <v>103</v>
       </c>
-      <c r="F5" s="42" t="s">
+      <c r="F5" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="G5" s="42" t="s">
+      <c r="G5" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="H5" s="42" t="s">
+      <c r="H5" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="I5" s="42" t="s">
+      <c r="I5" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K5" s="42"/>
-      <c r="L5" s="42"/>
-      <c r="M5" s="42"/>
+      <c r="K5" s="25"/>
+      <c r="L5" s="25"/>
+      <c r="M5" s="25"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="42" t="s">
+      <c r="A6" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="B6" s="42" t="s">
+      <c r="B6" s="25" t="s">
         <v>107</v>
       </c>
-      <c r="C6" s="42" t="s">
+      <c r="C6" s="25" t="s">
         <v>108</v>
       </c>
-      <c r="D6" s="42" t="s">
+      <c r="D6" s="25" t="s">
         <v>109</v>
       </c>
-      <c r="E6" s="42" t="s">
+      <c r="E6" s="25" t="s">
         <v>110</v>
       </c>
-      <c r="F6" s="42" t="s">
+      <c r="F6" s="25" t="s">
         <v>111</v>
       </c>
-      <c r="G6" s="42" t="s">
+      <c r="G6" s="25" t="s">
         <v>112</v>
       </c>
-      <c r="H6" s="42" t="s">
+      <c r="H6" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="I6" s="42" t="s">
+      <c r="I6" s="25" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="26" t="s">
         <v>115</v>
       </c>
-      <c r="C7" s="44" t="s">
+      <c r="C7" s="27" t="s">
         <v>116</v>
       </c>
-      <c r="D7" s="43" t="s">
+      <c r="D7" s="26" t="s">
         <v>117</v>
       </c>
-      <c r="E7" s="45" t="s">
+      <c r="E7" s="28" t="s">
         <v>118</v>
       </c>
-      <c r="F7" s="44" t="s">
+      <c r="F7" s="27" t="s">
         <v>119</v>
       </c>
-      <c r="G7" s="44" t="s">
+      <c r="G7" s="27" t="s">
         <v>120</v>
       </c>
-      <c r="H7" s="44" t="s">
+      <c r="H7" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="I7" s="46" t="s">
+      <c r="I7" s="29" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B8" s="43" t="s">
+      <c r="B8" s="26" t="s">
         <v>122</v>
       </c>
-      <c r="C8" s="44" t="s">
+      <c r="C8" s="27" t="s">
         <v>123</v>
       </c>
-      <c r="D8" s="43" t="s">
+      <c r="D8" s="26" t="s">
         <v>124</v>
       </c>
-      <c r="E8" s="43" t="s">
+      <c r="E8" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="F8" s="43" t="s">
+      <c r="F8" s="26" t="s">
         <v>126</v>
       </c>
-      <c r="H8" s="44" t="s">
+      <c r="H8" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="I8" s="46" t="s">
+      <c r="I8" s="29" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B9" s="43" t="s">
+      <c r="B9" s="26" t="s">
         <v>129</v>
       </c>
-      <c r="C9" s="44" t="s">
+      <c r="C9" s="27" t="s">
         <v>130</v>
       </c>
-      <c r="D9" s="43" t="s">
+      <c r="D9" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="E9" s="45" t="s">
+      <c r="E9" s="28" t="s">
         <v>132</v>
       </c>
-      <c r="F9" s="43" t="s">
+      <c r="F9" s="26" t="s">
         <v>133</v>
       </c>
-      <c r="I9" s="46" t="s">
+      <c r="I9" s="29" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B10" s="44" t="s">
+      <c r="B10" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="C10" s="44" t="s">
+      <c r="C10" s="27" t="s">
         <v>135</v>
       </c>
-      <c r="I10" s="46" t="s">
+      <c r="I10" s="29" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B11" s="44" t="s">
+      <c r="B11" s="27" t="s">
         <v>137</v>
       </c>
-      <c r="C11" s="44" t="s">
+      <c r="C11" s="27" t="s">
         <v>138</v>
       </c>
-      <c r="I11" s="47" t="s">
+      <c r="I11" s="30" t="s">
         <v>139</v>
       </c>
       <c r="J11">
@@ -52741,13 +52822,13 @@
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B12" s="44" t="s">
+      <c r="B12" s="27" t="s">
         <v>140</v>
       </c>
-      <c r="C12" s="44" t="s">
+      <c r="C12" s="27" t="s">
         <v>141</v>
       </c>
-      <c r="I12" s="47" t="s">
+      <c r="I12" s="30" t="s">
         <v>142</v>
       </c>
       <c r="J12">
@@ -52755,33 +52836,33 @@
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B13" s="44" t="s">
+      <c r="B13" s="27" t="s">
         <v>143</v>
       </c>
-      <c r="I13" s="47" t="s">
+      <c r="I13" s="30" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B14" s="44" t="s">
+      <c r="B14" s="27" t="s">
         <v>145</v>
       </c>
-      <c r="I14" s="47" t="s">
+      <c r="I14" s="30" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B18" s="44" t="s">
+      <c r="B18" s="27" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B19" s="43" t="s">
+      <c r="B19" s="26" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B20" s="45" t="s">
+      <c r="B20" s="28" t="s">
         <v>148</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Plan de configuración actualizado
</commit_message>
<xml_diff>
--- a/Organización/Configuración/Plan_Configuración.xlsx
+++ b/Organización/Configuración/Plan_Configuración.xlsx
@@ -299,7 +299,7 @@
     <t>Mecanismos de respaldo de Datos</t>
   </si>
   <si>
-    <t>Se omite la integración de un mecanismo de respaldos ya que la herramienta bitrix24 genera respaldos por parte de los creadores de forma diaria en cualqueira de sus planes (gratuito y de pago). En caso de requerir una reposición de la base de datos en bitrix24 será necesario ingresar a http://bitrix.es/soporte/helpdesk/index2.php?show_wizard=Y y generar un ticket para reposicion de la base de datos agregando la fecha a la cual se desea dicha actualización, el repositorio de git se encuentra ubicada en la nube por lo que se omite el respaldo del mismo.</t>
+    <t>Se omite la integración de un mecanismo de respaldos ya que la herramienta bitrix24 genera respaldos por parte de los creadores de forma diaria en cualquiera de sus planes (gratuito y de pago). En caso de requerir una reposición de la base de datos en bitrix24 será necesario ingresar a http://bitrix.es/soporte/helpdesk/index2.php?show_wizard=Y y generar un ticket para reposicion de la base de datos agregando la fecha a la cual se desea dicha actualización, el repositorio de git se encuentra ubicada en la nube por lo que se omite el respaldo del mismo.</t>
   </si>
   <si>
     <t>Sistema SOS, se respaldara la base de datos al finalizar cada mes, este respaldo se genera con una peridiocidad amplia debido a que su información por lo generar suele ser estatica la mayor parte del tiempo los archivos de respaldo se deberán almacenar en raíz de carpeta repositorio/backup con el nombre aaaamm.sql (Responsable de ejecución Jovanny Zepeda).</t>
@@ -1090,8 +1090,8 @@
   </sheetPr>
   <dimension ref="1:126"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A71" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D73" activeCellId="0" sqref="D73"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B53" activeCellId="0" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -53714,7 +53714,7 @@
       <c r="G59" s="0"/>
       <c r="H59" s="0"/>
     </row>
-    <row r="60" customFormat="false" ht="63" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="100.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="0"/>
       <c r="B60" s="28" t="s">
         <v>82</v>
@@ -53850,7 +53850,7 @@
       <c r="G71" s="0"/>
       <c r="H71" s="0"/>
     </row>
-    <row r="72" customFormat="false" ht="85.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="107.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="0"/>
       <c r="B72" s="22" t="s">
         <v>89</v>

</xml_diff>

<commit_message>
Plan de condiguracion actualizado
</commit_message>
<xml_diff>
--- a/Organización/Configuración/Plan_Configuración.xlsx
+++ b/Organización/Configuración/Plan_Configuración.xlsx
@@ -177,13 +177,13 @@
     <t>Proyectos</t>
   </si>
   <si>
+    <t>Año</t>
+  </si>
+  <si>
     <t>Minutas de Proyectos</t>
   </si>
   <si>
     <t>Minuta de Compromiso</t>
-  </si>
-  <si>
-    <t>Año</t>
   </si>
   <si>
     <t>MES</t>
@@ -882,12 +882,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1090,8 +1090,8 @@
   </sheetPr>
   <dimension ref="1:126"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A45" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B54" activeCellId="0" sqref="B54"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A30" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B34" activeCellId="0" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -32032,12 +32032,12 @@
       </c>
       <c r="C32" s="11"/>
     </row>
-    <row r="33" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="21"/>
-      <c r="B33" s="19" t="s">
+    <row r="33" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0"/>
+      <c r="B33" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="C33" s="19"/>
+      <c r="C33" s="22"/>
       <c r="D33" s="0"/>
       <c r="E33" s="0"/>
       <c r="F33" s="0"/>
@@ -33062,12 +33062,10 @@
     </row>
     <row r="34" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="0"/>
-      <c r="B34" s="17" t="s">
+      <c r="B34" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="C34" s="22" t="s">
-        <v>9</v>
-      </c>
+      <c r="C34" s="19"/>
       <c r="D34" s="0"/>
       <c r="E34" s="0"/>
       <c r="F34" s="0"/>
@@ -34092,10 +34090,12 @@
     </row>
     <row r="35" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="0"/>
-      <c r="B35" s="23" t="s">
+      <c r="B35" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="C35" s="23"/>
+      <c r="C35" s="23" t="s">
+        <v>9</v>
+      </c>
       <c r="D35" s="0"/>
       <c r="E35" s="0"/>
       <c r="F35" s="0"/>
@@ -35120,10 +35120,10 @@
     </row>
     <row r="36" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="0"/>
-      <c r="B36" s="23" t="s">
+      <c r="B36" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="C36" s="23"/>
+      <c r="C36" s="22"/>
       <c r="D36" s="0"/>
       <c r="E36" s="0"/>
       <c r="F36" s="0"/>
@@ -42325,7 +42325,7 @@
       <c r="B43" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="C43" s="22" t="s">
+      <c r="C43" s="23" t="s">
         <v>62</v>
       </c>
       <c r="D43" s="0"/>
@@ -43355,7 +43355,7 @@
       <c r="B44" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="C44" s="22" t="s">
+      <c r="C44" s="23" t="s">
         <v>63</v>
       </c>
       <c r="D44" s="0"/>
@@ -44385,7 +44385,7 @@
       <c r="B45" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="C45" s="22" t="s">
+      <c r="C45" s="23" t="s">
         <v>65</v>
       </c>
       <c r="D45" s="0"/>
@@ -46443,7 +46443,7 @@
       <c r="B47" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="C47" s="22" t="s">
+      <c r="C47" s="23" t="s">
         <v>67</v>
       </c>
       <c r="D47" s="0"/>
@@ -53840,10 +53840,10 @@
     </row>
     <row r="71" customFormat="false" ht="167.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="0"/>
-      <c r="B71" s="22" t="s">
+      <c r="B71" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="C71" s="22"/>
+      <c r="C71" s="23"/>
       <c r="D71" s="0"/>
       <c r="E71" s="0"/>
       <c r="F71" s="0"/>
@@ -53852,10 +53852,10 @@
     </row>
     <row r="72" customFormat="false" ht="107.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="0"/>
-      <c r="B72" s="22" t="s">
+      <c r="B72" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="C72" s="22"/>
+      <c r="C72" s="23"/>
       <c r="D72" s="0"/>
       <c r="E72" s="0"/>
       <c r="F72" s="0"/>
@@ -54414,7 +54414,7 @@
     <mergeCell ref="B30:C30"/>
     <mergeCell ref="B32:C32"/>
     <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B34:C34"/>
     <mergeCell ref="B36:C36"/>
     <mergeCell ref="B37:C37"/>
     <mergeCell ref="B41:C41"/>

</xml_diff>

<commit_message>
Actualizacion plan de configuración
</commit_message>
<xml_diff>
--- a/Organización/Configuración/Plan_Configuración.xlsx
+++ b/Organización/Configuración/Plan_Configuración.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="161">
   <si>
     <t>Plan de Administración de Configuración</t>
   </si>
@@ -238,6 +238,9 @@
   </si>
   <si>
     <t>Carta de aceptación</t>
+  </si>
+  <si>
+    <t>Carta aceptación</t>
   </si>
   <si>
     <t>Checklist de calidad</t>
@@ -1090,8 +1093,8 @@
   </sheetPr>
   <dimension ref="1:126"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A30" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B34" activeCellId="0" sqref="B34"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A32" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C50" activeCellId="0" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -49526,13 +49529,13 @@
       <c r="AMI49" s="0"/>
       <c r="AMJ49" s="0"/>
     </row>
-    <row r="50" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="10"/>
       <c r="B50" s="17" t="s">
         <v>71</v>
       </c>
       <c r="C50" s="18" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D50" s="0"/>
       <c r="E50" s="0"/>
@@ -51587,10 +51590,10 @@
     <row r="52" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="10"/>
       <c r="B52" s="18" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C52" s="18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D52" s="0"/>
       <c r="E52" s="0"/>
@@ -52617,10 +52620,10 @@
     <row r="53" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="10"/>
       <c r="B53" s="18" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C53" s="18" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D53" s="0"/>
       <c r="E53" s="0"/>
@@ -53653,10 +53656,10 @@
     <row r="55" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="21"/>
       <c r="B55" s="18" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C55" s="18" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D55" s="0"/>
       <c r="E55" s="0"/>
@@ -53667,7 +53670,7 @@
     <row r="56" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="21"/>
       <c r="B56" s="25" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C56" s="25"/>
       <c r="D56" s="0"/>
@@ -53679,7 +53682,7 @@
     <row r="57" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="0"/>
       <c r="B57" s="9" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C57" s="9"/>
       <c r="D57" s="0"/>
@@ -53691,10 +53694,10 @@
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="0"/>
       <c r="B58" s="26" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C58" s="26" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D58" s="0"/>
       <c r="E58" s="0"/>
@@ -53705,7 +53708,7 @@
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="0"/>
       <c r="B59" s="27" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C59" s="27"/>
       <c r="D59" s="0"/>
@@ -53717,10 +53720,10 @@
     <row r="60" customFormat="false" ht="100.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="0"/>
       <c r="B60" s="28" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C60" s="28" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D60" s="0"/>
       <c r="E60" s="0"/>
@@ -53741,7 +53744,7 @@
     <row r="62" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="0"/>
       <c r="B62" s="30" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C62" s="30"/>
       <c r="D62" s="0"/>
@@ -53753,7 +53756,7 @@
     <row r="63" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="0"/>
       <c r="B63" s="31" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C63" s="31"/>
       <c r="D63" s="0"/>
@@ -53797,7 +53800,7 @@
     <row r="67" customFormat="false" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="0"/>
       <c r="B67" s="32" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C67" s="32"/>
       <c r="D67" s="0"/>
@@ -53829,7 +53832,7 @@
     <row r="70" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="35"/>
       <c r="B70" s="36" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C70" s="36"/>
       <c r="D70" s="0"/>
@@ -53841,7 +53844,7 @@
     <row r="71" customFormat="false" ht="167.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="0"/>
       <c r="B71" s="23" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C71" s="23"/>
       <c r="D71" s="0"/>
@@ -53853,7 +53856,7 @@
     <row r="72" customFormat="false" ht="107.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="0"/>
       <c r="B72" s="23" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C72" s="23"/>
       <c r="D72" s="0"/>
@@ -53875,7 +53878,7 @@
     <row r="74" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="0"/>
       <c r="B74" s="9" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C74" s="9"/>
       <c r="D74" s="0"/>
@@ -53887,7 +53890,7 @@
     <row r="75" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="0"/>
       <c r="B75" s="38" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C75" s="38"/>
       <c r="D75" s="0"/>
@@ -53899,10 +53902,10 @@
     <row r="76" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="0"/>
       <c r="B76" s="39" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C76" s="39" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D76" s="0"/>
       <c r="E76" s="0"/>
@@ -53913,10 +53916,10 @@
     <row r="77" customFormat="false" ht="74.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="0"/>
       <c r="B77" s="40" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C77" s="40" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D77" s="0"/>
       <c r="E77" s="0"/>
@@ -53927,10 +53930,10 @@
     <row r="78" customFormat="false" ht="88.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="0"/>
       <c r="B78" s="40" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C78" s="40" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D78" s="0"/>
       <c r="E78" s="0"/>
@@ -53951,13 +53954,13 @@
     <row r="80" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0"/>
       <c r="B80" s="41" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C80" s="41" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D80" s="42" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E80" s="0"/>
       <c r="F80" s="0"/>
@@ -53967,13 +53970,13 @@
     <row r="81" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="43"/>
       <c r="B81" s="44" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C81" s="45" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D81" s="46" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E81" s="0"/>
       <c r="F81" s="0"/>
@@ -53983,13 +53986,13 @@
     <row r="82" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0"/>
       <c r="B82" s="44" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C82" s="45" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D82" s="46" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E82" s="0"/>
       <c r="F82" s="0"/>
@@ -53999,13 +54002,13 @@
     <row r="83" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="35"/>
       <c r="B83" s="47" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C83" s="47" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D83" s="46" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E83" s="0"/>
       <c r="F83" s="0"/>
@@ -54479,36 +54482,36 @@
   <sheetData>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="48" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B5" s="48" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="48" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D5" s="48" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E5" s="48" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F5" s="48" t="s">
         <v>47</v>
       </c>
       <c r="G5" s="48" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="H5" s="48" t="s">
         <v>39</v>
       </c>
       <c r="I5" s="48" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="K5" s="48"/>
       <c r="L5" s="48"/>
@@ -54516,100 +54519,100 @@
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="48" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B6" s="48" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C6" s="48" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D6" s="48" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E6" s="48" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F6" s="48" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="G6" s="48" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H6" s="48" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="I6" s="48" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="49" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C7" s="50" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D7" s="49" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E7" s="51" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F7" s="50" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="G7" s="50" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H7" s="50" t="s">
         <v>40</v>
       </c>
       <c r="I7" s="52" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="49" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C8" s="50" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D8" s="49" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E8" s="49" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F8" s="49" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="H8" s="50" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="I8" s="52" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="49" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C9" s="50" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D9" s="49" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E9" s="51" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="F9" s="49" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="I9" s="52" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -54617,21 +54620,21 @@
         <v>62</v>
       </c>
       <c r="C10" s="50" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="I10" s="52" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="50" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C11" s="50" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="I11" s="53" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="J11" s="0" t="n">
         <v>51</v>
@@ -54639,13 +54642,13 @@
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="50" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C12" s="50" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="I12" s="53" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="J12" s="0" t="n">
         <v>50</v>
@@ -54653,33 +54656,33 @@
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="50" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="I13" s="53" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="50" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="I14" s="53" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="50" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="49" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="51" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
actualizacion del plan de configuración
</commit_message>
<xml_diff>
--- a/Organización/Configuración/Plan_Configuración.xlsx
+++ b/Organización/Configuración/Plan_Configuración.xlsx
@@ -255,7 +255,7 @@
     <t>Reporte no conformidades</t>
   </si>
   <si>
-    <t>No_conformidades</t>
+    <t>No_conformidades_&lt;proyecto&gt;</t>
   </si>
   <si>
     <t>Solicitud de cambio</t>
@@ -264,7 +264,7 @@
     <t>Solicitud de cambios_aammdd</t>
   </si>
   <si>
-    <t>La linea base representa un espejo de la configuración del árbol principal, para acceder a ella es necesario cambiar de rama con git checkout base y seguir los documentos acorde a la configuración demostrada en el item de configuración anterior (carpeta de proyecto).</t>
+    <t>La linea base deberá estar como una carpeta adicional llamada lineabase que deberá estar dentro del proyecto y contener los documentos descritos a continuación</t>
   </si>
   <si>
     <t>Linea Base</t>
@@ -279,13 +279,13 @@
     <t>base</t>
   </si>
   <si>
-    <t>Requerimientos (Al finalizar etapa de Ventas) + Estimación(Al finalizar etapa de ventas) + Plan_de_proyecto(Al finalizar etapa de planeación) + Carta de aceptación(Al finalizar etapa de Cierre)</t>
+    <t>Requerimientos + Estimación + Plan_de_proyecto + Carta de aceptación</t>
   </si>
   <si>
-    <t>Mecanismos para la generacion de la linea base</t>
+    <t>Mecanismos para la generación de la linea base</t>
   </si>
   <si>
-    <t>Seleccion de los archivos dentro git, para agregarlos es necesario ejecutar el comando git add + nombre del archivo linea base , posteriormente se ingresan en una rama secundario del repositorio con el comando git push origin base.</t>
+    <t>Seleccionar los documentos linea base, copiarlos en la carpeta lineabase y subir al repositorio los archivos </t>
   </si>
   <si>
     <r>
@@ -1096,8 +1096,8 @@
   </sheetPr>
   <dimension ref="1:127"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A56" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D62" activeCellId="0" sqref="D62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>

<commit_message>
Cambios plan de configuración nomnclatura carta de aceptaciona a agradecimiento
</commit_message>
<xml_diff>
--- a/Organización/Configuración/Plan_Configuración.xlsx
+++ b/Organización/Configuración/Plan_Configuración.xlsx
@@ -51,7 +51,7 @@
     <t>Carta de aceptación</t>
   </si>
   <si>
-    <t>PTL_carta_aceptacion</t>
+    <t>PTL_carta_agradecimiento</t>
   </si>
   <si>
     <t>Planeación</t>
@@ -282,7 +282,7 @@
     <t>Encuesta_satisfacción</t>
   </si>
   <si>
-    <t>Carta aceptación</t>
+    <t>Carta_agradecimiento</t>
   </si>
   <si>
     <t>Compras</t>
@@ -1188,8 +1188,8 @@
   </sheetPr>
   <dimension ref="1:139"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A58" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B66" activeCellId="0" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2274,17 +2274,2059 @@
       <c r="C2" s="5"/>
       <c r="D2" s="6"/>
     </row>
-    <row r="3" s="4" customFormat="true" ht="79.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="79.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4"/>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
       <c r="D3" s="6"/>
+      <c r="E3" s="0"/>
+      <c r="F3" s="0"/>
+      <c r="G3" s="0"/>
+      <c r="H3" s="0"/>
+      <c r="I3" s="0"/>
+      <c r="J3" s="0"/>
+      <c r="K3" s="0"/>
+      <c r="L3" s="0"/>
+      <c r="M3" s="0"/>
+      <c r="N3" s="0"/>
+      <c r="O3" s="0"/>
+      <c r="P3" s="0"/>
+      <c r="Q3" s="0"/>
+      <c r="R3" s="0"/>
+      <c r="S3" s="0"/>
+      <c r="T3" s="0"/>
+      <c r="U3" s="0"/>
+      <c r="V3" s="0"/>
+      <c r="W3" s="0"/>
+      <c r="X3" s="0"/>
+      <c r="Y3" s="0"/>
+      <c r="Z3" s="0"/>
+      <c r="AA3" s="0"/>
+      <c r="AB3" s="0"/>
+      <c r="AC3" s="0"/>
+      <c r="AD3" s="0"/>
+      <c r="AE3" s="0"/>
+      <c r="AF3" s="0"/>
+      <c r="AG3" s="0"/>
+      <c r="AH3" s="0"/>
+      <c r="AI3" s="0"/>
+      <c r="AJ3" s="0"/>
+      <c r="AK3" s="0"/>
+      <c r="AL3" s="0"/>
+      <c r="AM3" s="0"/>
+      <c r="AN3" s="0"/>
+      <c r="AO3" s="0"/>
+      <c r="AP3" s="0"/>
+      <c r="AQ3" s="0"/>
+      <c r="AR3" s="0"/>
+      <c r="AS3" s="0"/>
+      <c r="AT3" s="0"/>
+      <c r="AU3" s="0"/>
+      <c r="AV3" s="0"/>
+      <c r="AW3" s="0"/>
+      <c r="AX3" s="0"/>
+      <c r="AY3" s="0"/>
+      <c r="AZ3" s="0"/>
+      <c r="BA3" s="0"/>
+      <c r="BB3" s="0"/>
+      <c r="BC3" s="0"/>
+      <c r="BD3" s="0"/>
+      <c r="BE3" s="0"/>
+      <c r="BF3" s="0"/>
+      <c r="BG3" s="0"/>
+      <c r="BH3" s="0"/>
+      <c r="BI3" s="0"/>
+      <c r="BJ3" s="0"/>
+      <c r="BK3" s="0"/>
+      <c r="BL3" s="0"/>
+      <c r="BM3" s="0"/>
+      <c r="BN3" s="0"/>
+      <c r="BO3" s="0"/>
+      <c r="BP3" s="0"/>
+      <c r="BQ3" s="0"/>
+      <c r="BR3" s="0"/>
+      <c r="BS3" s="0"/>
+      <c r="BT3" s="0"/>
+      <c r="BU3" s="0"/>
+      <c r="BV3" s="0"/>
+      <c r="BW3" s="0"/>
+      <c r="BX3" s="0"/>
+      <c r="BY3" s="0"/>
+      <c r="BZ3" s="0"/>
+      <c r="CA3" s="0"/>
+      <c r="CB3" s="0"/>
+      <c r="CC3" s="0"/>
+      <c r="CD3" s="0"/>
+      <c r="CE3" s="0"/>
+      <c r="CF3" s="0"/>
+      <c r="CG3" s="0"/>
+      <c r="CH3" s="0"/>
+      <c r="CI3" s="0"/>
+      <c r="CJ3" s="0"/>
+      <c r="CK3" s="0"/>
+      <c r="CL3" s="0"/>
+      <c r="CM3" s="0"/>
+      <c r="CN3" s="0"/>
+      <c r="CO3" s="0"/>
+      <c r="CP3" s="0"/>
+      <c r="CQ3" s="0"/>
+      <c r="CR3" s="0"/>
+      <c r="CS3" s="0"/>
+      <c r="CT3" s="0"/>
+      <c r="CU3" s="0"/>
+      <c r="CV3" s="0"/>
+      <c r="CW3" s="0"/>
+      <c r="CX3" s="0"/>
+      <c r="CY3" s="0"/>
+      <c r="CZ3" s="0"/>
+      <c r="DA3" s="0"/>
+      <c r="DB3" s="0"/>
+      <c r="DC3" s="0"/>
+      <c r="DD3" s="0"/>
+      <c r="DE3" s="0"/>
+      <c r="DF3" s="0"/>
+      <c r="DG3" s="0"/>
+      <c r="DH3" s="0"/>
+      <c r="DI3" s="0"/>
+      <c r="DJ3" s="0"/>
+      <c r="DK3" s="0"/>
+      <c r="DL3" s="0"/>
+      <c r="DM3" s="0"/>
+      <c r="DN3" s="0"/>
+      <c r="DO3" s="0"/>
+      <c r="DP3" s="0"/>
+      <c r="DQ3" s="0"/>
+      <c r="DR3" s="0"/>
+      <c r="DS3" s="0"/>
+      <c r="DT3" s="0"/>
+      <c r="DU3" s="0"/>
+      <c r="DV3" s="0"/>
+      <c r="DW3" s="0"/>
+      <c r="DX3" s="0"/>
+      <c r="DY3" s="0"/>
+      <c r="DZ3" s="0"/>
+      <c r="EA3" s="0"/>
+      <c r="EB3" s="0"/>
+      <c r="EC3" s="0"/>
+      <c r="ED3" s="0"/>
+      <c r="EE3" s="0"/>
+      <c r="EF3" s="0"/>
+      <c r="EG3" s="0"/>
+      <c r="EH3" s="0"/>
+      <c r="EI3" s="0"/>
+      <c r="EJ3" s="0"/>
+      <c r="EK3" s="0"/>
+      <c r="EL3" s="0"/>
+      <c r="EM3" s="0"/>
+      <c r="EN3" s="0"/>
+      <c r="EO3" s="0"/>
+      <c r="EP3" s="0"/>
+      <c r="EQ3" s="0"/>
+      <c r="ER3" s="0"/>
+      <c r="ES3" s="0"/>
+      <c r="ET3" s="0"/>
+      <c r="EU3" s="0"/>
+      <c r="EV3" s="0"/>
+      <c r="EW3" s="0"/>
+      <c r="EX3" s="0"/>
+      <c r="EY3" s="0"/>
+      <c r="EZ3" s="0"/>
+      <c r="FA3" s="0"/>
+      <c r="FB3" s="0"/>
+      <c r="FC3" s="0"/>
+      <c r="FD3" s="0"/>
+      <c r="FE3" s="0"/>
+      <c r="FF3" s="0"/>
+      <c r="FG3" s="0"/>
+      <c r="FH3" s="0"/>
+      <c r="FI3" s="0"/>
+      <c r="FJ3" s="0"/>
+      <c r="FK3" s="0"/>
+      <c r="FL3" s="0"/>
+      <c r="FM3" s="0"/>
+      <c r="FN3" s="0"/>
+      <c r="FO3" s="0"/>
+      <c r="FP3" s="0"/>
+      <c r="FQ3" s="0"/>
+      <c r="FR3" s="0"/>
+      <c r="FS3" s="0"/>
+      <c r="FT3" s="0"/>
+      <c r="FU3" s="0"/>
+      <c r="FV3" s="0"/>
+      <c r="FW3" s="0"/>
+      <c r="FX3" s="0"/>
+      <c r="FY3" s="0"/>
+      <c r="FZ3" s="0"/>
+      <c r="GA3" s="0"/>
+      <c r="GB3" s="0"/>
+      <c r="GC3" s="0"/>
+      <c r="GD3" s="0"/>
+      <c r="GE3" s="0"/>
+      <c r="GF3" s="0"/>
+      <c r="GG3" s="0"/>
+      <c r="GH3" s="0"/>
+      <c r="GI3" s="0"/>
+      <c r="GJ3" s="0"/>
+      <c r="GK3" s="0"/>
+      <c r="GL3" s="0"/>
+      <c r="GM3" s="0"/>
+      <c r="GN3" s="0"/>
+      <c r="GO3" s="0"/>
+      <c r="GP3" s="0"/>
+      <c r="GQ3" s="0"/>
+      <c r="GR3" s="0"/>
+      <c r="GS3" s="0"/>
+      <c r="GT3" s="0"/>
+      <c r="GU3" s="0"/>
+      <c r="GV3" s="0"/>
+      <c r="GW3" s="0"/>
+      <c r="GX3" s="0"/>
+      <c r="GY3" s="0"/>
+      <c r="GZ3" s="0"/>
+      <c r="HA3" s="0"/>
+      <c r="HB3" s="0"/>
+      <c r="HC3" s="0"/>
+      <c r="HD3" s="0"/>
+      <c r="HE3" s="0"/>
+      <c r="HF3" s="0"/>
+      <c r="HG3" s="0"/>
+      <c r="HH3" s="0"/>
+      <c r="HI3" s="0"/>
+      <c r="HJ3" s="0"/>
+      <c r="HK3" s="0"/>
+      <c r="HL3" s="0"/>
+      <c r="HM3" s="0"/>
+      <c r="HN3" s="0"/>
+      <c r="HO3" s="0"/>
+      <c r="HP3" s="0"/>
+      <c r="HQ3" s="0"/>
+      <c r="HR3" s="0"/>
+      <c r="HS3" s="0"/>
+      <c r="HT3" s="0"/>
+      <c r="HU3" s="0"/>
+      <c r="HV3" s="0"/>
+      <c r="HW3" s="0"/>
+      <c r="HX3" s="0"/>
+      <c r="HY3" s="0"/>
+      <c r="HZ3" s="0"/>
+      <c r="IA3" s="0"/>
+      <c r="IB3" s="0"/>
+      <c r="IC3" s="0"/>
+      <c r="ID3" s="0"/>
+      <c r="IE3" s="0"/>
+      <c r="IF3" s="0"/>
+      <c r="IG3" s="0"/>
+      <c r="IH3" s="0"/>
+      <c r="II3" s="0"/>
+      <c r="IJ3" s="0"/>
+      <c r="IK3" s="0"/>
+      <c r="IL3" s="0"/>
+      <c r="IM3" s="0"/>
+      <c r="IN3" s="0"/>
+      <c r="IO3" s="0"/>
+      <c r="IP3" s="0"/>
+      <c r="IQ3" s="0"/>
+      <c r="IR3" s="0"/>
+      <c r="IS3" s="0"/>
+      <c r="IT3" s="0"/>
+      <c r="IU3" s="0"/>
+      <c r="IV3" s="0"/>
+      <c r="IW3" s="0"/>
+      <c r="IX3" s="0"/>
+      <c r="IY3" s="0"/>
+      <c r="IZ3" s="0"/>
+      <c r="JA3" s="0"/>
+      <c r="JB3" s="0"/>
+      <c r="JC3" s="0"/>
+      <c r="JD3" s="0"/>
+      <c r="JE3" s="0"/>
+      <c r="JF3" s="0"/>
+      <c r="JG3" s="0"/>
+      <c r="JH3" s="0"/>
+      <c r="JI3" s="0"/>
+      <c r="JJ3" s="0"/>
+      <c r="JK3" s="0"/>
+      <c r="JL3" s="0"/>
+      <c r="JM3" s="0"/>
+      <c r="JN3" s="0"/>
+      <c r="JO3" s="0"/>
+      <c r="JP3" s="0"/>
+      <c r="JQ3" s="0"/>
+      <c r="JR3" s="0"/>
+      <c r="JS3" s="0"/>
+      <c r="JT3" s="0"/>
+      <c r="JU3" s="0"/>
+      <c r="JV3" s="0"/>
+      <c r="JW3" s="0"/>
+      <c r="JX3" s="0"/>
+      <c r="JY3" s="0"/>
+      <c r="JZ3" s="0"/>
+      <c r="KA3" s="0"/>
+      <c r="KB3" s="0"/>
+      <c r="KC3" s="0"/>
+      <c r="KD3" s="0"/>
+      <c r="KE3" s="0"/>
+      <c r="KF3" s="0"/>
+      <c r="KG3" s="0"/>
+      <c r="KH3" s="0"/>
+      <c r="KI3" s="0"/>
+      <c r="KJ3" s="0"/>
+      <c r="KK3" s="0"/>
+      <c r="KL3" s="0"/>
+      <c r="KM3" s="0"/>
+      <c r="KN3" s="0"/>
+      <c r="KO3" s="0"/>
+      <c r="KP3" s="0"/>
+      <c r="KQ3" s="0"/>
+      <c r="KR3" s="0"/>
+      <c r="KS3" s="0"/>
+      <c r="KT3" s="0"/>
+      <c r="KU3" s="0"/>
+      <c r="KV3" s="0"/>
+      <c r="KW3" s="0"/>
+      <c r="KX3" s="0"/>
+      <c r="KY3" s="0"/>
+      <c r="KZ3" s="0"/>
+      <c r="LA3" s="0"/>
+      <c r="LB3" s="0"/>
+      <c r="LC3" s="0"/>
+      <c r="LD3" s="0"/>
+      <c r="LE3" s="0"/>
+      <c r="LF3" s="0"/>
+      <c r="LG3" s="0"/>
+      <c r="LH3" s="0"/>
+      <c r="LI3" s="0"/>
+      <c r="LJ3" s="0"/>
+      <c r="LK3" s="0"/>
+      <c r="LL3" s="0"/>
+      <c r="LM3" s="0"/>
+      <c r="LN3" s="0"/>
+      <c r="LO3" s="0"/>
+      <c r="LP3" s="0"/>
+      <c r="LQ3" s="0"/>
+      <c r="LR3" s="0"/>
+      <c r="LS3" s="0"/>
+      <c r="LT3" s="0"/>
+      <c r="LU3" s="0"/>
+      <c r="LV3" s="0"/>
+      <c r="LW3" s="0"/>
+      <c r="LX3" s="0"/>
+      <c r="LY3" s="0"/>
+      <c r="LZ3" s="0"/>
+      <c r="MA3" s="0"/>
+      <c r="MB3" s="0"/>
+      <c r="MC3" s="0"/>
+      <c r="MD3" s="0"/>
+      <c r="ME3" s="0"/>
+      <c r="MF3" s="0"/>
+      <c r="MG3" s="0"/>
+      <c r="MH3" s="0"/>
+      <c r="MI3" s="0"/>
+      <c r="MJ3" s="0"/>
+      <c r="MK3" s="0"/>
+      <c r="ML3" s="0"/>
+      <c r="MM3" s="0"/>
+      <c r="MN3" s="0"/>
+      <c r="MO3" s="0"/>
+      <c r="MP3" s="0"/>
+      <c r="MQ3" s="0"/>
+      <c r="MR3" s="0"/>
+      <c r="MS3" s="0"/>
+      <c r="MT3" s="0"/>
+      <c r="MU3" s="0"/>
+      <c r="MV3" s="0"/>
+      <c r="MW3" s="0"/>
+      <c r="MX3" s="0"/>
+      <c r="MY3" s="0"/>
+      <c r="MZ3" s="0"/>
+      <c r="NA3" s="0"/>
+      <c r="NB3" s="0"/>
+      <c r="NC3" s="0"/>
+      <c r="ND3" s="0"/>
+      <c r="NE3" s="0"/>
+      <c r="NF3" s="0"/>
+      <c r="NG3" s="0"/>
+      <c r="NH3" s="0"/>
+      <c r="NI3" s="0"/>
+      <c r="NJ3" s="0"/>
+      <c r="NK3" s="0"/>
+      <c r="NL3" s="0"/>
+      <c r="NM3" s="0"/>
+      <c r="NN3" s="0"/>
+      <c r="NO3" s="0"/>
+      <c r="NP3" s="0"/>
+      <c r="NQ3" s="0"/>
+      <c r="NR3" s="0"/>
+      <c r="NS3" s="0"/>
+      <c r="NT3" s="0"/>
+      <c r="NU3" s="0"/>
+      <c r="NV3" s="0"/>
+      <c r="NW3" s="0"/>
+      <c r="NX3" s="0"/>
+      <c r="NY3" s="0"/>
+      <c r="NZ3" s="0"/>
+      <c r="OA3" s="0"/>
+      <c r="OB3" s="0"/>
+      <c r="OC3" s="0"/>
+      <c r="OD3" s="0"/>
+      <c r="OE3" s="0"/>
+      <c r="OF3" s="0"/>
+      <c r="OG3" s="0"/>
+      <c r="OH3" s="0"/>
+      <c r="OI3" s="0"/>
+      <c r="OJ3" s="0"/>
+      <c r="OK3" s="0"/>
+      <c r="OL3" s="0"/>
+      <c r="OM3" s="0"/>
+      <c r="ON3" s="0"/>
+      <c r="OO3" s="0"/>
+      <c r="OP3" s="0"/>
+      <c r="OQ3" s="0"/>
+      <c r="OR3" s="0"/>
+      <c r="OS3" s="0"/>
+      <c r="OT3" s="0"/>
+      <c r="OU3" s="0"/>
+      <c r="OV3" s="0"/>
+      <c r="OW3" s="0"/>
+      <c r="OX3" s="0"/>
+      <c r="OY3" s="0"/>
+      <c r="OZ3" s="0"/>
+      <c r="PA3" s="0"/>
+      <c r="PB3" s="0"/>
+      <c r="PC3" s="0"/>
+      <c r="PD3" s="0"/>
+      <c r="PE3" s="0"/>
+      <c r="PF3" s="0"/>
+      <c r="PG3" s="0"/>
+      <c r="PH3" s="0"/>
+      <c r="PI3" s="0"/>
+      <c r="PJ3" s="0"/>
+      <c r="PK3" s="0"/>
+      <c r="PL3" s="0"/>
+      <c r="PM3" s="0"/>
+      <c r="PN3" s="0"/>
+      <c r="PO3" s="0"/>
+      <c r="PP3" s="0"/>
+      <c r="PQ3" s="0"/>
+      <c r="PR3" s="0"/>
+      <c r="PS3" s="0"/>
+      <c r="PT3" s="0"/>
+      <c r="PU3" s="0"/>
+      <c r="PV3" s="0"/>
+      <c r="PW3" s="0"/>
+      <c r="PX3" s="0"/>
+      <c r="PY3" s="0"/>
+      <c r="PZ3" s="0"/>
+      <c r="QA3" s="0"/>
+      <c r="QB3" s="0"/>
+      <c r="QC3" s="0"/>
+      <c r="QD3" s="0"/>
+      <c r="QE3" s="0"/>
+      <c r="QF3" s="0"/>
+      <c r="QG3" s="0"/>
+      <c r="QH3" s="0"/>
+      <c r="QI3" s="0"/>
+      <c r="QJ3" s="0"/>
+      <c r="QK3" s="0"/>
+      <c r="QL3" s="0"/>
+      <c r="QM3" s="0"/>
+      <c r="QN3" s="0"/>
+      <c r="QO3" s="0"/>
+      <c r="QP3" s="0"/>
+      <c r="QQ3" s="0"/>
+      <c r="QR3" s="0"/>
+      <c r="QS3" s="0"/>
+      <c r="QT3" s="0"/>
+      <c r="QU3" s="0"/>
+      <c r="QV3" s="0"/>
+      <c r="QW3" s="0"/>
+      <c r="QX3" s="0"/>
+      <c r="QY3" s="0"/>
+      <c r="QZ3" s="0"/>
+      <c r="RA3" s="0"/>
+      <c r="RB3" s="0"/>
+      <c r="RC3" s="0"/>
+      <c r="RD3" s="0"/>
+      <c r="RE3" s="0"/>
+      <c r="RF3" s="0"/>
+      <c r="RG3" s="0"/>
+      <c r="RH3" s="0"/>
+      <c r="RI3" s="0"/>
+      <c r="RJ3" s="0"/>
+      <c r="RK3" s="0"/>
+      <c r="RL3" s="0"/>
+      <c r="RM3" s="0"/>
+      <c r="RN3" s="0"/>
+      <c r="RO3" s="0"/>
+      <c r="RP3" s="0"/>
+      <c r="RQ3" s="0"/>
+      <c r="RR3" s="0"/>
+      <c r="RS3" s="0"/>
+      <c r="RT3" s="0"/>
+      <c r="RU3" s="0"/>
+      <c r="RV3" s="0"/>
+      <c r="RW3" s="0"/>
+      <c r="RX3" s="0"/>
+      <c r="RY3" s="0"/>
+      <c r="RZ3" s="0"/>
+      <c r="SA3" s="0"/>
+      <c r="SB3" s="0"/>
+      <c r="SC3" s="0"/>
+      <c r="SD3" s="0"/>
+      <c r="SE3" s="0"/>
+      <c r="SF3" s="0"/>
+      <c r="SG3" s="0"/>
+      <c r="SH3" s="0"/>
+      <c r="SI3" s="0"/>
+      <c r="SJ3" s="0"/>
+      <c r="SK3" s="0"/>
+      <c r="SL3" s="0"/>
+      <c r="SM3" s="0"/>
+      <c r="SN3" s="0"/>
+      <c r="SO3" s="0"/>
+      <c r="SP3" s="0"/>
+      <c r="SQ3" s="0"/>
+      <c r="SR3" s="0"/>
+      <c r="SS3" s="0"/>
+      <c r="ST3" s="0"/>
+      <c r="SU3" s="0"/>
+      <c r="SV3" s="0"/>
+      <c r="SW3" s="0"/>
+      <c r="SX3" s="0"/>
+      <c r="SY3" s="0"/>
+      <c r="SZ3" s="0"/>
+      <c r="TA3" s="0"/>
+      <c r="TB3" s="0"/>
+      <c r="TC3" s="0"/>
+      <c r="TD3" s="0"/>
+      <c r="TE3" s="0"/>
+      <c r="TF3" s="0"/>
+      <c r="TG3" s="0"/>
+      <c r="TH3" s="0"/>
+      <c r="TI3" s="0"/>
+      <c r="TJ3" s="0"/>
+      <c r="TK3" s="0"/>
+      <c r="TL3" s="0"/>
+      <c r="TM3" s="0"/>
+      <c r="TN3" s="0"/>
+      <c r="TO3" s="0"/>
+      <c r="TP3" s="0"/>
+      <c r="TQ3" s="0"/>
+      <c r="TR3" s="0"/>
+      <c r="TS3" s="0"/>
+      <c r="TT3" s="0"/>
+      <c r="TU3" s="0"/>
+      <c r="TV3" s="0"/>
+      <c r="TW3" s="0"/>
+      <c r="TX3" s="0"/>
+      <c r="TY3" s="0"/>
+      <c r="TZ3" s="0"/>
+      <c r="UA3" s="0"/>
+      <c r="UB3" s="0"/>
+      <c r="UC3" s="0"/>
+      <c r="UD3" s="0"/>
+      <c r="UE3" s="0"/>
+      <c r="UF3" s="0"/>
+      <c r="UG3" s="0"/>
+      <c r="UH3" s="0"/>
+      <c r="UI3" s="0"/>
+      <c r="UJ3" s="0"/>
+      <c r="UK3" s="0"/>
+      <c r="UL3" s="0"/>
+      <c r="UM3" s="0"/>
+      <c r="UN3" s="0"/>
+      <c r="UO3" s="0"/>
+      <c r="UP3" s="0"/>
+      <c r="UQ3" s="0"/>
+      <c r="UR3" s="0"/>
+      <c r="US3" s="0"/>
+      <c r="UT3" s="0"/>
+      <c r="UU3" s="0"/>
+      <c r="UV3" s="0"/>
+      <c r="UW3" s="0"/>
+      <c r="UX3" s="0"/>
+      <c r="UY3" s="0"/>
+      <c r="UZ3" s="0"/>
+      <c r="VA3" s="0"/>
+      <c r="VB3" s="0"/>
+      <c r="VC3" s="0"/>
+      <c r="VD3" s="0"/>
+      <c r="VE3" s="0"/>
+      <c r="VF3" s="0"/>
+      <c r="VG3" s="0"/>
+      <c r="VH3" s="0"/>
+      <c r="VI3" s="0"/>
+      <c r="VJ3" s="0"/>
+      <c r="VK3" s="0"/>
+      <c r="VL3" s="0"/>
+      <c r="VM3" s="0"/>
+      <c r="VN3" s="0"/>
+      <c r="VO3" s="0"/>
+      <c r="VP3" s="0"/>
+      <c r="VQ3" s="0"/>
+      <c r="VR3" s="0"/>
+      <c r="VS3" s="0"/>
+      <c r="VT3" s="0"/>
+      <c r="VU3" s="0"/>
+      <c r="VV3" s="0"/>
+      <c r="VW3" s="0"/>
+      <c r="VX3" s="0"/>
+      <c r="VY3" s="0"/>
+      <c r="VZ3" s="0"/>
+      <c r="WA3" s="0"/>
+      <c r="WB3" s="0"/>
+      <c r="WC3" s="0"/>
+      <c r="WD3" s="0"/>
+      <c r="WE3" s="0"/>
+      <c r="WF3" s="0"/>
+      <c r="WG3" s="0"/>
+      <c r="WH3" s="0"/>
+      <c r="WI3" s="0"/>
+      <c r="WJ3" s="0"/>
+      <c r="WK3" s="0"/>
+      <c r="WL3" s="0"/>
+      <c r="WM3" s="0"/>
+      <c r="WN3" s="0"/>
+      <c r="WO3" s="0"/>
+      <c r="WP3" s="0"/>
+      <c r="WQ3" s="0"/>
+      <c r="WR3" s="0"/>
+      <c r="WS3" s="0"/>
+      <c r="WT3" s="0"/>
+      <c r="WU3" s="0"/>
+      <c r="WV3" s="0"/>
+      <c r="WW3" s="0"/>
+      <c r="WX3" s="0"/>
+      <c r="WY3" s="0"/>
+      <c r="WZ3" s="0"/>
+      <c r="XA3" s="0"/>
+      <c r="XB3" s="0"/>
+      <c r="XC3" s="0"/>
+      <c r="XD3" s="0"/>
+      <c r="XE3" s="0"/>
+      <c r="XF3" s="0"/>
+      <c r="XG3" s="0"/>
+      <c r="XH3" s="0"/>
+      <c r="XI3" s="0"/>
+      <c r="XJ3" s="0"/>
+      <c r="XK3" s="0"/>
+      <c r="XL3" s="0"/>
+      <c r="XM3" s="0"/>
+      <c r="XN3" s="0"/>
+      <c r="XO3" s="0"/>
+      <c r="XP3" s="0"/>
+      <c r="XQ3" s="0"/>
+      <c r="XR3" s="0"/>
+      <c r="XS3" s="0"/>
+      <c r="XT3" s="0"/>
+      <c r="XU3" s="0"/>
+      <c r="XV3" s="0"/>
+      <c r="XW3" s="0"/>
+      <c r="XX3" s="0"/>
+      <c r="XY3" s="0"/>
+      <c r="XZ3" s="0"/>
+      <c r="YA3" s="0"/>
+      <c r="YB3" s="0"/>
+      <c r="YC3" s="0"/>
+      <c r="YD3" s="0"/>
+      <c r="YE3" s="0"/>
+      <c r="YF3" s="0"/>
+      <c r="YG3" s="0"/>
+      <c r="YH3" s="0"/>
+      <c r="YI3" s="0"/>
+      <c r="YJ3" s="0"/>
+      <c r="YK3" s="0"/>
+      <c r="YL3" s="0"/>
+      <c r="YM3" s="0"/>
+      <c r="YN3" s="0"/>
+      <c r="YO3" s="0"/>
+      <c r="YP3" s="0"/>
+      <c r="YQ3" s="0"/>
+      <c r="YR3" s="0"/>
+      <c r="YS3" s="0"/>
+      <c r="YT3" s="0"/>
+      <c r="YU3" s="0"/>
+      <c r="YV3" s="0"/>
+      <c r="YW3" s="0"/>
+      <c r="YX3" s="0"/>
+      <c r="YY3" s="0"/>
+      <c r="YZ3" s="0"/>
+      <c r="ZA3" s="0"/>
+      <c r="ZB3" s="0"/>
+      <c r="ZC3" s="0"/>
+      <c r="ZD3" s="0"/>
+      <c r="ZE3" s="0"/>
+      <c r="ZF3" s="0"/>
+      <c r="ZG3" s="0"/>
+      <c r="ZH3" s="0"/>
+      <c r="ZI3" s="0"/>
+      <c r="ZJ3" s="0"/>
+      <c r="ZK3" s="0"/>
+      <c r="ZL3" s="0"/>
+      <c r="ZM3" s="0"/>
+      <c r="ZN3" s="0"/>
+      <c r="ZO3" s="0"/>
+      <c r="ZP3" s="0"/>
+      <c r="ZQ3" s="0"/>
+      <c r="ZR3" s="0"/>
+      <c r="ZS3" s="0"/>
+      <c r="ZT3" s="0"/>
+      <c r="ZU3" s="0"/>
+      <c r="ZV3" s="0"/>
+      <c r="ZW3" s="0"/>
+      <c r="ZX3" s="0"/>
+      <c r="ZY3" s="0"/>
+      <c r="ZZ3" s="0"/>
+      <c r="AAA3" s="0"/>
+      <c r="AAB3" s="0"/>
+      <c r="AAC3" s="0"/>
+      <c r="AAD3" s="0"/>
+      <c r="AAE3" s="0"/>
+      <c r="AAF3" s="0"/>
+      <c r="AAG3" s="0"/>
+      <c r="AAH3" s="0"/>
+      <c r="AAI3" s="0"/>
+      <c r="AAJ3" s="0"/>
+      <c r="AAK3" s="0"/>
+      <c r="AAL3" s="0"/>
+      <c r="AAM3" s="0"/>
+      <c r="AAN3" s="0"/>
+      <c r="AAO3" s="0"/>
+      <c r="AAP3" s="0"/>
+      <c r="AAQ3" s="0"/>
+      <c r="AAR3" s="0"/>
+      <c r="AAS3" s="0"/>
+      <c r="AAT3" s="0"/>
+      <c r="AAU3" s="0"/>
+      <c r="AAV3" s="0"/>
+      <c r="AAW3" s="0"/>
+      <c r="AAX3" s="0"/>
+      <c r="AAY3" s="0"/>
+      <c r="AAZ3" s="0"/>
+      <c r="ABA3" s="0"/>
+      <c r="ABB3" s="0"/>
+      <c r="ABC3" s="0"/>
+      <c r="ABD3" s="0"/>
+      <c r="ABE3" s="0"/>
+      <c r="ABF3" s="0"/>
+      <c r="ABG3" s="0"/>
+      <c r="ABH3" s="0"/>
+      <c r="ABI3" s="0"/>
+      <c r="ABJ3" s="0"/>
+      <c r="ABK3" s="0"/>
+      <c r="ABL3" s="0"/>
+      <c r="ABM3" s="0"/>
+      <c r="ABN3" s="0"/>
+      <c r="ABO3" s="0"/>
+      <c r="ABP3" s="0"/>
+      <c r="ABQ3" s="0"/>
+      <c r="ABR3" s="0"/>
+      <c r="ABS3" s="0"/>
+      <c r="ABT3" s="0"/>
+      <c r="ABU3" s="0"/>
+      <c r="ABV3" s="0"/>
+      <c r="ABW3" s="0"/>
+      <c r="ABX3" s="0"/>
+      <c r="ABY3" s="0"/>
+      <c r="ABZ3" s="0"/>
+      <c r="ACA3" s="0"/>
+      <c r="ACB3" s="0"/>
+      <c r="ACC3" s="0"/>
+      <c r="ACD3" s="0"/>
+      <c r="ACE3" s="0"/>
+      <c r="ACF3" s="0"/>
+      <c r="ACG3" s="0"/>
+      <c r="ACH3" s="0"/>
+      <c r="ACI3" s="0"/>
+      <c r="ACJ3" s="0"/>
+      <c r="ACK3" s="0"/>
+      <c r="ACL3" s="0"/>
+      <c r="ACM3" s="0"/>
+      <c r="ACN3" s="0"/>
+      <c r="ACO3" s="0"/>
+      <c r="ACP3" s="0"/>
+      <c r="ACQ3" s="0"/>
+      <c r="ACR3" s="0"/>
+      <c r="ACS3" s="0"/>
+      <c r="ACT3" s="0"/>
+      <c r="ACU3" s="0"/>
+      <c r="ACV3" s="0"/>
+      <c r="ACW3" s="0"/>
+      <c r="ACX3" s="0"/>
+      <c r="ACY3" s="0"/>
+      <c r="ACZ3" s="0"/>
+      <c r="ADA3" s="0"/>
+      <c r="ADB3" s="0"/>
+      <c r="ADC3" s="0"/>
+      <c r="ADD3" s="0"/>
+      <c r="ADE3" s="0"/>
+      <c r="ADF3" s="0"/>
+      <c r="ADG3" s="0"/>
+      <c r="ADH3" s="0"/>
+      <c r="ADI3" s="0"/>
+      <c r="ADJ3" s="0"/>
+      <c r="ADK3" s="0"/>
+      <c r="ADL3" s="0"/>
+      <c r="ADM3" s="0"/>
+      <c r="ADN3" s="0"/>
+      <c r="ADO3" s="0"/>
+      <c r="ADP3" s="0"/>
+      <c r="ADQ3" s="0"/>
+      <c r="ADR3" s="0"/>
+      <c r="ADS3" s="0"/>
+      <c r="ADT3" s="0"/>
+      <c r="ADU3" s="0"/>
+      <c r="ADV3" s="0"/>
+      <c r="ADW3" s="0"/>
+      <c r="ADX3" s="0"/>
+      <c r="ADY3" s="0"/>
+      <c r="ADZ3" s="0"/>
+      <c r="AEA3" s="0"/>
+      <c r="AEB3" s="0"/>
+      <c r="AEC3" s="0"/>
+      <c r="AED3" s="0"/>
+      <c r="AEE3" s="0"/>
+      <c r="AEF3" s="0"/>
+      <c r="AEG3" s="0"/>
+      <c r="AEH3" s="0"/>
+      <c r="AEI3" s="0"/>
+      <c r="AEJ3" s="0"/>
+      <c r="AEK3" s="0"/>
+      <c r="AEL3" s="0"/>
+      <c r="AEM3" s="0"/>
+      <c r="AEN3" s="0"/>
+      <c r="AEO3" s="0"/>
+      <c r="AEP3" s="0"/>
+      <c r="AEQ3" s="0"/>
+      <c r="AER3" s="0"/>
+      <c r="AES3" s="0"/>
+      <c r="AET3" s="0"/>
+      <c r="AEU3" s="0"/>
+      <c r="AEV3" s="0"/>
+      <c r="AEW3" s="0"/>
+      <c r="AEX3" s="0"/>
+      <c r="AEY3" s="0"/>
+      <c r="AEZ3" s="0"/>
+      <c r="AFA3" s="0"/>
+      <c r="AFB3" s="0"/>
+      <c r="AFC3" s="0"/>
+      <c r="AFD3" s="0"/>
+      <c r="AFE3" s="0"/>
+      <c r="AFF3" s="0"/>
+      <c r="AFG3" s="0"/>
+      <c r="AFH3" s="0"/>
+      <c r="AFI3" s="0"/>
+      <c r="AFJ3" s="0"/>
+      <c r="AFK3" s="0"/>
+      <c r="AFL3" s="0"/>
+      <c r="AFM3" s="0"/>
+      <c r="AFN3" s="0"/>
+      <c r="AFO3" s="0"/>
+      <c r="AFP3" s="0"/>
+      <c r="AFQ3" s="0"/>
+      <c r="AFR3" s="0"/>
+      <c r="AFS3" s="0"/>
+      <c r="AFT3" s="0"/>
+      <c r="AFU3" s="0"/>
+      <c r="AFV3" s="0"/>
+      <c r="AFW3" s="0"/>
+      <c r="AFX3" s="0"/>
+      <c r="AFY3" s="0"/>
+      <c r="AFZ3" s="0"/>
+      <c r="AGA3" s="0"/>
+      <c r="AGB3" s="0"/>
+      <c r="AGC3" s="0"/>
+      <c r="AGD3" s="0"/>
+      <c r="AGE3" s="0"/>
+      <c r="AGF3" s="0"/>
+      <c r="AGG3" s="0"/>
+      <c r="AGH3" s="0"/>
+      <c r="AGI3" s="0"/>
+      <c r="AGJ3" s="0"/>
+      <c r="AGK3" s="0"/>
+      <c r="AGL3" s="0"/>
+      <c r="AGM3" s="0"/>
+      <c r="AGN3" s="0"/>
+      <c r="AGO3" s="0"/>
+      <c r="AGP3" s="0"/>
+      <c r="AGQ3" s="0"/>
+      <c r="AGR3" s="0"/>
+      <c r="AGS3" s="0"/>
+      <c r="AGT3" s="0"/>
+      <c r="AGU3" s="0"/>
+      <c r="AGV3" s="0"/>
+      <c r="AGW3" s="0"/>
+      <c r="AGX3" s="0"/>
+      <c r="AGY3" s="0"/>
+      <c r="AGZ3" s="0"/>
+      <c r="AHA3" s="0"/>
+      <c r="AHB3" s="0"/>
+      <c r="AHC3" s="0"/>
+      <c r="AHD3" s="0"/>
+      <c r="AHE3" s="0"/>
+      <c r="AHF3" s="0"/>
+      <c r="AHG3" s="0"/>
+      <c r="AHH3" s="0"/>
+      <c r="AHI3" s="0"/>
+      <c r="AHJ3" s="0"/>
+      <c r="AHK3" s="0"/>
+      <c r="AHL3" s="0"/>
+      <c r="AHM3" s="0"/>
+      <c r="AHN3" s="0"/>
+      <c r="AHO3" s="0"/>
+      <c r="AHP3" s="0"/>
+      <c r="AHQ3" s="0"/>
+      <c r="AHR3" s="0"/>
+      <c r="AHS3" s="0"/>
+      <c r="AHT3" s="0"/>
+      <c r="AHU3" s="0"/>
+      <c r="AHV3" s="0"/>
+      <c r="AHW3" s="0"/>
+      <c r="AHX3" s="0"/>
+      <c r="AHY3" s="0"/>
+      <c r="AHZ3" s="0"/>
+      <c r="AIA3" s="0"/>
+      <c r="AIB3" s="0"/>
+      <c r="AIC3" s="0"/>
+      <c r="AID3" s="0"/>
+      <c r="AIE3" s="0"/>
+      <c r="AIF3" s="0"/>
+      <c r="AIG3" s="0"/>
+      <c r="AIH3" s="0"/>
+      <c r="AII3" s="0"/>
+      <c r="AIJ3" s="0"/>
+      <c r="AIK3" s="0"/>
+      <c r="AIL3" s="0"/>
+      <c r="AIM3" s="0"/>
+      <c r="AIN3" s="0"/>
+      <c r="AIO3" s="0"/>
+      <c r="AIP3" s="0"/>
+      <c r="AIQ3" s="0"/>
+      <c r="AIR3" s="0"/>
+      <c r="AIS3" s="0"/>
+      <c r="AIT3" s="0"/>
+      <c r="AIU3" s="0"/>
+      <c r="AIV3" s="0"/>
+      <c r="AIW3" s="0"/>
+      <c r="AIX3" s="0"/>
+      <c r="AIY3" s="0"/>
+      <c r="AIZ3" s="0"/>
+      <c r="AJA3" s="0"/>
+      <c r="AJB3" s="0"/>
+      <c r="AJC3" s="0"/>
+      <c r="AJD3" s="0"/>
+      <c r="AJE3" s="0"/>
+      <c r="AJF3" s="0"/>
+      <c r="AJG3" s="0"/>
+      <c r="AJH3" s="0"/>
+      <c r="AJI3" s="0"/>
+      <c r="AJJ3" s="0"/>
+      <c r="AJK3" s="0"/>
+      <c r="AJL3" s="0"/>
+      <c r="AJM3" s="0"/>
+      <c r="AJN3" s="0"/>
+      <c r="AJO3" s="0"/>
+      <c r="AJP3" s="0"/>
+      <c r="AJQ3" s="0"/>
+      <c r="AJR3" s="0"/>
+      <c r="AJS3" s="0"/>
+      <c r="AJT3" s="0"/>
+      <c r="AJU3" s="0"/>
+      <c r="AJV3" s="0"/>
+      <c r="AJW3" s="0"/>
+      <c r="AJX3" s="0"/>
+      <c r="AJY3" s="0"/>
+      <c r="AJZ3" s="0"/>
+      <c r="AKA3" s="0"/>
+      <c r="AKB3" s="0"/>
+      <c r="AKC3" s="0"/>
+      <c r="AKD3" s="0"/>
+      <c r="AKE3" s="0"/>
+      <c r="AKF3" s="0"/>
+      <c r="AKG3" s="0"/>
+      <c r="AKH3" s="0"/>
+      <c r="AKI3" s="0"/>
+      <c r="AKJ3" s="0"/>
+      <c r="AKK3" s="0"/>
+      <c r="AKL3" s="0"/>
+      <c r="AKM3" s="0"/>
+      <c r="AKN3" s="0"/>
+      <c r="AKO3" s="0"/>
+      <c r="AKP3" s="0"/>
+      <c r="AKQ3" s="0"/>
+      <c r="AKR3" s="0"/>
+      <c r="AKS3" s="0"/>
+      <c r="AKT3" s="0"/>
+      <c r="AKU3" s="0"/>
+      <c r="AKV3" s="0"/>
+      <c r="AKW3" s="0"/>
+      <c r="AKX3" s="0"/>
+      <c r="AKY3" s="0"/>
+      <c r="AKZ3" s="0"/>
+      <c r="ALA3" s="0"/>
+      <c r="ALB3" s="0"/>
+      <c r="ALC3" s="0"/>
+      <c r="ALD3" s="0"/>
+      <c r="ALE3" s="0"/>
+      <c r="ALF3" s="0"/>
+      <c r="ALG3" s="0"/>
+      <c r="ALH3" s="0"/>
+      <c r="ALI3" s="0"/>
+      <c r="ALJ3" s="0"/>
+      <c r="ALK3" s="0"/>
+      <c r="ALL3" s="0"/>
+      <c r="ALM3" s="0"/>
+      <c r="ALN3" s="0"/>
+      <c r="ALO3" s="0"/>
+      <c r="ALP3" s="0"/>
+      <c r="ALQ3" s="0"/>
+      <c r="ALR3" s="0"/>
+      <c r="ALS3" s="0"/>
+      <c r="ALT3" s="0"/>
+      <c r="ALU3" s="0"/>
+      <c r="ALV3" s="0"/>
+      <c r="ALW3" s="0"/>
+      <c r="ALX3" s="0"/>
+      <c r="ALY3" s="0"/>
+      <c r="ALZ3" s="0"/>
+      <c r="AMA3" s="0"/>
+      <c r="AMB3" s="0"/>
+      <c r="AMC3" s="0"/>
+      <c r="AMD3" s="0"/>
+      <c r="AME3" s="0"/>
+      <c r="AMF3" s="0"/>
+      <c r="AMG3" s="0"/>
+      <c r="AMH3" s="0"/>
+      <c r="AMI3" s="0"/>
+      <c r="AMJ3" s="0"/>
     </row>
-    <row r="4" s="4" customFormat="true" ht="79.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="79.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4"/>
       <c r="B4" s="8" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="6"/>
+      <c r="E4" s="0"/>
+      <c r="F4" s="0"/>
+      <c r="G4" s="0"/>
+      <c r="H4" s="0"/>
+      <c r="I4" s="0"/>
+      <c r="J4" s="0"/>
+      <c r="K4" s="0"/>
+      <c r="L4" s="0"/>
+      <c r="M4" s="0"/>
+      <c r="N4" s="0"/>
+      <c r="O4" s="0"/>
+      <c r="P4" s="0"/>
+      <c r="Q4" s="0"/>
+      <c r="R4" s="0"/>
+      <c r="S4" s="0"/>
+      <c r="T4" s="0"/>
+      <c r="U4" s="0"/>
+      <c r="V4" s="0"/>
+      <c r="W4" s="0"/>
+      <c r="X4" s="0"/>
+      <c r="Y4" s="0"/>
+      <c r="Z4" s="0"/>
+      <c r="AA4" s="0"/>
+      <c r="AB4" s="0"/>
+      <c r="AC4" s="0"/>
+      <c r="AD4" s="0"/>
+      <c r="AE4" s="0"/>
+      <c r="AF4" s="0"/>
+      <c r="AG4" s="0"/>
+      <c r="AH4" s="0"/>
+      <c r="AI4" s="0"/>
+      <c r="AJ4" s="0"/>
+      <c r="AK4" s="0"/>
+      <c r="AL4" s="0"/>
+      <c r="AM4" s="0"/>
+      <c r="AN4" s="0"/>
+      <c r="AO4" s="0"/>
+      <c r="AP4" s="0"/>
+      <c r="AQ4" s="0"/>
+      <c r="AR4" s="0"/>
+      <c r="AS4" s="0"/>
+      <c r="AT4" s="0"/>
+      <c r="AU4" s="0"/>
+      <c r="AV4" s="0"/>
+      <c r="AW4" s="0"/>
+      <c r="AX4" s="0"/>
+      <c r="AY4" s="0"/>
+      <c r="AZ4" s="0"/>
+      <c r="BA4" s="0"/>
+      <c r="BB4" s="0"/>
+      <c r="BC4" s="0"/>
+      <c r="BD4" s="0"/>
+      <c r="BE4" s="0"/>
+      <c r="BF4" s="0"/>
+      <c r="BG4" s="0"/>
+      <c r="BH4" s="0"/>
+      <c r="BI4" s="0"/>
+      <c r="BJ4" s="0"/>
+      <c r="BK4" s="0"/>
+      <c r="BL4" s="0"/>
+      <c r="BM4" s="0"/>
+      <c r="BN4" s="0"/>
+      <c r="BO4" s="0"/>
+      <c r="BP4" s="0"/>
+      <c r="BQ4" s="0"/>
+      <c r="BR4" s="0"/>
+      <c r="BS4" s="0"/>
+      <c r="BT4" s="0"/>
+      <c r="BU4" s="0"/>
+      <c r="BV4" s="0"/>
+      <c r="BW4" s="0"/>
+      <c r="BX4" s="0"/>
+      <c r="BY4" s="0"/>
+      <c r="BZ4" s="0"/>
+      <c r="CA4" s="0"/>
+      <c r="CB4" s="0"/>
+      <c r="CC4" s="0"/>
+      <c r="CD4" s="0"/>
+      <c r="CE4" s="0"/>
+      <c r="CF4" s="0"/>
+      <c r="CG4" s="0"/>
+      <c r="CH4" s="0"/>
+      <c r="CI4" s="0"/>
+      <c r="CJ4" s="0"/>
+      <c r="CK4" s="0"/>
+      <c r="CL4" s="0"/>
+      <c r="CM4" s="0"/>
+      <c r="CN4" s="0"/>
+      <c r="CO4" s="0"/>
+      <c r="CP4" s="0"/>
+      <c r="CQ4" s="0"/>
+      <c r="CR4" s="0"/>
+      <c r="CS4" s="0"/>
+      <c r="CT4" s="0"/>
+      <c r="CU4" s="0"/>
+      <c r="CV4" s="0"/>
+      <c r="CW4" s="0"/>
+      <c r="CX4" s="0"/>
+      <c r="CY4" s="0"/>
+      <c r="CZ4" s="0"/>
+      <c r="DA4" s="0"/>
+      <c r="DB4" s="0"/>
+      <c r="DC4" s="0"/>
+      <c r="DD4" s="0"/>
+      <c r="DE4" s="0"/>
+      <c r="DF4" s="0"/>
+      <c r="DG4" s="0"/>
+      <c r="DH4" s="0"/>
+      <c r="DI4" s="0"/>
+      <c r="DJ4" s="0"/>
+      <c r="DK4" s="0"/>
+      <c r="DL4" s="0"/>
+      <c r="DM4" s="0"/>
+      <c r="DN4" s="0"/>
+      <c r="DO4" s="0"/>
+      <c r="DP4" s="0"/>
+      <c r="DQ4" s="0"/>
+      <c r="DR4" s="0"/>
+      <c r="DS4" s="0"/>
+      <c r="DT4" s="0"/>
+      <c r="DU4" s="0"/>
+      <c r="DV4" s="0"/>
+      <c r="DW4" s="0"/>
+      <c r="DX4" s="0"/>
+      <c r="DY4" s="0"/>
+      <c r="DZ4" s="0"/>
+      <c r="EA4" s="0"/>
+      <c r="EB4" s="0"/>
+      <c r="EC4" s="0"/>
+      <c r="ED4" s="0"/>
+      <c r="EE4" s="0"/>
+      <c r="EF4" s="0"/>
+      <c r="EG4" s="0"/>
+      <c r="EH4" s="0"/>
+      <c r="EI4" s="0"/>
+      <c r="EJ4" s="0"/>
+      <c r="EK4" s="0"/>
+      <c r="EL4" s="0"/>
+      <c r="EM4" s="0"/>
+      <c r="EN4" s="0"/>
+      <c r="EO4" s="0"/>
+      <c r="EP4" s="0"/>
+      <c r="EQ4" s="0"/>
+      <c r="ER4" s="0"/>
+      <c r="ES4" s="0"/>
+      <c r="ET4" s="0"/>
+      <c r="EU4" s="0"/>
+      <c r="EV4" s="0"/>
+      <c r="EW4" s="0"/>
+      <c r="EX4" s="0"/>
+      <c r="EY4" s="0"/>
+      <c r="EZ4" s="0"/>
+      <c r="FA4" s="0"/>
+      <c r="FB4" s="0"/>
+      <c r="FC4" s="0"/>
+      <c r="FD4" s="0"/>
+      <c r="FE4" s="0"/>
+      <c r="FF4" s="0"/>
+      <c r="FG4" s="0"/>
+      <c r="FH4" s="0"/>
+      <c r="FI4" s="0"/>
+      <c r="FJ4" s="0"/>
+      <c r="FK4" s="0"/>
+      <c r="FL4" s="0"/>
+      <c r="FM4" s="0"/>
+      <c r="FN4" s="0"/>
+      <c r="FO4" s="0"/>
+      <c r="FP4" s="0"/>
+      <c r="FQ4" s="0"/>
+      <c r="FR4" s="0"/>
+      <c r="FS4" s="0"/>
+      <c r="FT4" s="0"/>
+      <c r="FU4" s="0"/>
+      <c r="FV4" s="0"/>
+      <c r="FW4" s="0"/>
+      <c r="FX4" s="0"/>
+      <c r="FY4" s="0"/>
+      <c r="FZ4" s="0"/>
+      <c r="GA4" s="0"/>
+      <c r="GB4" s="0"/>
+      <c r="GC4" s="0"/>
+      <c r="GD4" s="0"/>
+      <c r="GE4" s="0"/>
+      <c r="GF4" s="0"/>
+      <c r="GG4" s="0"/>
+      <c r="GH4" s="0"/>
+      <c r="GI4" s="0"/>
+      <c r="GJ4" s="0"/>
+      <c r="GK4" s="0"/>
+      <c r="GL4" s="0"/>
+      <c r="GM4" s="0"/>
+      <c r="GN4" s="0"/>
+      <c r="GO4" s="0"/>
+      <c r="GP4" s="0"/>
+      <c r="GQ4" s="0"/>
+      <c r="GR4" s="0"/>
+      <c r="GS4" s="0"/>
+      <c r="GT4" s="0"/>
+      <c r="GU4" s="0"/>
+      <c r="GV4" s="0"/>
+      <c r="GW4" s="0"/>
+      <c r="GX4" s="0"/>
+      <c r="GY4" s="0"/>
+      <c r="GZ4" s="0"/>
+      <c r="HA4" s="0"/>
+      <c r="HB4" s="0"/>
+      <c r="HC4" s="0"/>
+      <c r="HD4" s="0"/>
+      <c r="HE4" s="0"/>
+      <c r="HF4" s="0"/>
+      <c r="HG4" s="0"/>
+      <c r="HH4" s="0"/>
+      <c r="HI4" s="0"/>
+      <c r="HJ4" s="0"/>
+      <c r="HK4" s="0"/>
+      <c r="HL4" s="0"/>
+      <c r="HM4" s="0"/>
+      <c r="HN4" s="0"/>
+      <c r="HO4" s="0"/>
+      <c r="HP4" s="0"/>
+      <c r="HQ4" s="0"/>
+      <c r="HR4" s="0"/>
+      <c r="HS4" s="0"/>
+      <c r="HT4" s="0"/>
+      <c r="HU4" s="0"/>
+      <c r="HV4" s="0"/>
+      <c r="HW4" s="0"/>
+      <c r="HX4" s="0"/>
+      <c r="HY4" s="0"/>
+      <c r="HZ4" s="0"/>
+      <c r="IA4" s="0"/>
+      <c r="IB4" s="0"/>
+      <c r="IC4" s="0"/>
+      <c r="ID4" s="0"/>
+      <c r="IE4" s="0"/>
+      <c r="IF4" s="0"/>
+      <c r="IG4" s="0"/>
+      <c r="IH4" s="0"/>
+      <c r="II4" s="0"/>
+      <c r="IJ4" s="0"/>
+      <c r="IK4" s="0"/>
+      <c r="IL4" s="0"/>
+      <c r="IM4" s="0"/>
+      <c r="IN4" s="0"/>
+      <c r="IO4" s="0"/>
+      <c r="IP4" s="0"/>
+      <c r="IQ4" s="0"/>
+      <c r="IR4" s="0"/>
+      <c r="IS4" s="0"/>
+      <c r="IT4" s="0"/>
+      <c r="IU4" s="0"/>
+      <c r="IV4" s="0"/>
+      <c r="IW4" s="0"/>
+      <c r="IX4" s="0"/>
+      <c r="IY4" s="0"/>
+      <c r="IZ4" s="0"/>
+      <c r="JA4" s="0"/>
+      <c r="JB4" s="0"/>
+      <c r="JC4" s="0"/>
+      <c r="JD4" s="0"/>
+      <c r="JE4" s="0"/>
+      <c r="JF4" s="0"/>
+      <c r="JG4" s="0"/>
+      <c r="JH4" s="0"/>
+      <c r="JI4" s="0"/>
+      <c r="JJ4" s="0"/>
+      <c r="JK4" s="0"/>
+      <c r="JL4" s="0"/>
+      <c r="JM4" s="0"/>
+      <c r="JN4" s="0"/>
+      <c r="JO4" s="0"/>
+      <c r="JP4" s="0"/>
+      <c r="JQ4" s="0"/>
+      <c r="JR4" s="0"/>
+      <c r="JS4" s="0"/>
+      <c r="JT4" s="0"/>
+      <c r="JU4" s="0"/>
+      <c r="JV4" s="0"/>
+      <c r="JW4" s="0"/>
+      <c r="JX4" s="0"/>
+      <c r="JY4" s="0"/>
+      <c r="JZ4" s="0"/>
+      <c r="KA4" s="0"/>
+      <c r="KB4" s="0"/>
+      <c r="KC4" s="0"/>
+      <c r="KD4" s="0"/>
+      <c r="KE4" s="0"/>
+      <c r="KF4" s="0"/>
+      <c r="KG4" s="0"/>
+      <c r="KH4" s="0"/>
+      <c r="KI4" s="0"/>
+      <c r="KJ4" s="0"/>
+      <c r="KK4" s="0"/>
+      <c r="KL4" s="0"/>
+      <c r="KM4" s="0"/>
+      <c r="KN4" s="0"/>
+      <c r="KO4" s="0"/>
+      <c r="KP4" s="0"/>
+      <c r="KQ4" s="0"/>
+      <c r="KR4" s="0"/>
+      <c r="KS4" s="0"/>
+      <c r="KT4" s="0"/>
+      <c r="KU4" s="0"/>
+      <c r="KV4" s="0"/>
+      <c r="KW4" s="0"/>
+      <c r="KX4" s="0"/>
+      <c r="KY4" s="0"/>
+      <c r="KZ4" s="0"/>
+      <c r="LA4" s="0"/>
+      <c r="LB4" s="0"/>
+      <c r="LC4" s="0"/>
+      <c r="LD4" s="0"/>
+      <c r="LE4" s="0"/>
+      <c r="LF4" s="0"/>
+      <c r="LG4" s="0"/>
+      <c r="LH4" s="0"/>
+      <c r="LI4" s="0"/>
+      <c r="LJ4" s="0"/>
+      <c r="LK4" s="0"/>
+      <c r="LL4" s="0"/>
+      <c r="LM4" s="0"/>
+      <c r="LN4" s="0"/>
+      <c r="LO4" s="0"/>
+      <c r="LP4" s="0"/>
+      <c r="LQ4" s="0"/>
+      <c r="LR4" s="0"/>
+      <c r="LS4" s="0"/>
+      <c r="LT4" s="0"/>
+      <c r="LU4" s="0"/>
+      <c r="LV4" s="0"/>
+      <c r="LW4" s="0"/>
+      <c r="LX4" s="0"/>
+      <c r="LY4" s="0"/>
+      <c r="LZ4" s="0"/>
+      <c r="MA4" s="0"/>
+      <c r="MB4" s="0"/>
+      <c r="MC4" s="0"/>
+      <c r="MD4" s="0"/>
+      <c r="ME4" s="0"/>
+      <c r="MF4" s="0"/>
+      <c r="MG4" s="0"/>
+      <c r="MH4" s="0"/>
+      <c r="MI4" s="0"/>
+      <c r="MJ4" s="0"/>
+      <c r="MK4" s="0"/>
+      <c r="ML4" s="0"/>
+      <c r="MM4" s="0"/>
+      <c r="MN4" s="0"/>
+      <c r="MO4" s="0"/>
+      <c r="MP4" s="0"/>
+      <c r="MQ4" s="0"/>
+      <c r="MR4" s="0"/>
+      <c r="MS4" s="0"/>
+      <c r="MT4" s="0"/>
+      <c r="MU4" s="0"/>
+      <c r="MV4" s="0"/>
+      <c r="MW4" s="0"/>
+      <c r="MX4" s="0"/>
+      <c r="MY4" s="0"/>
+      <c r="MZ4" s="0"/>
+      <c r="NA4" s="0"/>
+      <c r="NB4" s="0"/>
+      <c r="NC4" s="0"/>
+      <c r="ND4" s="0"/>
+      <c r="NE4" s="0"/>
+      <c r="NF4" s="0"/>
+      <c r="NG4" s="0"/>
+      <c r="NH4" s="0"/>
+      <c r="NI4" s="0"/>
+      <c r="NJ4" s="0"/>
+      <c r="NK4" s="0"/>
+      <c r="NL4" s="0"/>
+      <c r="NM4" s="0"/>
+      <c r="NN4" s="0"/>
+      <c r="NO4" s="0"/>
+      <c r="NP4" s="0"/>
+      <c r="NQ4" s="0"/>
+      <c r="NR4" s="0"/>
+      <c r="NS4" s="0"/>
+      <c r="NT4" s="0"/>
+      <c r="NU4" s="0"/>
+      <c r="NV4" s="0"/>
+      <c r="NW4" s="0"/>
+      <c r="NX4" s="0"/>
+      <c r="NY4" s="0"/>
+      <c r="NZ4" s="0"/>
+      <c r="OA4" s="0"/>
+      <c r="OB4" s="0"/>
+      <c r="OC4" s="0"/>
+      <c r="OD4" s="0"/>
+      <c r="OE4" s="0"/>
+      <c r="OF4" s="0"/>
+      <c r="OG4" s="0"/>
+      <c r="OH4" s="0"/>
+      <c r="OI4" s="0"/>
+      <c r="OJ4" s="0"/>
+      <c r="OK4" s="0"/>
+      <c r="OL4" s="0"/>
+      <c r="OM4" s="0"/>
+      <c r="ON4" s="0"/>
+      <c r="OO4" s="0"/>
+      <c r="OP4" s="0"/>
+      <c r="OQ4" s="0"/>
+      <c r="OR4" s="0"/>
+      <c r="OS4" s="0"/>
+      <c r="OT4" s="0"/>
+      <c r="OU4" s="0"/>
+      <c r="OV4" s="0"/>
+      <c r="OW4" s="0"/>
+      <c r="OX4" s="0"/>
+      <c r="OY4" s="0"/>
+      <c r="OZ4" s="0"/>
+      <c r="PA4" s="0"/>
+      <c r="PB4" s="0"/>
+      <c r="PC4" s="0"/>
+      <c r="PD4" s="0"/>
+      <c r="PE4" s="0"/>
+      <c r="PF4" s="0"/>
+      <c r="PG4" s="0"/>
+      <c r="PH4" s="0"/>
+      <c r="PI4" s="0"/>
+      <c r="PJ4" s="0"/>
+      <c r="PK4" s="0"/>
+      <c r="PL4" s="0"/>
+      <c r="PM4" s="0"/>
+      <c r="PN4" s="0"/>
+      <c r="PO4" s="0"/>
+      <c r="PP4" s="0"/>
+      <c r="PQ4" s="0"/>
+      <c r="PR4" s="0"/>
+      <c r="PS4" s="0"/>
+      <c r="PT4" s="0"/>
+      <c r="PU4" s="0"/>
+      <c r="PV4" s="0"/>
+      <c r="PW4" s="0"/>
+      <c r="PX4" s="0"/>
+      <c r="PY4" s="0"/>
+      <c r="PZ4" s="0"/>
+      <c r="QA4" s="0"/>
+      <c r="QB4" s="0"/>
+      <c r="QC4" s="0"/>
+      <c r="QD4" s="0"/>
+      <c r="QE4" s="0"/>
+      <c r="QF4" s="0"/>
+      <c r="QG4" s="0"/>
+      <c r="QH4" s="0"/>
+      <c r="QI4" s="0"/>
+      <c r="QJ4" s="0"/>
+      <c r="QK4" s="0"/>
+      <c r="QL4" s="0"/>
+      <c r="QM4" s="0"/>
+      <c r="QN4" s="0"/>
+      <c r="QO4" s="0"/>
+      <c r="QP4" s="0"/>
+      <c r="QQ4" s="0"/>
+      <c r="QR4" s="0"/>
+      <c r="QS4" s="0"/>
+      <c r="QT4" s="0"/>
+      <c r="QU4" s="0"/>
+      <c r="QV4" s="0"/>
+      <c r="QW4" s="0"/>
+      <c r="QX4" s="0"/>
+      <c r="QY4" s="0"/>
+      <c r="QZ4" s="0"/>
+      <c r="RA4" s="0"/>
+      <c r="RB4" s="0"/>
+      <c r="RC4" s="0"/>
+      <c r="RD4" s="0"/>
+      <c r="RE4" s="0"/>
+      <c r="RF4" s="0"/>
+      <c r="RG4" s="0"/>
+      <c r="RH4" s="0"/>
+      <c r="RI4" s="0"/>
+      <c r="RJ4" s="0"/>
+      <c r="RK4" s="0"/>
+      <c r="RL4" s="0"/>
+      <c r="RM4" s="0"/>
+      <c r="RN4" s="0"/>
+      <c r="RO4" s="0"/>
+      <c r="RP4" s="0"/>
+      <c r="RQ4" s="0"/>
+      <c r="RR4" s="0"/>
+      <c r="RS4" s="0"/>
+      <c r="RT4" s="0"/>
+      <c r="RU4" s="0"/>
+      <c r="RV4" s="0"/>
+      <c r="RW4" s="0"/>
+      <c r="RX4" s="0"/>
+      <c r="RY4" s="0"/>
+      <c r="RZ4" s="0"/>
+      <c r="SA4" s="0"/>
+      <c r="SB4" s="0"/>
+      <c r="SC4" s="0"/>
+      <c r="SD4" s="0"/>
+      <c r="SE4" s="0"/>
+      <c r="SF4" s="0"/>
+      <c r="SG4" s="0"/>
+      <c r="SH4" s="0"/>
+      <c r="SI4" s="0"/>
+      <c r="SJ4" s="0"/>
+      <c r="SK4" s="0"/>
+      <c r="SL4" s="0"/>
+      <c r="SM4" s="0"/>
+      <c r="SN4" s="0"/>
+      <c r="SO4" s="0"/>
+      <c r="SP4" s="0"/>
+      <c r="SQ4" s="0"/>
+      <c r="SR4" s="0"/>
+      <c r="SS4" s="0"/>
+      <c r="ST4" s="0"/>
+      <c r="SU4" s="0"/>
+      <c r="SV4" s="0"/>
+      <c r="SW4" s="0"/>
+      <c r="SX4" s="0"/>
+      <c r="SY4" s="0"/>
+      <c r="SZ4" s="0"/>
+      <c r="TA4" s="0"/>
+      <c r="TB4" s="0"/>
+      <c r="TC4" s="0"/>
+      <c r="TD4" s="0"/>
+      <c r="TE4" s="0"/>
+      <c r="TF4" s="0"/>
+      <c r="TG4" s="0"/>
+      <c r="TH4" s="0"/>
+      <c r="TI4" s="0"/>
+      <c r="TJ4" s="0"/>
+      <c r="TK4" s="0"/>
+      <c r="TL4" s="0"/>
+      <c r="TM4" s="0"/>
+      <c r="TN4" s="0"/>
+      <c r="TO4" s="0"/>
+      <c r="TP4" s="0"/>
+      <c r="TQ4" s="0"/>
+      <c r="TR4" s="0"/>
+      <c r="TS4" s="0"/>
+      <c r="TT4" s="0"/>
+      <c r="TU4" s="0"/>
+      <c r="TV4" s="0"/>
+      <c r="TW4" s="0"/>
+      <c r="TX4" s="0"/>
+      <c r="TY4" s="0"/>
+      <c r="TZ4" s="0"/>
+      <c r="UA4" s="0"/>
+      <c r="UB4" s="0"/>
+      <c r="UC4" s="0"/>
+      <c r="UD4" s="0"/>
+      <c r="UE4" s="0"/>
+      <c r="UF4" s="0"/>
+      <c r="UG4" s="0"/>
+      <c r="UH4" s="0"/>
+      <c r="UI4" s="0"/>
+      <c r="UJ4" s="0"/>
+      <c r="UK4" s="0"/>
+      <c r="UL4" s="0"/>
+      <c r="UM4" s="0"/>
+      <c r="UN4" s="0"/>
+      <c r="UO4" s="0"/>
+      <c r="UP4" s="0"/>
+      <c r="UQ4" s="0"/>
+      <c r="UR4" s="0"/>
+      <c r="US4" s="0"/>
+      <c r="UT4" s="0"/>
+      <c r="UU4" s="0"/>
+      <c r="UV4" s="0"/>
+      <c r="UW4" s="0"/>
+      <c r="UX4" s="0"/>
+      <c r="UY4" s="0"/>
+      <c r="UZ4" s="0"/>
+      <c r="VA4" s="0"/>
+      <c r="VB4" s="0"/>
+      <c r="VC4" s="0"/>
+      <c r="VD4" s="0"/>
+      <c r="VE4" s="0"/>
+      <c r="VF4" s="0"/>
+      <c r="VG4" s="0"/>
+      <c r="VH4" s="0"/>
+      <c r="VI4" s="0"/>
+      <c r="VJ4" s="0"/>
+      <c r="VK4" s="0"/>
+      <c r="VL4" s="0"/>
+      <c r="VM4" s="0"/>
+      <c r="VN4" s="0"/>
+      <c r="VO4" s="0"/>
+      <c r="VP4" s="0"/>
+      <c r="VQ4" s="0"/>
+      <c r="VR4" s="0"/>
+      <c r="VS4" s="0"/>
+      <c r="VT4" s="0"/>
+      <c r="VU4" s="0"/>
+      <c r="VV4" s="0"/>
+      <c r="VW4" s="0"/>
+      <c r="VX4" s="0"/>
+      <c r="VY4" s="0"/>
+      <c r="VZ4" s="0"/>
+      <c r="WA4" s="0"/>
+      <c r="WB4" s="0"/>
+      <c r="WC4" s="0"/>
+      <c r="WD4" s="0"/>
+      <c r="WE4" s="0"/>
+      <c r="WF4" s="0"/>
+      <c r="WG4" s="0"/>
+      <c r="WH4" s="0"/>
+      <c r="WI4" s="0"/>
+      <c r="WJ4" s="0"/>
+      <c r="WK4" s="0"/>
+      <c r="WL4" s="0"/>
+      <c r="WM4" s="0"/>
+      <c r="WN4" s="0"/>
+      <c r="WO4" s="0"/>
+      <c r="WP4" s="0"/>
+      <c r="WQ4" s="0"/>
+      <c r="WR4" s="0"/>
+      <c r="WS4" s="0"/>
+      <c r="WT4" s="0"/>
+      <c r="WU4" s="0"/>
+      <c r="WV4" s="0"/>
+      <c r="WW4" s="0"/>
+      <c r="WX4" s="0"/>
+      <c r="WY4" s="0"/>
+      <c r="WZ4" s="0"/>
+      <c r="XA4" s="0"/>
+      <c r="XB4" s="0"/>
+      <c r="XC4" s="0"/>
+      <c r="XD4" s="0"/>
+      <c r="XE4" s="0"/>
+      <c r="XF4" s="0"/>
+      <c r="XG4" s="0"/>
+      <c r="XH4" s="0"/>
+      <c r="XI4" s="0"/>
+      <c r="XJ4" s="0"/>
+      <c r="XK4" s="0"/>
+      <c r="XL4" s="0"/>
+      <c r="XM4" s="0"/>
+      <c r="XN4" s="0"/>
+      <c r="XO4" s="0"/>
+      <c r="XP4" s="0"/>
+      <c r="XQ4" s="0"/>
+      <c r="XR4" s="0"/>
+      <c r="XS4" s="0"/>
+      <c r="XT4" s="0"/>
+      <c r="XU4" s="0"/>
+      <c r="XV4" s="0"/>
+      <c r="XW4" s="0"/>
+      <c r="XX4" s="0"/>
+      <c r="XY4" s="0"/>
+      <c r="XZ4" s="0"/>
+      <c r="YA4" s="0"/>
+      <c r="YB4" s="0"/>
+      <c r="YC4" s="0"/>
+      <c r="YD4" s="0"/>
+      <c r="YE4" s="0"/>
+      <c r="YF4" s="0"/>
+      <c r="YG4" s="0"/>
+      <c r="YH4" s="0"/>
+      <c r="YI4" s="0"/>
+      <c r="YJ4" s="0"/>
+      <c r="YK4" s="0"/>
+      <c r="YL4" s="0"/>
+      <c r="YM4" s="0"/>
+      <c r="YN4" s="0"/>
+      <c r="YO4" s="0"/>
+      <c r="YP4" s="0"/>
+      <c r="YQ4" s="0"/>
+      <c r="YR4" s="0"/>
+      <c r="YS4" s="0"/>
+      <c r="YT4" s="0"/>
+      <c r="YU4" s="0"/>
+      <c r="YV4" s="0"/>
+      <c r="YW4" s="0"/>
+      <c r="YX4" s="0"/>
+      <c r="YY4" s="0"/>
+      <c r="YZ4" s="0"/>
+      <c r="ZA4" s="0"/>
+      <c r="ZB4" s="0"/>
+      <c r="ZC4" s="0"/>
+      <c r="ZD4" s="0"/>
+      <c r="ZE4" s="0"/>
+      <c r="ZF4" s="0"/>
+      <c r="ZG4" s="0"/>
+      <c r="ZH4" s="0"/>
+      <c r="ZI4" s="0"/>
+      <c r="ZJ4" s="0"/>
+      <c r="ZK4" s="0"/>
+      <c r="ZL4" s="0"/>
+      <c r="ZM4" s="0"/>
+      <c r="ZN4" s="0"/>
+      <c r="ZO4" s="0"/>
+      <c r="ZP4" s="0"/>
+      <c r="ZQ4" s="0"/>
+      <c r="ZR4" s="0"/>
+      <c r="ZS4" s="0"/>
+      <c r="ZT4" s="0"/>
+      <c r="ZU4" s="0"/>
+      <c r="ZV4" s="0"/>
+      <c r="ZW4" s="0"/>
+      <c r="ZX4" s="0"/>
+      <c r="ZY4" s="0"/>
+      <c r="ZZ4" s="0"/>
+      <c r="AAA4" s="0"/>
+      <c r="AAB4" s="0"/>
+      <c r="AAC4" s="0"/>
+      <c r="AAD4" s="0"/>
+      <c r="AAE4" s="0"/>
+      <c r="AAF4" s="0"/>
+      <c r="AAG4" s="0"/>
+      <c r="AAH4" s="0"/>
+      <c r="AAI4" s="0"/>
+      <c r="AAJ4" s="0"/>
+      <c r="AAK4" s="0"/>
+      <c r="AAL4" s="0"/>
+      <c r="AAM4" s="0"/>
+      <c r="AAN4" s="0"/>
+      <c r="AAO4" s="0"/>
+      <c r="AAP4" s="0"/>
+      <c r="AAQ4" s="0"/>
+      <c r="AAR4" s="0"/>
+      <c r="AAS4" s="0"/>
+      <c r="AAT4" s="0"/>
+      <c r="AAU4" s="0"/>
+      <c r="AAV4" s="0"/>
+      <c r="AAW4" s="0"/>
+      <c r="AAX4" s="0"/>
+      <c r="AAY4" s="0"/>
+      <c r="AAZ4" s="0"/>
+      <c r="ABA4" s="0"/>
+      <c r="ABB4" s="0"/>
+      <c r="ABC4" s="0"/>
+      <c r="ABD4" s="0"/>
+      <c r="ABE4" s="0"/>
+      <c r="ABF4" s="0"/>
+      <c r="ABG4" s="0"/>
+      <c r="ABH4" s="0"/>
+      <c r="ABI4" s="0"/>
+      <c r="ABJ4" s="0"/>
+      <c r="ABK4" s="0"/>
+      <c r="ABL4" s="0"/>
+      <c r="ABM4" s="0"/>
+      <c r="ABN4" s="0"/>
+      <c r="ABO4" s="0"/>
+      <c r="ABP4" s="0"/>
+      <c r="ABQ4" s="0"/>
+      <c r="ABR4" s="0"/>
+      <c r="ABS4" s="0"/>
+      <c r="ABT4" s="0"/>
+      <c r="ABU4" s="0"/>
+      <c r="ABV4" s="0"/>
+      <c r="ABW4" s="0"/>
+      <c r="ABX4" s="0"/>
+      <c r="ABY4" s="0"/>
+      <c r="ABZ4" s="0"/>
+      <c r="ACA4" s="0"/>
+      <c r="ACB4" s="0"/>
+      <c r="ACC4" s="0"/>
+      <c r="ACD4" s="0"/>
+      <c r="ACE4" s="0"/>
+      <c r="ACF4" s="0"/>
+      <c r="ACG4" s="0"/>
+      <c r="ACH4" s="0"/>
+      <c r="ACI4" s="0"/>
+      <c r="ACJ4" s="0"/>
+      <c r="ACK4" s="0"/>
+      <c r="ACL4" s="0"/>
+      <c r="ACM4" s="0"/>
+      <c r="ACN4" s="0"/>
+      <c r="ACO4" s="0"/>
+      <c r="ACP4" s="0"/>
+      <c r="ACQ4" s="0"/>
+      <c r="ACR4" s="0"/>
+      <c r="ACS4" s="0"/>
+      <c r="ACT4" s="0"/>
+      <c r="ACU4" s="0"/>
+      <c r="ACV4" s="0"/>
+      <c r="ACW4" s="0"/>
+      <c r="ACX4" s="0"/>
+      <c r="ACY4" s="0"/>
+      <c r="ACZ4" s="0"/>
+      <c r="ADA4" s="0"/>
+      <c r="ADB4" s="0"/>
+      <c r="ADC4" s="0"/>
+      <c r="ADD4" s="0"/>
+      <c r="ADE4" s="0"/>
+      <c r="ADF4" s="0"/>
+      <c r="ADG4" s="0"/>
+      <c r="ADH4" s="0"/>
+      <c r="ADI4" s="0"/>
+      <c r="ADJ4" s="0"/>
+      <c r="ADK4" s="0"/>
+      <c r="ADL4" s="0"/>
+      <c r="ADM4" s="0"/>
+      <c r="ADN4" s="0"/>
+      <c r="ADO4" s="0"/>
+      <c r="ADP4" s="0"/>
+      <c r="ADQ4" s="0"/>
+      <c r="ADR4" s="0"/>
+      <c r="ADS4" s="0"/>
+      <c r="ADT4" s="0"/>
+      <c r="ADU4" s="0"/>
+      <c r="ADV4" s="0"/>
+      <c r="ADW4" s="0"/>
+      <c r="ADX4" s="0"/>
+      <c r="ADY4" s="0"/>
+      <c r="ADZ4" s="0"/>
+      <c r="AEA4" s="0"/>
+      <c r="AEB4" s="0"/>
+      <c r="AEC4" s="0"/>
+      <c r="AED4" s="0"/>
+      <c r="AEE4" s="0"/>
+      <c r="AEF4" s="0"/>
+      <c r="AEG4" s="0"/>
+      <c r="AEH4" s="0"/>
+      <c r="AEI4" s="0"/>
+      <c r="AEJ4" s="0"/>
+      <c r="AEK4" s="0"/>
+      <c r="AEL4" s="0"/>
+      <c r="AEM4" s="0"/>
+      <c r="AEN4" s="0"/>
+      <c r="AEO4" s="0"/>
+      <c r="AEP4" s="0"/>
+      <c r="AEQ4" s="0"/>
+      <c r="AER4" s="0"/>
+      <c r="AES4" s="0"/>
+      <c r="AET4" s="0"/>
+      <c r="AEU4" s="0"/>
+      <c r="AEV4" s="0"/>
+      <c r="AEW4" s="0"/>
+      <c r="AEX4" s="0"/>
+      <c r="AEY4" s="0"/>
+      <c r="AEZ4" s="0"/>
+      <c r="AFA4" s="0"/>
+      <c r="AFB4" s="0"/>
+      <c r="AFC4" s="0"/>
+      <c r="AFD4" s="0"/>
+      <c r="AFE4" s="0"/>
+      <c r="AFF4" s="0"/>
+      <c r="AFG4" s="0"/>
+      <c r="AFH4" s="0"/>
+      <c r="AFI4" s="0"/>
+      <c r="AFJ4" s="0"/>
+      <c r="AFK4" s="0"/>
+      <c r="AFL4" s="0"/>
+      <c r="AFM4" s="0"/>
+      <c r="AFN4" s="0"/>
+      <c r="AFO4" s="0"/>
+      <c r="AFP4" s="0"/>
+      <c r="AFQ4" s="0"/>
+      <c r="AFR4" s="0"/>
+      <c r="AFS4" s="0"/>
+      <c r="AFT4" s="0"/>
+      <c r="AFU4" s="0"/>
+      <c r="AFV4" s="0"/>
+      <c r="AFW4" s="0"/>
+      <c r="AFX4" s="0"/>
+      <c r="AFY4" s="0"/>
+      <c r="AFZ4" s="0"/>
+      <c r="AGA4" s="0"/>
+      <c r="AGB4" s="0"/>
+      <c r="AGC4" s="0"/>
+      <c r="AGD4" s="0"/>
+      <c r="AGE4" s="0"/>
+      <c r="AGF4" s="0"/>
+      <c r="AGG4" s="0"/>
+      <c r="AGH4" s="0"/>
+      <c r="AGI4" s="0"/>
+      <c r="AGJ4" s="0"/>
+      <c r="AGK4" s="0"/>
+      <c r="AGL4" s="0"/>
+      <c r="AGM4" s="0"/>
+      <c r="AGN4" s="0"/>
+      <c r="AGO4" s="0"/>
+      <c r="AGP4" s="0"/>
+      <c r="AGQ4" s="0"/>
+      <c r="AGR4" s="0"/>
+      <c r="AGS4" s="0"/>
+      <c r="AGT4" s="0"/>
+      <c r="AGU4" s="0"/>
+      <c r="AGV4" s="0"/>
+      <c r="AGW4" s="0"/>
+      <c r="AGX4" s="0"/>
+      <c r="AGY4" s="0"/>
+      <c r="AGZ4" s="0"/>
+      <c r="AHA4" s="0"/>
+      <c r="AHB4" s="0"/>
+      <c r="AHC4" s="0"/>
+      <c r="AHD4" s="0"/>
+      <c r="AHE4" s="0"/>
+      <c r="AHF4" s="0"/>
+      <c r="AHG4" s="0"/>
+      <c r="AHH4" s="0"/>
+      <c r="AHI4" s="0"/>
+      <c r="AHJ4" s="0"/>
+      <c r="AHK4" s="0"/>
+      <c r="AHL4" s="0"/>
+      <c r="AHM4" s="0"/>
+      <c r="AHN4" s="0"/>
+      <c r="AHO4" s="0"/>
+      <c r="AHP4" s="0"/>
+      <c r="AHQ4" s="0"/>
+      <c r="AHR4" s="0"/>
+      <c r="AHS4" s="0"/>
+      <c r="AHT4" s="0"/>
+      <c r="AHU4" s="0"/>
+      <c r="AHV4" s="0"/>
+      <c r="AHW4" s="0"/>
+      <c r="AHX4" s="0"/>
+      <c r="AHY4" s="0"/>
+      <c r="AHZ4" s="0"/>
+      <c r="AIA4" s="0"/>
+      <c r="AIB4" s="0"/>
+      <c r="AIC4" s="0"/>
+      <c r="AID4" s="0"/>
+      <c r="AIE4" s="0"/>
+      <c r="AIF4" s="0"/>
+      <c r="AIG4" s="0"/>
+      <c r="AIH4" s="0"/>
+      <c r="AII4" s="0"/>
+      <c r="AIJ4" s="0"/>
+      <c r="AIK4" s="0"/>
+      <c r="AIL4" s="0"/>
+      <c r="AIM4" s="0"/>
+      <c r="AIN4" s="0"/>
+      <c r="AIO4" s="0"/>
+      <c r="AIP4" s="0"/>
+      <c r="AIQ4" s="0"/>
+      <c r="AIR4" s="0"/>
+      <c r="AIS4" s="0"/>
+      <c r="AIT4" s="0"/>
+      <c r="AIU4" s="0"/>
+      <c r="AIV4" s="0"/>
+      <c r="AIW4" s="0"/>
+      <c r="AIX4" s="0"/>
+      <c r="AIY4" s="0"/>
+      <c r="AIZ4" s="0"/>
+      <c r="AJA4" s="0"/>
+      <c r="AJB4" s="0"/>
+      <c r="AJC4" s="0"/>
+      <c r="AJD4" s="0"/>
+      <c r="AJE4" s="0"/>
+      <c r="AJF4" s="0"/>
+      <c r="AJG4" s="0"/>
+      <c r="AJH4" s="0"/>
+      <c r="AJI4" s="0"/>
+      <c r="AJJ4" s="0"/>
+      <c r="AJK4" s="0"/>
+      <c r="AJL4" s="0"/>
+      <c r="AJM4" s="0"/>
+      <c r="AJN4" s="0"/>
+      <c r="AJO4" s="0"/>
+      <c r="AJP4" s="0"/>
+      <c r="AJQ4" s="0"/>
+      <c r="AJR4" s="0"/>
+      <c r="AJS4" s="0"/>
+      <c r="AJT4" s="0"/>
+      <c r="AJU4" s="0"/>
+      <c r="AJV4" s="0"/>
+      <c r="AJW4" s="0"/>
+      <c r="AJX4" s="0"/>
+      <c r="AJY4" s="0"/>
+      <c r="AJZ4" s="0"/>
+      <c r="AKA4" s="0"/>
+      <c r="AKB4" s="0"/>
+      <c r="AKC4" s="0"/>
+      <c r="AKD4" s="0"/>
+      <c r="AKE4" s="0"/>
+      <c r="AKF4" s="0"/>
+      <c r="AKG4" s="0"/>
+      <c r="AKH4" s="0"/>
+      <c r="AKI4" s="0"/>
+      <c r="AKJ4" s="0"/>
+      <c r="AKK4" s="0"/>
+      <c r="AKL4" s="0"/>
+      <c r="AKM4" s="0"/>
+      <c r="AKN4" s="0"/>
+      <c r="AKO4" s="0"/>
+      <c r="AKP4" s="0"/>
+      <c r="AKQ4" s="0"/>
+      <c r="AKR4" s="0"/>
+      <c r="AKS4" s="0"/>
+      <c r="AKT4" s="0"/>
+      <c r="AKU4" s="0"/>
+      <c r="AKV4" s="0"/>
+      <c r="AKW4" s="0"/>
+      <c r="AKX4" s="0"/>
+      <c r="AKY4" s="0"/>
+      <c r="AKZ4" s="0"/>
+      <c r="ALA4" s="0"/>
+      <c r="ALB4" s="0"/>
+      <c r="ALC4" s="0"/>
+      <c r="ALD4" s="0"/>
+      <c r="ALE4" s="0"/>
+      <c r="ALF4" s="0"/>
+      <c r="ALG4" s="0"/>
+      <c r="ALH4" s="0"/>
+      <c r="ALI4" s="0"/>
+      <c r="ALJ4" s="0"/>
+      <c r="ALK4" s="0"/>
+      <c r="ALL4" s="0"/>
+      <c r="ALM4" s="0"/>
+      <c r="ALN4" s="0"/>
+      <c r="ALO4" s="0"/>
+      <c r="ALP4" s="0"/>
+      <c r="ALQ4" s="0"/>
+      <c r="ALR4" s="0"/>
+      <c r="ALS4" s="0"/>
+      <c r="ALT4" s="0"/>
+      <c r="ALU4" s="0"/>
+      <c r="ALV4" s="0"/>
+      <c r="ALW4" s="0"/>
+      <c r="ALX4" s="0"/>
+      <c r="ALY4" s="0"/>
+      <c r="ALZ4" s="0"/>
+      <c r="AMA4" s="0"/>
+      <c r="AMB4" s="0"/>
+      <c r="AMC4" s="0"/>
+      <c r="AMD4" s="0"/>
+      <c r="AME4" s="0"/>
+      <c r="AMF4" s="0"/>
+      <c r="AMG4" s="0"/>
+      <c r="AMH4" s="0"/>
+      <c r="AMI4" s="0"/>
+      <c r="AMJ4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="4"/>

</xml_diff>